<commit_message>
Rework the bear event to include other animals aswell
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erki\Documents\GitHub\Skull132\Aurora.3\tools\Event Probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekte\SS13\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -189,9 +189,6 @@
     <t>Space Vines</t>
   </si>
   <si>
-    <t>Bear Attack</t>
-  </si>
-  <si>
     <t>Wallrot</t>
   </si>
   <si>
@@ -200,12 +197,15 @@
   <si>
     <t>CCIAA General Notice</t>
   </si>
+  <si>
+    <t>Hostile Animals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,6 +213,11 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -259,18 +264,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -286,7 +292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -584,25 +590,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="13" width="7" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="26" width="7" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" customWidth="1"/>
+    <col min="9" max="13" width="7" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" style="3" customWidth="1"/>
+    <col min="17" max="26" width="7" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="15.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -621,31 +628,31 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="2"/>
@@ -653,32 +660,32 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <f>SUM(B3:I3)*1.5</f>
         <v>34.5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>4</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <v>4</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
@@ -723,747 +730,747 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>120</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="6">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="7">
         <f t="shared" ref="N7:N28" si="0">SUM(B7+E7*$A$3+F7*$B$3+G7*$C$3+H7*$D$3+I7*$E$3+J7*$F$3+K7*$G$3+L7*$H$3+M7*$I$3)</f>
         <v>120</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="7">
         <f t="shared" ref="O7:O28" si="1">MEDIAN(C7,N7,D7)</f>
         <v>120</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="8">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
         <v>5.1303976058144504E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>20</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6">
         <v>15</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="6">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="8">
         <f t="shared" si="2"/>
         <v>3.4202650705429674E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>15</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6">
         <v>20</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="6">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="7">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="7">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="8">
         <f t="shared" si="2"/>
         <v>1.4963659683625482E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
         <v>10</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="6">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="7">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="7">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="8">
         <f t="shared" si="2"/>
         <v>2.5651988029072252E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>300</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="6">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="7">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="8">
         <f t="shared" si="2"/>
         <v>0.12825994014536127</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>20</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
         <v>10</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="8">
         <f t="shared" si="2"/>
         <v>3.4202650705429674E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="6">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="8">
         <f t="shared" si="2"/>
         <v>4.2753313381787093E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>0</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>5</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>15</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="6">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="7">
         <f t="shared" si="0"/>
         <v>34.5</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="8">
         <f t="shared" si="2"/>
         <v>6.412997007268063E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>300</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="6">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="7">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="8">
         <f t="shared" si="2"/>
         <v>0.12825994014536127</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>0</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>25</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <v>50</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="5">
         <v>4</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="6">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="7">
         <f t="shared" si="0"/>
         <v>138</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="7">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="8">
         <f t="shared" si="2"/>
         <v>2.1376656690893545E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>30</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6">
         <v>2</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="6">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="7">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="7">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="8">
         <f t="shared" si="2"/>
         <v>4.2325780247969215E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>400</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="6">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="7">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="7">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="8">
         <f t="shared" si="2"/>
         <v>0.17101325352714836</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>60</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6">
         <v>20</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="5">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="6">
         <v>10</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="7">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="7">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19" s="8">
         <f t="shared" si="2"/>
         <v>5.9854638734501926E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="5">
+      <c r="A20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="6">
         <v>75</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6">
         <v>5</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="6">
         <v>20</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="6">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="7">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="7">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="8">
         <f t="shared" si="2"/>
         <v>4.9166310389055154E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>55</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="6">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="7">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="7">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="8">
         <f t="shared" si="2"/>
         <v>2.3514322359982898E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>100</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="6">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="7">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="8">
         <f t="shared" si="2"/>
         <v>4.2753313381787089E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>80</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="6">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="8">
         <f t="shared" si="2"/>
         <v>3.4202650705429674E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5">
         <v>300</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="6">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="7">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="8">
         <f t="shared" si="2"/>
         <v>0.12825994014536127</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="6">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="6">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="6">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="6">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1478,11 +1485,11 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="6">
+      <c r="O29" s="7">
         <f>SUM(O7:O28)</f>
         <v>2339</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1508,668 +1515,668 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N31" s="3" t="s">
+      <c r="N31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="P31" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>200</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="6">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="7">
         <f t="shared" ref="N32:N47" si="3">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>200</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="7">
         <f t="shared" ref="O32:O50" si="4">MEDIAN(C32,N32,D32)</f>
         <v>200</v>
       </c>
-      <c r="P32" s="7">
+      <c r="P32" s="8">
         <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="5">
         <v>0</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="5">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="6">
         <v>25</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="6">
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33" s="8">
         <f t="shared" si="5"/>
         <v>5.1059484299208577E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>50</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="5">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="6">
         <v>25</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="7">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="7">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34" s="8">
         <f t="shared" si="5"/>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="6">
         <v>60</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="6">
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="7">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="7">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="P35" s="7">
+      <c r="P35" s="8">
         <f t="shared" si="5"/>
         <v>3.0635690579525147E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="6">
         <v>50</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="5">
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="6">
         <v>5</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="5">
+      <c r="I36" s="5"/>
+      <c r="J36" s="6">
         <v>20</v>
       </c>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="6">
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="7">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="7">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="P36" s="7">
+      <c r="P36" s="8">
         <f t="shared" si="5"/>
         <v>4.5953535869287722E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="6">
         <v>100</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="6">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="P37" s="7">
+      <c r="P37" s="8">
         <f t="shared" si="5"/>
         <v>5.1059484299208577E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>80</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="6">
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="7">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="O38" s="6">
+      <c r="O38" s="7">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="P38" s="7">
+      <c r="P38" s="8">
         <f t="shared" si="5"/>
         <v>4.084758743936686E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="5">
         <v>0</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="5">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6">
         <v>45</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="6">
         <v>25</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="6">
         <v>6</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="5">
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="6">
         <v>6</v>
       </c>
-      <c r="M39" s="4"/>
-      <c r="N39" s="6">
+      <c r="M39" s="5"/>
+      <c r="N39" s="7">
         <f t="shared" si="3"/>
         <v>143</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="7">
         <f t="shared" si="4"/>
         <v>143</v>
       </c>
-      <c r="P39" s="7">
+      <c r="P39" s="8">
         <f t="shared" si="5"/>
         <v>7.301506254786827E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="6">
         <v>40</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="5">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="6">
         <v>13</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="6">
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="7">
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="7">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="P40" s="7">
+      <c r="P40" s="8">
         <f t="shared" si="5"/>
         <v>4.6974725555271893E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="5">
         <v>0</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6">
         <v>20</v>
       </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="5">
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="6">
         <v>15</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N41" s="7">
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="7">
         <f t="shared" si="4"/>
         <v>130</v>
       </c>
-      <c r="P41" s="7">
+      <c r="P41" s="8">
         <f t="shared" si="5"/>
         <v>6.6377329588971148E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="6">
         <v>100</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="6">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="P42" s="7">
+      <c r="P42" s="8">
         <f t="shared" si="5"/>
         <v>5.1059484299208577E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>0</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="6">
         <v>10</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="6">
         <v>125</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="6">
         <v>1</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4">
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5">
         <v>1</v>
       </c>
-      <c r="N43" s="6">
+      <c r="N43" s="7">
         <f t="shared" si="3"/>
         <v>50.5</v>
       </c>
-      <c r="O43" s="6">
+      <c r="O43" s="7">
         <f t="shared" si="4"/>
         <v>50.5</v>
       </c>
-      <c r="P43" s="7">
+      <c r="P43" s="8">
         <f t="shared" si="5"/>
         <v>2.5785039571100333E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="6">
         <v>50</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="5">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="6">
         <v>25</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N44" s="7">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="O44" s="6">
+      <c r="O44" s="7">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="P44" s="7">
+      <c r="P44" s="8">
         <f t="shared" si="5"/>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="5">
+      <c r="A45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="6">
         <v>50</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="5">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="6">
         <v>25</v>
       </c>
-      <c r="N45" s="6">
+      <c r="N45" s="7">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="7">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="P45" s="7">
+      <c r="P45" s="8">
         <f t="shared" si="5"/>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="5">
         <v>0</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="5">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6">
         <v>12</v>
       </c>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="6">
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="7">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="O46" s="6">
+      <c r="O46" s="7">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="P46" s="7">
+      <c r="P46" s="8">
         <f t="shared" si="5"/>
         <v>2.4508552463620117E-2</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <v>60</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="5">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6">
         <v>15</v>
       </c>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="5">
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="6">
         <v>15</v>
       </c>
-      <c r="N47" s="6">
+      <c r="N47" s="7">
         <f t="shared" si="3"/>
         <v>165</v>
       </c>
-      <c r="O47" s="6">
+      <c r="O47" s="7">
         <f t="shared" si="4"/>
         <v>165</v>
       </c>
-      <c r="P47" s="7">
+      <c r="P47" s="8">
         <f t="shared" si="5"/>
         <v>8.4248149093694158E-2</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="6">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="7">
         <f t="shared" ref="N48:N50" si="6">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
         <v>0</v>
       </c>
-      <c r="O48" s="6">
+      <c r="O48" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P48" s="7">
+      <c r="P48" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="6">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="6">
+      <c r="O49" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P49" s="7">
+      <c r="P49" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="6">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="6">
+      <c r="O50" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P50" s="7">
+      <c r="P50" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2184,11 +2191,11 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="6">
+      <c r="O51" s="7">
         <f>SUM(O32:O50)</f>
         <v>1958.5</v>
       </c>
-      <c r="P51" s="7">
+      <c r="P51" s="8">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2214,616 +2221,616 @@
       <c r="P52" s="2"/>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="J53" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L53" s="3" t="s">
+      <c r="L53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M53" s="3" t="s">
+      <c r="M53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N53" s="3" t="s">
+      <c r="N53" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O53" s="3" t="s">
+      <c r="O53" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P53" s="3" t="s">
+      <c r="P53" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="6">
         <v>135</v>
       </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="6">
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="7">
         <f t="shared" ref="N54:N72" si="7">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
-      <c r="O54" s="6">
+      <c r="O54" s="7">
         <f t="shared" ref="O54:O72" si="8">MEDIAN(C54,N54,D54)</f>
         <v>135</v>
       </c>
-      <c r="P54" s="7">
+      <c r="P54" s="8">
         <f t="shared" ref="P54:P73" si="9">O54/SUM(O$54:O$72)</f>
-        <v>0.16463414634146342</v>
+        <v>0.16770186335403728</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="6">
         <v>40</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="5">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="6">
         <v>5</v>
       </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="5">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="6">
         <v>5</v>
       </c>
-      <c r="N55" s="6">
+      <c r="N55" s="7">
         <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="O55" s="6">
+      <c r="O55" s="7">
         <f t="shared" si="8"/>
         <v>90</v>
       </c>
-      <c r="P55" s="7">
+      <c r="P55" s="8">
         <f t="shared" si="9"/>
-        <v>0.10975609756097561</v>
+        <v>0.11180124223602485</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="6">
         <v>50</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="5">
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="6">
         <v>10</v>
       </c>
-      <c r="N56" s="6">
+      <c r="N56" s="7">
         <f t="shared" si="7"/>
         <v>110</v>
       </c>
-      <c r="O56" s="6">
+      <c r="O56" s="7">
         <f t="shared" si="8"/>
         <v>110</v>
       </c>
-      <c r="P56" s="7">
+      <c r="P56" s="8">
         <f t="shared" si="9"/>
-        <v>0.13414634146341464</v>
+        <v>0.13664596273291926</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="6">
         <v>40</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="5">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="6">
         <v>10</v>
       </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="6">
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="7">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="O57" s="6">
+      <c r="O57" s="7">
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
-      <c r="P57" s="7">
+      <c r="P57" s="8">
         <f t="shared" si="9"/>
-        <v>9.7560975609756101E-2</v>
+        <v>9.9378881987577633E-2</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="6">
         <v>75</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="5">
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="6">
         <v>10</v>
       </c>
-      <c r="I58" s="5">
+      <c r="I58" s="6">
         <v>20</v>
       </c>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="6">
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="7">
         <f t="shared" si="7"/>
         <v>135</v>
       </c>
-      <c r="O58" s="6">
+      <c r="O58" s="7">
         <f t="shared" si="8"/>
         <v>135</v>
       </c>
-      <c r="P58" s="7">
+      <c r="P58" s="8">
         <f t="shared" si="9"/>
-        <v>0.16463414634146342</v>
+        <v>0.16770186335403728</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="6">
         <v>20</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="5">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="6">
         <v>15</v>
       </c>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="6">
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="7">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="O59" s="6">
+      <c r="O59" s="7">
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
-      <c r="P59" s="7">
+      <c r="P59" s="8">
         <f t="shared" si="9"/>
-        <v>9.7560975609756101E-2</v>
+        <v>9.9378881987577633E-2</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="5">
+      <c r="A60" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6">
+        <v>10</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="6">
+        <v>10</v>
+      </c>
+      <c r="N60" s="7">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="O60" s="7">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="P60" s="8">
+        <f t="shared" si="9"/>
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61" s="5">
         <v>25</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="5">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5">
+        <v>5</v>
+      </c>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5">
         <v>10</v>
       </c>
-      <c r="N60" s="6">
-        <f t="shared" si="7"/>
-        <v>85</v>
-      </c>
-      <c r="O60" s="6">
-        <f t="shared" si="8"/>
-        <v>85</v>
-      </c>
-      <c r="P60" s="7">
-        <f t="shared" si="9"/>
-        <v>0.10365853658536585</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61" s="4">
-        <v>25</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4">
-        <v>5</v>
-      </c>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4">
-        <v>10</v>
-      </c>
-      <c r="N61" s="6">
+      <c r="N61" s="7">
         <f t="shared" si="7"/>
         <v>105</v>
       </c>
-      <c r="O61" s="6">
+      <c r="O61" s="7">
         <f t="shared" si="8"/>
         <v>105</v>
       </c>
-      <c r="P61" s="7">
+      <c r="P61" s="8">
         <f t="shared" si="9"/>
-        <v>0.12804878048780488</v>
+        <v>0.13043478260869565</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="6">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O62" s="6">
+      <c r="O62" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P62" s="7">
+      <c r="P62" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="6">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O63" s="6">
+      <c r="O63" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P63" s="7">
+      <c r="P63" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="6">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O64" s="6">
+      <c r="O64" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P64" s="7">
+      <c r="P64" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="6">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O65" s="6">
+      <c r="O65" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P65" s="7">
+      <c r="P65" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="6">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O66" s="6">
+      <c r="O66" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P66" s="7">
+      <c r="P66" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="6">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O67" s="6">
+      <c r="O67" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P67" s="7">
+      <c r="P67" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="6">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O68" s="6">
+      <c r="O68" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P68" s="7">
+      <c r="P68" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="6">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O69" s="6">
+      <c r="O69" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P69" s="7">
+      <c r="P69" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="6">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O70" s="6">
+      <c r="O70" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P70" s="7">
+      <c r="P70" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="6">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O71" s="6">
+      <c r="O71" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P71" s="7">
+      <c r="P71" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
-      <c r="N72" s="6">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O72" s="6">
+      <c r="O72" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P72" s="7">
+      <c r="P72" s="8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -2838,11 +2845,11 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="N73" s="2"/>
-      <c r="O73" s="6">
+      <c r="O73" s="7">
         <f>SUM(O53:O72)</f>
-        <v>820</v>
-      </c>
-      <c r="P73" s="7">
+        <v>805</v>
+      </c>
+      <c r="P73" s="8">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Remove Bear Attack (#3611)
No one seems to like it.
Associated Thread: https://forums.aurorastation.org/viewtopic.php?f=18&t=8579
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erki\Documents\GitHub\Skull132\Aurora.3\tools\Event Probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Aurora\Maploader\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Space Vines</t>
   </si>
   <si>
-    <t>Bear Attack</t>
-  </si>
-  <si>
     <t>Wallrot</t>
   </si>
   <si>
@@ -204,8 +201,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,6 +210,11 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -259,15 +261,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,28 +584,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P999"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="13" width="7" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="26" width="7" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" customWidth="1"/>
+    <col min="9" max="13" width="7" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" style="3" customWidth="1"/>
+    <col min="17" max="26" width="7" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="15.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -621,31 +625,31 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="2"/>
@@ -653,32 +657,32 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <f>SUM(B3:I3)*1.5</f>
         <v>34.5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>4</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <v>4</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>6</v>
       </c>
       <c r="N3" s="2"/>
@@ -723,747 +727,747 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>120</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="6">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="7">
         <f t="shared" ref="N7:N28" si="0">SUM(B7+E7*$A$3+F7*$B$3+G7*$C$3+H7*$D$3+I7*$E$3+J7*$F$3+K7*$G$3+L7*$H$3+M7*$I$3)</f>
         <v>120</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="7">
         <f t="shared" ref="O7:O28" si="1">MEDIAN(C7,N7,D7)</f>
         <v>120</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="8">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
         <v>5.1303976058144504E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>20</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6">
         <v>15</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="6">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="8">
         <f t="shared" si="2"/>
         <v>3.4202650705429674E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>15</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6">
         <v>20</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="6">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="7">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="7">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="8">
         <f t="shared" si="2"/>
         <v>1.4963659683625482E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
         <v>10</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="6">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="7">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="7">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="8">
         <f t="shared" si="2"/>
         <v>2.5651988029072252E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>300</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="6">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="7">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="8">
         <f t="shared" si="2"/>
         <v>0.12825994014536127</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>20</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
         <v>10</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="8">
         <f t="shared" si="2"/>
         <v>3.4202650705429674E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="6">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="8">
         <f t="shared" si="2"/>
         <v>4.2753313381787093E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>0</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>5</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>15</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="6">
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="7">
         <f t="shared" si="0"/>
         <v>34.5</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="8">
         <f t="shared" si="2"/>
         <v>6.412997007268063E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>300</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="6">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="7">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="8">
         <f t="shared" si="2"/>
         <v>0.12825994014536127</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>0</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>25</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <v>50</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="5">
         <v>4</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="6">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="7">
         <f t="shared" si="0"/>
         <v>138</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="7">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="8">
         <f t="shared" si="2"/>
         <v>2.1376656690893545E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>30</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6">
         <v>2</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="6">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="7">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="7">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="8">
         <f t="shared" si="2"/>
         <v>4.2325780247969215E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>400</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="6">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="7">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="7">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="8">
         <f t="shared" si="2"/>
         <v>0.17101325352714836</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>60</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6">
         <v>20</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="5">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="6">
         <v>10</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="7">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="7">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19" s="8">
         <f t="shared" si="2"/>
         <v>5.9854638734501926E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="5">
+      <c r="A20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="6">
         <v>75</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6">
         <v>5</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="6">
         <v>20</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="6">
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="7">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="7">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="8">
         <f t="shared" si="2"/>
         <v>4.9166310389055154E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>55</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="6">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="7">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="7">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="8">
         <f t="shared" si="2"/>
         <v>2.3514322359982898E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>100</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="6">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="7">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="7">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="8">
         <f t="shared" si="2"/>
         <v>4.2753313381787089E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>80</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="6">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="7">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="7">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="8">
         <f t="shared" si="2"/>
         <v>3.4202650705429674E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5">
         <v>300</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="6">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="7">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="7">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="8">
         <f t="shared" si="2"/>
         <v>0.12825994014536127</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="6">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="6">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="6">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="6">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1478,11 +1482,11 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="6">
+      <c r="O29" s="7">
         <f>SUM(O7:O28)</f>
         <v>2339</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1508,668 +1512,668 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N31" s="3" t="s">
+      <c r="N31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="P31" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>200</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="6">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="7">
         <f t="shared" ref="N32:N47" si="3">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>200</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="7">
         <f t="shared" ref="O32:O50" si="4">MEDIAN(C32,N32,D32)</f>
         <v>200</v>
       </c>
-      <c r="P32" s="7">
+      <c r="P32" s="8">
         <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="5">
         <v>0</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="5">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="6">
         <v>25</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="6">
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33" s="8">
         <f t="shared" si="5"/>
         <v>5.1059484299208577E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>50</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="5">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="6">
         <v>25</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="7">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="7">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34" s="8">
         <f t="shared" si="5"/>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="6">
         <v>60</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="6">
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="7">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="7">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="P35" s="7">
+      <c r="P35" s="8">
         <f t="shared" si="5"/>
         <v>3.0635690579525147E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="6">
         <v>50</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="5">
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="6">
         <v>5</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="5">
+      <c r="I36" s="5"/>
+      <c r="J36" s="6">
         <v>20</v>
       </c>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="6">
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="7">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="7">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="P36" s="7">
+      <c r="P36" s="8">
         <f t="shared" si="5"/>
         <v>4.5953535869287722E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="6">
         <v>100</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="6">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="P37" s="7">
+      <c r="P37" s="8">
         <f t="shared" si="5"/>
         <v>5.1059484299208577E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>80</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="6">
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="7">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="O38" s="6">
+      <c r="O38" s="7">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="P38" s="7">
+      <c r="P38" s="8">
         <f t="shared" si="5"/>
         <v>4.084758743936686E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="5">
         <v>0</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="5">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6">
         <v>45</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="6">
         <v>25</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="6">
         <v>6</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="5">
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="6">
         <v>6</v>
       </c>
-      <c r="M39" s="4"/>
-      <c r="N39" s="6">
+      <c r="M39" s="5"/>
+      <c r="N39" s="7">
         <f t="shared" si="3"/>
         <v>143</v>
       </c>
-      <c r="O39" s="6">
+      <c r="O39" s="7">
         <f t="shared" si="4"/>
         <v>143</v>
       </c>
-      <c r="P39" s="7">
+      <c r="P39" s="8">
         <f t="shared" si="5"/>
         <v>7.301506254786827E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="6">
         <v>40</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="5">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="6">
         <v>13</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="6">
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="7">
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="7">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="P40" s="7">
+      <c r="P40" s="8">
         <f t="shared" si="5"/>
         <v>4.6974725555271893E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="5">
         <v>0</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="6">
         <v>20</v>
       </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="5">
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="6">
         <v>15</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N41" s="7">
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="7">
         <f t="shared" si="4"/>
         <v>130</v>
       </c>
-      <c r="P41" s="7">
+      <c r="P41" s="8">
         <f t="shared" si="5"/>
         <v>6.6377329588971148E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="6">
         <v>100</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="6">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="7">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="7">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="P42" s="7">
+      <c r="P42" s="8">
         <f t="shared" si="5"/>
         <v>5.1059484299208577E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>0</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="6">
         <v>10</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="6">
         <v>125</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="6">
         <v>1</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4">
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5">
         <v>1</v>
       </c>
-      <c r="N43" s="6">
+      <c r="N43" s="7">
         <f t="shared" si="3"/>
         <v>50.5</v>
       </c>
-      <c r="O43" s="6">
+      <c r="O43" s="7">
         <f t="shared" si="4"/>
         <v>50.5</v>
       </c>
-      <c r="P43" s="7">
+      <c r="P43" s="8">
         <f t="shared" si="5"/>
         <v>2.5785039571100333E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="6">
         <v>50</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="5">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="6">
         <v>25</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N44" s="7">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="O44" s="6">
+      <c r="O44" s="7">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="P44" s="7">
+      <c r="P44" s="8">
         <f t="shared" si="5"/>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="5">
+      <c r="A45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="6">
         <v>50</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="5">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="6">
         <v>25</v>
       </c>
-      <c r="N45" s="6">
+      <c r="N45" s="7">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="7">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="P45" s="7">
+      <c r="P45" s="8">
         <f t="shared" si="5"/>
         <v>0.10211896859841715</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="5">
         <v>0</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="5">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6">
         <v>12</v>
       </c>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="6">
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="7">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="O46" s="6">
+      <c r="O46" s="7">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="P46" s="7">
+      <c r="P46" s="8">
         <f t="shared" si="5"/>
         <v>2.4508552463620117E-2</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <v>60</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="5">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6">
         <v>15</v>
       </c>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="5">
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="6">
         <v>15</v>
       </c>
-      <c r="N47" s="6">
+      <c r="N47" s="7">
         <f t="shared" si="3"/>
         <v>165</v>
       </c>
-      <c r="O47" s="6">
+      <c r="O47" s="7">
         <f t="shared" si="4"/>
         <v>165</v>
       </c>
-      <c r="P47" s="7">
+      <c r="P47" s="8">
         <f t="shared" si="5"/>
         <v>8.4248149093694158E-2</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="6">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="7">
         <f t="shared" ref="N48:N50" si="6">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
         <v>0</v>
       </c>
-      <c r="O48" s="6">
+      <c r="O48" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P48" s="7">
+      <c r="P48" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="6">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="6">
+      <c r="O49" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P49" s="7">
+      <c r="P49" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="6">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="6">
+      <c r="O50" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P50" s="7">
+      <c r="P50" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2184,11 +2188,11 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="N51" s="2"/>
-      <c r="O51" s="6">
+      <c r="O51" s="7">
         <f>SUM(O32:O50)</f>
         <v>1958.5</v>
       </c>
-      <c r="P51" s="7">
+      <c r="P51" s="8">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -2214,618 +2218,604 @@
       <c r="P52" s="2"/>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="J53" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="K53" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L53" s="3" t="s">
+      <c r="L53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M53" s="3" t="s">
+      <c r="M53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N53" s="3" t="s">
+      <c r="N53" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O53" s="3" t="s">
+      <c r="O53" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P53" s="3" t="s">
+      <c r="P53" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="6">
         <v>135</v>
       </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="6">
-        <f t="shared" ref="N54:N72" si="7">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="7">
+        <f t="shared" ref="N54:N71" si="7">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
-      <c r="O54" s="6">
-        <f t="shared" ref="O54:O72" si="8">MEDIAN(C54,N54,D54)</f>
+      <c r="O54" s="7">
+        <f t="shared" ref="O54:O71" si="8">MEDIAN(C54,N54,D54)</f>
         <v>135</v>
       </c>
-      <c r="P54" s="7">
-        <f t="shared" ref="P54:P73" si="9">O54/SUM(O$54:O$72)</f>
-        <v>0.16463414634146342</v>
+      <c r="P54" s="8">
+        <f>O54/SUM(O$54:O$71)</f>
+        <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="6">
         <v>40</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="5">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="6">
         <v>5</v>
       </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="5">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="6">
         <v>5</v>
       </c>
-      <c r="N55" s="6">
+      <c r="N55" s="7">
         <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="O55" s="6">
+      <c r="O55" s="7">
         <f t="shared" si="8"/>
         <v>90</v>
       </c>
-      <c r="P55" s="7">
-        <f t="shared" si="9"/>
-        <v>0.10975609756097561</v>
+      <c r="P55" s="8">
+        <f>O55/SUM(O$54:O$71)</f>
+        <v>0.12244897959183673</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="6">
         <v>50</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="5">
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="6">
         <v>10</v>
       </c>
-      <c r="N56" s="6">
+      <c r="N56" s="7">
         <f t="shared" si="7"/>
         <v>110</v>
       </c>
-      <c r="O56" s="6">
+      <c r="O56" s="7">
         <f t="shared" si="8"/>
         <v>110</v>
       </c>
-      <c r="P56" s="7">
-        <f t="shared" si="9"/>
-        <v>0.13414634146341464</v>
+      <c r="P56" s="8">
+        <f>O56/SUM(O$54:O$71)</f>
+        <v>0.14965986394557823</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="6">
         <v>40</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="5">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="6">
         <v>10</v>
       </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="6">
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="7">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="O57" s="6">
+      <c r="O57" s="7">
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
-      <c r="P57" s="7">
-        <f t="shared" si="9"/>
-        <v>9.7560975609756101E-2</v>
+      <c r="P57" s="8">
+        <f>O57/SUM(O$54:O$71)</f>
+        <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="6">
         <v>75</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="5">
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="6">
         <v>10</v>
       </c>
-      <c r="I58" s="5">
+      <c r="I58" s="6">
         <v>20</v>
       </c>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="6">
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="7">
         <f t="shared" si="7"/>
         <v>135</v>
       </c>
-      <c r="O58" s="6">
+      <c r="O58" s="7">
         <f t="shared" si="8"/>
         <v>135</v>
       </c>
-      <c r="P58" s="7">
-        <f t="shared" si="9"/>
-        <v>0.16463414634146342</v>
+      <c r="P58" s="8">
+        <f>O58/SUM(O$54:O$71)</f>
+        <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="6">
         <v>20</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="5">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="6">
         <v>15</v>
       </c>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="6">
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="7">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="O59" s="6">
+      <c r="O59" s="7">
         <f t="shared" si="8"/>
         <v>80</v>
       </c>
-      <c r="P59" s="7">
-        <f t="shared" si="9"/>
-        <v>9.7560975609756101E-2</v>
+      <c r="P59" s="8">
+        <f>O59/SUM(O$54:O$71)</f>
+        <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B60" s="5">
         <v>25</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5">
+        <v>5</v>
+      </c>
+      <c r="L60" s="5"/>
       <c r="M60" s="5">
         <v>10</v>
       </c>
-      <c r="N60" s="6">
-        <f t="shared" si="7"/>
-        <v>85</v>
-      </c>
-      <c r="O60" s="6">
-        <f t="shared" si="8"/>
-        <v>85</v>
-      </c>
-      <c r="P60" s="7">
-        <f t="shared" si="9"/>
-        <v>0.10365853658536585</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B61" s="4">
-        <v>25</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4">
-        <v>5</v>
-      </c>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4">
-        <v>10</v>
-      </c>
-      <c r="N61" s="6">
+      <c r="N60" s="7">
         <f t="shared" si="7"/>
         <v>105</v>
       </c>
-      <c r="O61" s="6">
+      <c r="O60" s="7">
         <f t="shared" si="8"/>
         <v>105</v>
       </c>
-      <c r="P61" s="7">
-        <f t="shared" si="9"/>
-        <v>0.12804878048780488</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="6">
+      <c r="P60" s="8">
+        <f>O60/SUM(O$54:O$71)</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O62" s="6">
+      <c r="O61" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P62" s="7">
-        <f t="shared" si="9"/>
+      <c r="P61" s="8">
+        <f>O61/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="6">
+    <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O63" s="6">
+      <c r="O62" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P63" s="7">
-        <f t="shared" si="9"/>
+      <c r="P62" s="8">
+        <f>O62/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="6">
+    <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O64" s="6">
+      <c r="O63" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P64" s="7">
-        <f t="shared" si="9"/>
+      <c r="P63" s="8">
+        <f>O63/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="6">
+    <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O65" s="6">
+      <c r="O64" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P65" s="7">
-        <f t="shared" si="9"/>
+      <c r="P64" s="8">
+        <f>O64/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="6">
+    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O66" s="6">
+      <c r="O65" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P66" s="7">
-        <f t="shared" si="9"/>
+      <c r="P65" s="8">
+        <f>O65/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="6">
+    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O67" s="6">
+      <c r="O66" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P67" s="7">
-        <f t="shared" si="9"/>
+      <c r="P66" s="8">
+        <f>O66/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="6">
+    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O68" s="6">
+      <c r="O67" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P68" s="7">
-        <f t="shared" si="9"/>
+      <c r="P67" s="8">
+        <f>O67/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="6">
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O69" s="6">
+      <c r="O68" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P69" s="7">
-        <f t="shared" si="9"/>
+      <c r="P68" s="8">
+        <f>O68/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="6">
+    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O70" s="6">
+      <c r="O69" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P70" s="7">
-        <f t="shared" si="9"/>
+      <c r="P69" s="8">
+        <f>O69/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="6">
+    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O71" s="6">
+      <c r="O70" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P71" s="7">
-        <f t="shared" si="9"/>
+      <c r="P70" s="8">
+        <f>O70/SUM(O$54:O$71)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="4"/>
-      <c r="N72" s="6">
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O72" s="6">
+      <c r="O71" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P72" s="7">
-        <f t="shared" si="9"/>
+      <c r="P71" s="8">
+        <f>O71/SUM(O$54:O$71)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="7">
+        <f>SUM(O53:O71)</f>
+        <v>735</v>
+      </c>
+      <c r="P72" s="8">
+        <f>O72/SUM(O$54:O$71)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2838,14 +2828,8 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="N73" s="2"/>
-      <c r="O73" s="6">
-        <f>SUM(O53:O72)</f>
-        <v>820</v>
-      </c>
-      <c r="P73" s="7">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
     </row>
     <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
@@ -14872,19 +14856,6 @@
       <c r="O998" s="2"/>
       <c r="P998" s="2"/>
     </row>
-    <row r="999" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add lore news loaded from the DB
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Aurora\Maploader\tools\Event Probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\GitHub\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -197,6 +197,9 @@
   <si>
     <t>CCIAA General Notice</t>
   </si>
+  <si>
+    <t>Lore News</t>
+  </si>
 </sst>
 </file>
 
@@ -261,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,6 +274,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -804,7 +808,7 @@
       </c>
       <c r="P7" s="8">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>5.1303976058144504E-2</v>
+        <v>5.3595355069227336E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,7 +841,7 @@
       </c>
       <c r="P8" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>3.573023671281822E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,7 +874,7 @@
       </c>
       <c r="P9" s="8">
         <f t="shared" si="2"/>
-        <v>1.4963659683625482E-2</v>
+        <v>1.5631978561857971E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +907,7 @@
       </c>
       <c r="P10" s="8">
         <f t="shared" si="2"/>
-        <v>2.5651988029072252E-2</v>
+        <v>2.6797677534613668E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -934,7 +938,7 @@
       </c>
       <c r="P11" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0.13398838767306834</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,7 +971,7 @@
       </c>
       <c r="P12" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>3.573023671281822E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -998,7 +1002,7 @@
       </c>
       <c r="P13" s="8">
         <f t="shared" si="2"/>
-        <v>4.2753313381787093E-3</v>
+        <v>4.4662795891022775E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1035,7 +1039,7 @@
       </c>
       <c r="P14" s="8">
         <f t="shared" si="2"/>
-        <v>6.412997007268063E-3</v>
+        <v>6.6994193836534171E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1043,7 +1047,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="5">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1058,15 +1062,15 @@
       <c r="M15" s="5"/>
       <c r="N15" s="7">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="O15" s="7">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>8.9325591782045549E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1094,16 +1098,16 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B16+E16*$A$3+F16*$B$3+G16*$C$3+H16*$D$3+I16*$E$3+J16*$F$3+K16*$G$3+L16*$H$3+M16*$I$3)</f>
         <v>138</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C16,N16,D16)</f>
         <v>50</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" si="2"/>
-        <v>2.1376656690893545E-2</v>
+        <v>2.2331397945511387E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1127,16 +1131,16 @@
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B17+E17*$A$3+F17*$B$3+G17*$C$3+H17*$D$3+I17*$E$3+J17*$F$3+K17*$G$3+L17*$H$3+M17*$I$3)</f>
         <v>99</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C17,N17,D17)</f>
         <v>99</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" si="2"/>
-        <v>4.2325780247969215E-2</v>
+        <v>4.4216167932112548E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1144,7 +1148,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="5">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1158,16 +1162,16 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="7">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>SUM(B18+E18*$A$3+F18*$B$3+G18*$C$3+H18*$D$3+I18*$E$3+J18*$F$3+K18*$G$3+L18*$H$3+M18*$I$3)</f>
+        <v>100</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="1"/>
-        <v>400</v>
+        <f>MEDIAN(C18,N18,D18)</f>
+        <v>100</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="2"/>
-        <v>0.17101325352714836</v>
+        <v>4.4662795891022775E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1193,16 +1197,16 @@
         <v>10</v>
       </c>
       <c r="N19" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B19+E19*$A$3+F19*$B$3+G19*$C$3+H19*$D$3+I19*$E$3+J19*$F$3+K19*$G$3+L19*$H$3+M19*$I$3)</f>
         <v>140</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C19,N19,D19)</f>
         <v>140</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" si="2"/>
-        <v>5.9854638734501926E-2</v>
+        <v>6.2527914247431884E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1228,16 +1232,16 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B20+E20*$A$3+F20*$B$3+G20*$C$3+H20*$D$3+I20*$E$3+J20*$F$3+K20*$G$3+L20*$H$3+M20*$I$3)</f>
         <v>115</v>
       </c>
       <c r="O20" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C20,N20,D20)</f>
         <v>115</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="2"/>
-        <v>4.9166310389055154E-2</v>
+        <v>5.1362215274676194E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1259,16 +1263,16 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B21+E21*$A$3+F21*$B$3+G21*$C$3+H21*$D$3+I21*$E$3+J21*$F$3+K21*$G$3+L21*$H$3+M21*$I$3)</f>
         <v>55</v>
       </c>
       <c r="O21" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C21,N21,D21)</f>
         <v>55</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="2"/>
-        <v>2.3514322359982898E-2</v>
+        <v>2.4564537740062529E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1290,16 +1294,16 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B22+E22*$A$3+F22*$B$3+G22*$C$3+H22*$D$3+I22*$E$3+J22*$F$3+K22*$G$3+L22*$H$3+M22*$I$3)</f>
         <v>100</v>
       </c>
       <c r="O22" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C22,N22,D22)</f>
         <v>100</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="2"/>
-        <v>4.2753313381787089E-2</v>
+        <v>4.4662795891022775E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1321,16 +1325,16 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B23+E23*$A$3+F23*$B$3+G23*$C$3+H23*$D$3+I23*$E$3+J23*$F$3+K23*$G$3+L23*$H$3+M23*$I$3)</f>
         <v>80</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C23,N23,D23)</f>
         <v>80</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>3.573023671281822E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1352,21 +1356,25 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B24+E24*$A$3+F24*$B$3+G24*$C$3+H24*$D$3+I24*$E$3+J24*$F$3+K24*$G$3+L24*$H$3+M24*$I$3)</f>
         <v>300</v>
       </c>
       <c r="O24" s="7">
-        <f t="shared" si="1"/>
+        <f>MEDIAN(C24,N24,D24)</f>
         <v>300</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0.13398838767306834</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="5">
+        <v>300</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1379,16 +1387,16 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
       <c r="N25" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(B25+E25*$A$3+F25*$B$3+G25*$C$3+H25*$D$3+I25*$E$3+J25*$F$3+K25*$G$3+L25*$H$3+M25*$I$3)</f>
+        <v>300</v>
       </c>
       <c r="O25" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>MEDIAN(C25,N25,D25)</f>
+        <v>300</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.13398838767306834</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1484,7 +1492,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="7">
         <f>SUM(O7:O28)</f>
-        <v>2339</v>
+        <v>2239</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="2"/>
@@ -2294,7 +2302,7 @@
         <v>135</v>
       </c>
       <c r="P54" s="8">
-        <f>O54/SUM(O$54:O$71)</f>
+        <f t="shared" ref="P54:P72" si="9">O54/SUM(O$54:O$71)</f>
         <v>0.18367346938775511</v>
       </c>
     </row>
@@ -2329,7 +2337,7 @@
         <v>90</v>
       </c>
       <c r="P55" s="8">
-        <f>O55/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.12244897959183673</v>
       </c>
     </row>
@@ -2362,7 +2370,7 @@
         <v>110</v>
       </c>
       <c r="P56" s="8">
-        <f>O56/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.14965986394557823</v>
       </c>
     </row>
@@ -2395,7 +2403,7 @@
         <v>80</v>
       </c>
       <c r="P57" s="8">
-        <f>O57/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
@@ -2430,7 +2438,7 @@
         <v>135</v>
       </c>
       <c r="P58" s="8">
-        <f>O58/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.18367346938775511</v>
       </c>
     </row>
@@ -2463,7 +2471,7 @@
         <v>80</v>
       </c>
       <c r="P59" s="8">
-        <f>O59/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
@@ -2498,7 +2506,7 @@
         <v>105</v>
       </c>
       <c r="P60" s="8">
-        <f>O60/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -2525,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="P61" s="8">
-        <f>O61/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2552,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="8">
-        <f>O62/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2579,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="P63" s="8">
-        <f>O63/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2606,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="P64" s="8">
-        <f>O64/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2633,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="P65" s="8">
-        <f>O65/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2660,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="8">
-        <f>O66/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2687,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="P67" s="8">
-        <f>O67/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2714,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="P68" s="8">
-        <f>O68/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2741,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="P69" s="8">
-        <f>O69/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2768,7 +2776,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="8">
-        <f>O70/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2795,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="P71" s="8">
-        <f>O71/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2814,7 +2822,7 @@
         <v>735</v>
       </c>
       <c r="P72" s="8">
-        <f>O72/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed the trivial news from the event rotation. Added in the currently unused xenobio and virology containment events
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Aurora\Maploader\tools\Event Probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekte\SS13\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BA166FF8-B3CC-49F7-8913-2567B97BB06F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -111,12 +112,6 @@
     <t>PDA Spam</t>
   </si>
   <si>
-    <t>Shipping Error</t>
-  </si>
-  <si>
-    <t>Trivial News</t>
-  </si>
-  <si>
     <t>Vermin Infestation</t>
   </si>
   <si>
@@ -197,12 +192,18 @@
   <si>
     <t>CCIAA General Notice</t>
   </si>
+  <si>
+    <t>Containment Error - Virology</t>
+  </si>
+  <si>
+    <t>Containment Error - Xenobiology</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -218,6 +219,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -261,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,9 +278,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -289,7 +297,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -587,11 +595,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
@@ -804,7 +812,7 @@
       </c>
       <c r="P7" s="8">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>5.1303976058144504E-2</v>
+        <v>6.5217391304347824E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,7 +845,7 @@
       </c>
       <c r="P8" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,7 +878,7 @@
       </c>
       <c r="P9" s="8">
         <f t="shared" si="2"/>
-        <v>1.4963659683625482E-2</v>
+        <v>1.9021739130434784E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +911,7 @@
       </c>
       <c r="P10" s="8">
         <f t="shared" si="2"/>
-        <v>2.5651988029072252E-2</v>
+        <v>3.2608695652173912E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -934,7 +942,7 @@
       </c>
       <c r="P11" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,7 +975,7 @@
       </c>
       <c r="P12" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -998,7 +1006,7 @@
       </c>
       <c r="P13" s="8">
         <f t="shared" si="2"/>
-        <v>4.2753313381787093E-3</v>
+        <v>5.434782608695652E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1035,7 +1043,7 @@
       </c>
       <c r="P14" s="8">
         <f t="shared" si="2"/>
-        <v>6.412997007268063E-3</v>
+        <v>8.152173913043478E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,7 +1074,7 @@
       </c>
       <c r="P15" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1103,79 +1111,85 @@
       </c>
       <c r="P16" s="8">
         <f t="shared" si="2"/>
-        <v>2.1376656690893545E-2</v>
+        <v>2.717391304347826E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="6">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="6">
-        <v>2</v>
-      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="6">
+        <v>20</v>
+      </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="M17" s="6">
+        <v>10</v>
+      </c>
       <c r="N17" s="7">
-        <f t="shared" si="0"/>
-        <v>99</v>
+        <f>SUM(B17+E17*$A$3+F17*$B$3+G17*$C$3+H17*$D$3+I17*$E$3+J17*$F$3+K17*$G$3+L17*$H$3+M17*$I$3)</f>
+        <v>140</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" si="1"/>
-        <v>99</v>
+        <f>MEDIAN(C17,N17,D17)</f>
+        <v>140</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" si="2"/>
-        <v>4.2325780247969215E-2</v>
+        <v>7.6086956521739135E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="5">
-        <v>400</v>
+        <v>54</v>
+      </c>
+      <c r="B18" s="6">
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6">
+        <v>20</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="7">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>SUM(B18+E18*$A$3+F18*$B$3+G18*$C$3+H18*$D$3+I18*$E$3+J18*$F$3+K18*$G$3+L18*$H$3+M18*$I$3)</f>
+        <v>115</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="1"/>
-        <v>400</v>
+        <f>MEDIAN(C18,N18,D18)</f>
+        <v>115</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="2"/>
-        <v>0.17101325352714836</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>32</v>
+      <c r="A19" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B19" s="6">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1184,60 +1198,52 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="6">
-        <v>20</v>
-      </c>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="6">
-        <v>10</v>
-      </c>
+      <c r="M19" s="5"/>
       <c r="N19" s="7">
-        <f t="shared" si="0"/>
-        <v>140</v>
+        <f>SUM(B19+E19*$A$3+F19*$B$3+G19*$C$3+H19*$D$3+I19*$E$3+J19*$F$3+K19*$G$3+L19*$H$3+M19*$I$3)</f>
+        <v>55</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" si="1"/>
-        <v>140</v>
+        <f>MEDIAN(C19,N19,D19)</f>
+        <v>55</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" si="2"/>
-        <v>5.9854638734501926E-2</v>
+        <v>2.9891304347826088E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>56</v>
+      <c r="A20" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B20" s="6">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="6">
-        <v>5</v>
-      </c>
-      <c r="I20" s="6">
-        <v>20</v>
-      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="7">
-        <f t="shared" si="0"/>
-        <v>115</v>
+        <f>SUM(B20+E20*$A$3+F20*$B$3+G20*$C$3+H20*$D$3+I20*$E$3+J20*$F$3+K20*$G$3+L20*$H$3+M20*$I$3)</f>
+        <v>100</v>
       </c>
       <c r="O20" s="7">
-        <f t="shared" si="1"/>
-        <v>115</v>
+        <f>MEDIAN(C20,N20,D20)</f>
+        <v>100</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="2"/>
-        <v>4.9166310389055154E-2</v>
+        <v>5.434782608695652E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1245,7 +1251,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="6">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1259,24 +1265,24 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="7">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <f>SUM(B21+E21*$A$3+F21*$B$3+G21*$C$3+H21*$D$3+I21*$E$3+J21*$F$3+K21*$G$3+L21*$H$3+M21*$I$3)</f>
+        <v>80</v>
       </c>
       <c r="O21" s="7">
-        <f t="shared" si="1"/>
-        <v>55</v>
+        <f>MEDIAN(C21,N21,D21)</f>
+        <v>80</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="2"/>
-        <v>2.3514322359982898E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="6">
-        <v>100</v>
+      <c r="A22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="5">
+        <v>300</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1290,25 +1296,21 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(B22+E22*$A$3+F22*$B$3+G22*$C$3+H22*$D$3+I22*$E$3+J22*$F$3+K22*$G$3+L22*$H$3+M22*$I$3)</f>
+        <v>300</v>
       </c>
       <c r="O22" s="7">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>MEDIAN(C22,N22,D22)</f>
+        <v>300</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="2"/>
-        <v>4.2753313381787089E-2</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="6">
-        <v>80</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1321,25 +1323,21 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="7">
-        <f t="shared" si="0"/>
-        <v>80</v>
+        <f>SUM(B23+E23*$A$3+F23*$B$3+G23*$C$3+H23*$D$3+I23*$E$3+J23*$F$3+K23*$G$3+L23*$H$3+M23*$I$3)</f>
+        <v>0</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>MEDIAN(C23,N23,D23)</f>
+        <v>0</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="5">
-        <v>300</v>
-      </c>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1352,16 +1350,16 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="7">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>SUM(B24+E24*$A$3+F24*$B$3+G24*$C$3+H24*$D$3+I24*$E$3+J24*$F$3+K24*$G$3+L24*$H$3+M24*$I$3)</f>
+        <v>0</v>
       </c>
       <c r="O24" s="7">
-        <f t="shared" si="1"/>
-        <v>300</v>
+        <f>MEDIAN(C24,N24,D24)</f>
+        <v>0</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1484,7 +1482,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="7">
         <f>SUM(O7:O28)</f>
-        <v>2339</v>
+        <v>1840</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="2"/>
@@ -1493,7 +1491,7 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1589,12 +1587,12 @@
       </c>
       <c r="P32" s="8">
         <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
-        <v>0.10211896859841715</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -1622,12 +1620,12 @@
       </c>
       <c r="P33" s="8">
         <f t="shared" si="5"/>
-        <v>5.1059484299208577E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6">
         <v>50</v>
@@ -1655,12 +1653,12 @@
       </c>
       <c r="P34" s="8">
         <f t="shared" si="5"/>
-        <v>0.10211896859841715</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="6">
         <v>60</v>
@@ -1686,12 +1684,12 @@
       </c>
       <c r="P35" s="8">
         <f t="shared" si="5"/>
-        <v>3.0635690579525147E-2</v>
+        <v>2.7797081306462822E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="6">
         <v>50</v>
@@ -1721,12 +1719,12 @@
       </c>
       <c r="P36" s="8">
         <f t="shared" si="5"/>
-        <v>4.5953535869287722E-2</v>
+        <v>4.1695621959694229E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" s="6">
         <v>100</v>
@@ -1752,12 +1750,12 @@
       </c>
       <c r="P37" s="8">
         <f t="shared" si="5"/>
-        <v>5.1059484299208577E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6">
         <v>80</v>
@@ -1783,12 +1781,12 @@
       </c>
       <c r="P38" s="8">
         <f t="shared" si="5"/>
-        <v>4.084758743936686E-2</v>
+        <v>3.7062775075283765E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -1822,12 +1820,12 @@
       </c>
       <c r="P39" s="8">
         <f t="shared" si="5"/>
-        <v>7.301506254786827E-2</v>
+        <v>6.6249710447069718E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6">
         <v>40</v>
@@ -1855,12 +1853,12 @@
       </c>
       <c r="P40" s="8">
         <f t="shared" si="5"/>
-        <v>4.6974725555271893E-2</v>
+        <v>4.2622191336576326E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -1890,25 +1888,29 @@
       </c>
       <c r="P41" s="8">
         <f t="shared" si="5"/>
-        <v>6.6377329588971148E-2</v>
+        <v>6.0227009497336115E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>46</v>
+      <c r="A42" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="B42" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="G42" s="5">
+        <v>20</v>
+      </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="6"/>
+      <c r="K42" s="6">
+        <v>15</v>
+      </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="7">
@@ -1921,54 +1923,50 @@
       </c>
       <c r="P42" s="8">
         <f t="shared" si="5"/>
-        <v>5.1059484299208577E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>47</v>
+      <c r="A43" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="6">
         <v>0</v>
       </c>
-      <c r="C43" s="6">
-        <v>10</v>
-      </c>
-      <c r="D43" s="6">
-        <v>125</v>
-      </c>
-      <c r="E43" s="6">
-        <v>1</v>
-      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="G43" s="5">
+        <v>20</v>
+      </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5">
-        <v>1</v>
-      </c>
+      <c r="L43" s="5">
+        <v>15</v>
+      </c>
+      <c r="M43" s="5"/>
       <c r="N43" s="7">
         <f t="shared" si="3"/>
-        <v>50.5</v>
+        <v>100</v>
       </c>
       <c r="O43" s="7">
         <f t="shared" si="4"/>
-        <v>50.5</v>
+        <v>100</v>
       </c>
       <c r="P43" s="8">
         <f t="shared" si="5"/>
-        <v>2.5785039571100333E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B44" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1978,34 +1976,38 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
+      <c r="K44" s="6"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="6">
-        <v>25</v>
-      </c>
+      <c r="M44" s="5"/>
       <c r="N44" s="7">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O44" s="7">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="P44" s="8">
         <f t="shared" si="5"/>
-        <v>0.10211896859841715</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B45" s="6">
-        <v>50</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="C45" s="6">
+        <v>10</v>
+      </c>
+      <c r="D45" s="6">
+        <v>125</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1</v>
+      </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -2013,28 +2015,28 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="6">
-        <v>25</v>
+      <c r="M45" s="5">
+        <v>1</v>
       </c>
       <c r="N45" s="7">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>50.5</v>
       </c>
       <c r="O45" s="7">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>50.5</v>
       </c>
       <c r="P45" s="8">
         <f t="shared" si="5"/>
-        <v>0.10211896859841715</v>
+        <v>2.3395876766272874E-2</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="6">
         <v>50</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2044,30 +2046,30 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="6">
-        <v>12</v>
-      </c>
+      <c r="K46" s="5"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
+      <c r="M46" s="6">
+        <v>25</v>
+      </c>
       <c r="N46" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="O46" s="7">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="P46" s="8">
         <f t="shared" si="5"/>
-        <v>2.4508552463620117E-2</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B47" s="6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2076,30 +2078,32 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="6">
-        <v>15</v>
-      </c>
+      <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="6">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N47" s="7">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="O47" s="7">
         <f t="shared" si="4"/>
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="P47" s="8">
         <f t="shared" si="5"/>
-        <v>8.4248149093694158E-2</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -2108,25 +2112,31 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
+      <c r="K48" s="6">
+        <v>12</v>
+      </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="7">
         <f t="shared" ref="N48:N50" si="6">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="O48" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="P48" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.2237665045170257E-2</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="6">
+        <v>60</v>
+      </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -2134,21 +2144,25 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
+      <c r="J49" s="6">
+        <v>15</v>
+      </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
+      <c r="M49" s="6">
+        <v>15</v>
+      </c>
       <c r="N49" s="7">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="O49" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="P49" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.6441973592772758E-2</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2190,7 +2204,7 @@
       <c r="N51" s="2"/>
       <c r="O51" s="7">
         <f>SUM(O32:O50)</f>
-        <v>1958.5</v>
+        <v>2158.5</v>
       </c>
       <c r="P51" s="8">
         <f t="shared" si="5"/>
@@ -2199,7 +2213,7 @@
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2294,13 +2308,13 @@
         <v>135</v>
       </c>
       <c r="P54" s="8">
-        <f>O54/SUM(O$54:O$71)</f>
+        <f t="shared" ref="P54:P72" si="9">O54/SUM(O$54:O$71)</f>
         <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55" s="6">
         <v>40</v>
@@ -2329,13 +2343,13 @@
         <v>90</v>
       </c>
       <c r="P55" s="8">
-        <f>O55/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.12244897959183673</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B56" s="6">
         <v>50</v>
@@ -2362,13 +2376,13 @@
         <v>110</v>
       </c>
       <c r="P56" s="8">
-        <f>O56/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.14965986394557823</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B57" s="6">
         <v>40</v>
@@ -2395,13 +2409,13 @@
         <v>80</v>
       </c>
       <c r="P57" s="8">
-        <f>O57/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B58" s="6">
         <v>75</v>
@@ -2430,13 +2444,13 @@
         <v>135</v>
       </c>
       <c r="P58" s="8">
-        <f>O58/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B59" s="6">
         <v>20</v>
@@ -2463,13 +2477,13 @@
         <v>80</v>
       </c>
       <c r="P59" s="8">
-        <f>O59/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="5">
         <v>25</v>
@@ -2498,7 +2512,7 @@
         <v>105</v>
       </c>
       <c r="P60" s="8">
-        <f>O60/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -2525,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="P61" s="8">
-        <f>O61/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2552,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="8">
-        <f>O62/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2579,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="P63" s="8">
-        <f>O63/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2606,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="P64" s="8">
-        <f>O64/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2633,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="P65" s="8">
-        <f>O65/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2660,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="8">
-        <f>O66/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2687,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="P67" s="8">
-        <f>O67/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2714,7 +2728,7 @@
         <v>0</v>
       </c>
       <c r="P68" s="8">
-        <f>O68/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2741,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="P69" s="8">
-        <f>O69/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2768,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="8">
-        <f>O70/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2795,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="P71" s="8">
-        <f>O71/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2814,7 +2828,7 @@
         <v>735</v>
       </c>
       <c r="P72" s="8">
-        <f>O72/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -14858,5 +14872,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Load static lore news from the DB at the start of the round (#4618)
Converts the news network into a subsystem
Loads news from a database at the start of the round
No longer ties the PDAs to the tcoms system to access the news (which was broken anyway)
Removes the trivial news event
Adds the already existing virology / xenobiology containment events to the rotation
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Aurora\Maploader\tools\Event Probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekte\SS13\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BA166FF8-B3CC-49F7-8913-2567B97BB06F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -111,12 +112,6 @@
     <t>PDA Spam</t>
   </si>
   <si>
-    <t>Shipping Error</t>
-  </si>
-  <si>
-    <t>Trivial News</t>
-  </si>
-  <si>
     <t>Vermin Infestation</t>
   </si>
   <si>
@@ -197,12 +192,18 @@
   <si>
     <t>CCIAA General Notice</t>
   </si>
+  <si>
+    <t>Containment Error - Virology</t>
+  </si>
+  <si>
+    <t>Containment Error - Xenobiology</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -218,6 +219,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -261,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,9 +278,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -289,7 +297,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -587,11 +595,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
@@ -804,7 +812,7 @@
       </c>
       <c r="P7" s="8">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>5.1303976058144504E-2</v>
+        <v>6.5217391304347824E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,7 +845,7 @@
       </c>
       <c r="P8" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,7 +878,7 @@
       </c>
       <c r="P9" s="8">
         <f t="shared" si="2"/>
-        <v>1.4963659683625482E-2</v>
+        <v>1.9021739130434784E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +911,7 @@
       </c>
       <c r="P10" s="8">
         <f t="shared" si="2"/>
-        <v>2.5651988029072252E-2</v>
+        <v>3.2608695652173912E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -934,7 +942,7 @@
       </c>
       <c r="P11" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,7 +975,7 @@
       </c>
       <c r="P12" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -998,7 +1006,7 @@
       </c>
       <c r="P13" s="8">
         <f t="shared" si="2"/>
-        <v>4.2753313381787093E-3</v>
+        <v>5.434782608695652E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1035,7 +1043,7 @@
       </c>
       <c r="P14" s="8">
         <f t="shared" si="2"/>
-        <v>6.412997007268063E-3</v>
+        <v>8.152173913043478E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,7 +1074,7 @@
       </c>
       <c r="P15" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1103,79 +1111,85 @@
       </c>
       <c r="P16" s="8">
         <f t="shared" si="2"/>
-        <v>2.1376656690893545E-2</v>
+        <v>2.717391304347826E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="6">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="6">
-        <v>2</v>
-      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="6">
+        <v>20</v>
+      </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="M17" s="6">
+        <v>10</v>
+      </c>
       <c r="N17" s="7">
-        <f t="shared" si="0"/>
-        <v>99</v>
+        <f>SUM(B17+E17*$A$3+F17*$B$3+G17*$C$3+H17*$D$3+I17*$E$3+J17*$F$3+K17*$G$3+L17*$H$3+M17*$I$3)</f>
+        <v>140</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" si="1"/>
-        <v>99</v>
+        <f>MEDIAN(C17,N17,D17)</f>
+        <v>140</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" si="2"/>
-        <v>4.2325780247969215E-2</v>
+        <v>7.6086956521739135E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="5">
-        <v>400</v>
+        <v>54</v>
+      </c>
+      <c r="B18" s="6">
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6">
+        <v>20</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="7">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>SUM(B18+E18*$A$3+F18*$B$3+G18*$C$3+H18*$D$3+I18*$E$3+J18*$F$3+K18*$G$3+L18*$H$3+M18*$I$3)</f>
+        <v>115</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="1"/>
-        <v>400</v>
+        <f>MEDIAN(C18,N18,D18)</f>
+        <v>115</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="2"/>
-        <v>0.17101325352714836</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>32</v>
+      <c r="A19" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B19" s="6">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1184,60 +1198,52 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="6">
-        <v>20</v>
-      </c>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="6">
-        <v>10</v>
-      </c>
+      <c r="M19" s="5"/>
       <c r="N19" s="7">
-        <f t="shared" si="0"/>
-        <v>140</v>
+        <f>SUM(B19+E19*$A$3+F19*$B$3+G19*$C$3+H19*$D$3+I19*$E$3+J19*$F$3+K19*$G$3+L19*$H$3+M19*$I$3)</f>
+        <v>55</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" si="1"/>
-        <v>140</v>
+        <f>MEDIAN(C19,N19,D19)</f>
+        <v>55</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" si="2"/>
-        <v>5.9854638734501926E-2</v>
+        <v>2.9891304347826088E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>56</v>
+      <c r="A20" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B20" s="6">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="6">
-        <v>5</v>
-      </c>
-      <c r="I20" s="6">
-        <v>20</v>
-      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="7">
-        <f t="shared" si="0"/>
-        <v>115</v>
+        <f>SUM(B20+E20*$A$3+F20*$B$3+G20*$C$3+H20*$D$3+I20*$E$3+J20*$F$3+K20*$G$3+L20*$H$3+M20*$I$3)</f>
+        <v>100</v>
       </c>
       <c r="O20" s="7">
-        <f t="shared" si="1"/>
-        <v>115</v>
+        <f>MEDIAN(C20,N20,D20)</f>
+        <v>100</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="2"/>
-        <v>4.9166310389055154E-2</v>
+        <v>5.434782608695652E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1245,7 +1251,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="6">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1259,24 +1265,24 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="7">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <f>SUM(B21+E21*$A$3+F21*$B$3+G21*$C$3+H21*$D$3+I21*$E$3+J21*$F$3+K21*$G$3+L21*$H$3+M21*$I$3)</f>
+        <v>80</v>
       </c>
       <c r="O21" s="7">
-        <f t="shared" si="1"/>
-        <v>55</v>
+        <f>MEDIAN(C21,N21,D21)</f>
+        <v>80</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="2"/>
-        <v>2.3514322359982898E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="6">
-        <v>100</v>
+      <c r="A22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="5">
+        <v>300</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1290,25 +1296,21 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
       <c r="N22" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>SUM(B22+E22*$A$3+F22*$B$3+G22*$C$3+H22*$D$3+I22*$E$3+J22*$F$3+K22*$G$3+L22*$H$3+M22*$I$3)</f>
+        <v>300</v>
       </c>
       <c r="O22" s="7">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <f>MEDIAN(C22,N22,D22)</f>
+        <v>300</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="2"/>
-        <v>4.2753313381787089E-2</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="6">
-        <v>80</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1321,25 +1323,21 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="7">
-        <f t="shared" si="0"/>
-        <v>80</v>
+        <f>SUM(B23+E23*$A$3+F23*$B$3+G23*$C$3+H23*$D$3+I23*$E$3+J23*$F$3+K23*$G$3+L23*$H$3+M23*$I$3)</f>
+        <v>0</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>MEDIAN(C23,N23,D23)</f>
+        <v>0</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="2"/>
-        <v>3.4202650705429674E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="5">
-        <v>300</v>
-      </c>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1352,16 +1350,16 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="7">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>SUM(B24+E24*$A$3+F24*$B$3+G24*$C$3+H24*$D$3+I24*$E$3+J24*$F$3+K24*$G$3+L24*$H$3+M24*$I$3)</f>
+        <v>0</v>
       </c>
       <c r="O24" s="7">
-        <f t="shared" si="1"/>
-        <v>300</v>
+        <f>MEDIAN(C24,N24,D24)</f>
+        <v>0</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="2"/>
-        <v>0.12825994014536127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1484,7 +1482,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="7">
         <f>SUM(O7:O28)</f>
-        <v>2339</v>
+        <v>1840</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="2"/>
@@ -1493,7 +1491,7 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1589,12 +1587,12 @@
       </c>
       <c r="P32" s="8">
         <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
-        <v>0.10211896859841715</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -1622,12 +1620,12 @@
       </c>
       <c r="P33" s="8">
         <f t="shared" si="5"/>
-        <v>5.1059484299208577E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6">
         <v>50</v>
@@ -1655,12 +1653,12 @@
       </c>
       <c r="P34" s="8">
         <f t="shared" si="5"/>
-        <v>0.10211896859841715</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="6">
         <v>60</v>
@@ -1686,12 +1684,12 @@
       </c>
       <c r="P35" s="8">
         <f t="shared" si="5"/>
-        <v>3.0635690579525147E-2</v>
+        <v>2.7797081306462822E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="6">
         <v>50</v>
@@ -1721,12 +1719,12 @@
       </c>
       <c r="P36" s="8">
         <f t="shared" si="5"/>
-        <v>4.5953535869287722E-2</v>
+        <v>4.1695621959694229E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" s="6">
         <v>100</v>
@@ -1752,12 +1750,12 @@
       </c>
       <c r="P37" s="8">
         <f t="shared" si="5"/>
-        <v>5.1059484299208577E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6">
         <v>80</v>
@@ -1783,12 +1781,12 @@
       </c>
       <c r="P38" s="8">
         <f t="shared" si="5"/>
-        <v>4.084758743936686E-2</v>
+        <v>3.7062775075283765E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -1822,12 +1820,12 @@
       </c>
       <c r="P39" s="8">
         <f t="shared" si="5"/>
-        <v>7.301506254786827E-2</v>
+        <v>6.6249710447069718E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6">
         <v>40</v>
@@ -1855,12 +1853,12 @@
       </c>
       <c r="P40" s="8">
         <f t="shared" si="5"/>
-        <v>4.6974725555271893E-2</v>
+        <v>4.2622191336576326E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -1890,25 +1888,29 @@
       </c>
       <c r="P41" s="8">
         <f t="shared" si="5"/>
-        <v>6.6377329588971148E-2</v>
+        <v>6.0227009497336115E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>46</v>
+      <c r="A42" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="B42" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="G42" s="5">
+        <v>20</v>
+      </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="6"/>
+      <c r="K42" s="6">
+        <v>15</v>
+      </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="7">
@@ -1921,54 +1923,50 @@
       </c>
       <c r="P42" s="8">
         <f t="shared" si="5"/>
-        <v>5.1059484299208577E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>47</v>
+      <c r="A43" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="6">
         <v>0</v>
       </c>
-      <c r="C43" s="6">
-        <v>10</v>
-      </c>
-      <c r="D43" s="6">
-        <v>125</v>
-      </c>
-      <c r="E43" s="6">
-        <v>1</v>
-      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="G43" s="5">
+        <v>20</v>
+      </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5">
-        <v>1</v>
-      </c>
+      <c r="L43" s="5">
+        <v>15</v>
+      </c>
+      <c r="M43" s="5"/>
       <c r="N43" s="7">
         <f t="shared" si="3"/>
-        <v>50.5</v>
+        <v>100</v>
       </c>
       <c r="O43" s="7">
         <f t="shared" si="4"/>
-        <v>50.5</v>
+        <v>100</v>
       </c>
       <c r="P43" s="8">
         <f t="shared" si="5"/>
-        <v>2.5785039571100333E-2</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B44" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1978,34 +1976,38 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
+      <c r="K44" s="6"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="6">
-        <v>25</v>
-      </c>
+      <c r="M44" s="5"/>
       <c r="N44" s="7">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="O44" s="7">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="P44" s="8">
         <f t="shared" si="5"/>
-        <v>0.10211896859841715</v>
+        <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B45" s="6">
-        <v>50</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="C45" s="6">
+        <v>10</v>
+      </c>
+      <c r="D45" s="6">
+        <v>125</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1</v>
+      </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -2013,28 +2015,28 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
-      <c r="M45" s="6">
-        <v>25</v>
+      <c r="M45" s="5">
+        <v>1</v>
       </c>
       <c r="N45" s="7">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>50.5</v>
       </c>
       <c r="O45" s="7">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>50.5</v>
       </c>
       <c r="P45" s="8">
         <f t="shared" si="5"/>
-        <v>0.10211896859841715</v>
+        <v>2.3395876766272874E-2</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="6">
         <v>50</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2044,30 +2046,30 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="6">
-        <v>12</v>
-      </c>
+      <c r="K46" s="5"/>
       <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
+      <c r="M46" s="6">
+        <v>25</v>
+      </c>
       <c r="N46" s="7">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="O46" s="7">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>200</v>
       </c>
       <c r="P46" s="8">
         <f t="shared" si="5"/>
-        <v>2.4508552463620117E-2</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B47" s="6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2076,30 +2078,32 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="6">
-        <v>15</v>
-      </c>
+      <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
       <c r="M47" s="6">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N47" s="7">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="O47" s="7">
         <f t="shared" si="4"/>
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="P47" s="8">
         <f t="shared" si="5"/>
-        <v>8.4248149093694158E-2</v>
+        <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -2108,25 +2112,31 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
+      <c r="K48" s="6">
+        <v>12</v>
+      </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="7">
         <f t="shared" ref="N48:N50" si="6">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="O48" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="P48" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.2237665045170257E-2</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="6">
+        <v>60</v>
+      </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -2134,21 +2144,25 @@
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
+      <c r="J49" s="6">
+        <v>15</v>
+      </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
+      <c r="M49" s="6">
+        <v>15</v>
+      </c>
       <c r="N49" s="7">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="O49" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="P49" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.6441973592772758E-2</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2190,7 +2204,7 @@
       <c r="N51" s="2"/>
       <c r="O51" s="7">
         <f>SUM(O32:O50)</f>
-        <v>1958.5</v>
+        <v>2158.5</v>
       </c>
       <c r="P51" s="8">
         <f t="shared" si="5"/>
@@ -2199,7 +2213,7 @@
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2294,13 +2308,13 @@
         <v>135</v>
       </c>
       <c r="P54" s="8">
-        <f>O54/SUM(O$54:O$71)</f>
+        <f t="shared" ref="P54:P72" si="9">O54/SUM(O$54:O$71)</f>
         <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55" s="6">
         <v>40</v>
@@ -2329,13 +2343,13 @@
         <v>90</v>
       </c>
       <c r="P55" s="8">
-        <f>O55/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.12244897959183673</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B56" s="6">
         <v>50</v>
@@ -2362,13 +2376,13 @@
         <v>110</v>
       </c>
       <c r="P56" s="8">
-        <f>O56/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.14965986394557823</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B57" s="6">
         <v>40</v>
@@ -2395,13 +2409,13 @@
         <v>80</v>
       </c>
       <c r="P57" s="8">
-        <f>O57/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B58" s="6">
         <v>75</v>
@@ -2430,13 +2444,13 @@
         <v>135</v>
       </c>
       <c r="P58" s="8">
-        <f>O58/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B59" s="6">
         <v>20</v>
@@ -2463,13 +2477,13 @@
         <v>80</v>
       </c>
       <c r="P59" s="8">
-        <f>O59/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="5">
         <v>25</v>
@@ -2498,7 +2512,7 @@
         <v>105</v>
       </c>
       <c r="P60" s="8">
-        <f>O60/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -2525,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="P61" s="8">
-        <f>O61/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2552,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="8">
-        <f>O62/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2579,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="P63" s="8">
-        <f>O63/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2606,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="P64" s="8">
-        <f>O64/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2633,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="P65" s="8">
-        <f>O65/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2660,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="8">
-        <f>O66/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2687,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="P67" s="8">
-        <f>O67/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2714,7 +2728,7 @@
         <v>0</v>
       </c>
       <c r="P68" s="8">
-        <f>O68/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2741,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="P69" s="8">
-        <f>O69/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2768,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="8">
-        <f>O70/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2795,7 +2809,7 @@
         <v>0</v>
       </c>
       <c r="P71" s="8">
-        <f>O71/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2814,7 +2828,7 @@
         <v>735</v>
       </c>
       <c r="P72" s="8">
-        <f>O72/SUM(O$54:O$71)</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -14858,5 +14872,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The Grand Slam Lottery has been relaunched under new management
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekte\SS13\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{317441D2-7D29-4DF5-A3E9-7C3FAD219C22}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BA166FF8-B3CC-49F7-8913-2567B97BB06F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Money Hacker</t>
+  </si>
+  <si>
+    <t>Money Lotto</t>
   </si>
   <si>
     <t>Mundane News</t>
@@ -592,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -809,7 +812,7 @@
       </c>
       <c r="P7" s="8">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>6.575342465753424E-2</v>
+        <v>6.5217391304347824E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -842,7 +845,7 @@
       </c>
       <c r="P8" s="8">
         <f t="shared" si="2"/>
-        <v>4.3835616438356165E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,7 +878,7 @@
       </c>
       <c r="P9" s="8">
         <f t="shared" si="2"/>
-        <v>1.9178082191780823E-2</v>
+        <v>1.9021739130434784E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -908,7 +911,7 @@
       </c>
       <c r="P10" s="8">
         <f t="shared" si="2"/>
-        <v>3.287671232876712E-2</v>
+        <v>3.2608695652173912E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -939,7 +942,7 @@
       </c>
       <c r="P11" s="8">
         <f t="shared" si="2"/>
-        <v>0.16438356164383561</v>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -972,7 +975,7 @@
       </c>
       <c r="P12" s="8">
         <f t="shared" si="2"/>
-        <v>4.3835616438356165E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1003,7 +1006,7 @@
       </c>
       <c r="P13" s="8">
         <f t="shared" si="2"/>
-        <v>5.4794520547945206E-3</v>
+        <v>5.434782608695652E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,11 +1014,17 @@
         <v>27</v>
       </c>
       <c r="B14" s="5">
-        <v>300</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1025,16 +1034,16 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="7">
-        <f t="shared" ref="N14:N21" si="3">SUM(B14+E14*$A$3+F14*$B$3+G14*$C$3+H14*$D$3+I14*$E$3+J14*$F$3+K14*$G$3+L14*$H$3+M14*$I$3)</f>
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>34.5</v>
       </c>
       <c r="O14" s="7">
-        <f t="shared" ref="O14:O21" si="4">MEDIAN(C14,N14,D14)</f>
-        <v>300</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="P14" s="8">
-        <f t="shared" ref="P14:P21" si="5">O14/SUM(O$7:O$28)</f>
-        <v>0.16438356164383561</v>
+        <f t="shared" si="2"/>
+        <v>8.152173913043478E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1042,17 +1051,11 @@
         <v>28</v>
       </c>
       <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>25</v>
-      </c>
-      <c r="D15" s="5">
-        <v>50</v>
-      </c>
-      <c r="E15" s="5">
-        <v>4</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1062,117 +1065,123 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="7">
-        <f t="shared" si="3"/>
-        <v>138</v>
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="O15" s="7">
-        <f t="shared" si="4"/>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
       <c r="P15" s="8">
-        <f t="shared" si="5"/>
-        <v>2.7397260273972601E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.16304347826086957</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="6">
-        <v>60</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5">
+        <v>50</v>
+      </c>
+      <c r="E16" s="5">
+        <v>4</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="6">
-        <v>20</v>
-      </c>
+      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="6">
-        <v>10</v>
-      </c>
+      <c r="M16" s="5"/>
       <c r="N16" s="7">
-        <f t="shared" si="3"/>
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>138</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="4"/>
-        <v>140</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="5"/>
-        <v>7.6712328767123292E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.717391304347826E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="6">
-        <v>5</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6">
         <v>20</v>
       </c>
-      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="M17" s="6">
+        <v>10</v>
+      </c>
       <c r="N17" s="7">
-        <f t="shared" si="3"/>
-        <v>115</v>
+        <f>SUM(B17+E17*$A$3+F17*$B$3+G17*$C$3+H17*$D$3+I17*$E$3+J17*$F$3+K17*$G$3+L17*$H$3+M17*$I$3)</f>
+        <v>140</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" si="4"/>
-        <v>115</v>
+        <f>MEDIAN(C17,N17,D17)</f>
+        <v>140</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" si="5"/>
-        <v>6.3013698630136991E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.6086956521739135E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>30</v>
+      <c r="A18" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B18" s="6">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="6">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6">
+        <v>20</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="7">
-        <f t="shared" si="3"/>
-        <v>55</v>
+        <f>SUM(B18+E18*$A$3+F18*$B$3+G18*$C$3+H18*$D$3+I18*$E$3+J18*$F$3+K18*$G$3+L18*$H$3+M18*$I$3)</f>
+        <v>115</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="4"/>
-        <v>55</v>
+        <f>MEDIAN(C18,N18,D18)</f>
+        <v>115</v>
       </c>
       <c r="P18" s="8">
-        <f t="shared" si="5"/>
-        <v>3.0136986301369864E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1180,7 +1189,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="6">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1194,16 +1203,16 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="7">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f>SUM(B19+E19*$A$3+F19*$B$3+G19*$C$3+H19*$D$3+I19*$E$3+J19*$F$3+K19*$G$3+L19*$H$3+M19*$I$3)</f>
+        <v>55</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" si="4"/>
-        <v>100</v>
+        <f>MEDIAN(C19,N19,D19)</f>
+        <v>55</v>
       </c>
       <c r="P19" s="8">
-        <f t="shared" si="5"/>
-        <v>5.4794520547945202E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.9891304347826088E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1211,7 +1220,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="6">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1225,24 +1234,24 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="7">
-        <f t="shared" si="3"/>
+        <f>SUM(B20+E20*$A$3+F20*$B$3+G20*$C$3+H20*$D$3+I20*$E$3+J20*$F$3+K20*$G$3+L20*$H$3+M20*$I$3)</f>
+        <v>100</v>
+      </c>
+      <c r="O20" s="7">
+        <f>MEDIAN(C20,N20,D20)</f>
+        <v>100</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" si="2"/>
+        <v>5.434782608695652E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="6">
         <v>80</v>
-      </c>
-      <c r="O20" s="7">
-        <f t="shared" si="4"/>
-        <v>80</v>
-      </c>
-      <c r="P20" s="8">
-        <f t="shared" si="5"/>
-        <v>4.3835616438356165E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="5">
-        <v>300</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -1256,21 +1265,25 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="7">
-        <f t="shared" si="3"/>
+        <f>SUM(B21+E21*$A$3+F21*$B$3+G21*$C$3+H21*$D$3+I21*$E$3+J21*$F$3+K21*$G$3+L21*$H$3+M21*$I$3)</f>
+        <v>80</v>
+      </c>
+      <c r="O21" s="7">
+        <f>MEDIAN(C21,N21,D21)</f>
+        <v>80</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" si="2"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="5">
         <v>300</v>
       </c>
-      <c r="O21" s="7">
-        <f t="shared" si="4"/>
-        <v>300</v>
-      </c>
-      <c r="P21" s="8">
-        <f t="shared" si="5"/>
-        <v>0.16438356164383561</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1282,9 +1295,18 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="8"/>
+      <c r="N22" s="7">
+        <f>SUM(B22+E22*$A$3+F22*$B$3+G22*$C$3+H22*$D$3+I22*$E$3+J22*$F$3+K22*$G$3+L22*$H$3+M22*$I$3)</f>
+        <v>300</v>
+      </c>
+      <c r="O22" s="7">
+        <f>MEDIAN(C22,N22,D22)</f>
+        <v>300</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="2"/>
+        <v>0.16304347826086957</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
@@ -1301,11 +1323,11 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="7">
-        <f t="shared" ref="N17:N24" si="6">SUM(B23+E23*$A$3+F23*$B$3+G23*$C$3+H23*$D$3+I23*$E$3+J23*$F$3+K23*$G$3+L23*$H$3+M23*$I$3)</f>
+        <f>SUM(B23+E23*$A$3+F23*$B$3+G23*$C$3+H23*$D$3+I23*$E$3+J23*$F$3+K23*$G$3+L23*$H$3+M23*$I$3)</f>
         <v>0</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" ref="O17:O24" si="7">MEDIAN(C23,N23,D23)</f>
+        <f>MEDIAN(C23,N23,D23)</f>
         <v>0</v>
       </c>
       <c r="P23" s="8">
@@ -1328,11 +1350,11 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="7">
-        <f t="shared" si="6"/>
+        <f>SUM(B24+E24*$A$3+F24*$B$3+G24*$C$3+H24*$D$3+I24*$E$3+J24*$F$3+K24*$G$3+L24*$H$3+M24*$I$3)</f>
         <v>0</v>
       </c>
       <c r="O24" s="7">
-        <f t="shared" si="7"/>
+        <f>MEDIAN(C24,N24,D24)</f>
         <v>0</v>
       </c>
       <c r="P24" s="8">
@@ -1460,7 +1482,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="7">
         <f>SUM(O7:O28)</f>
-        <v>1825</v>
+        <v>1840</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="2"/>
@@ -1469,7 +1491,7 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1556,21 +1578,21 @@
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
       <c r="N32" s="7">
-        <f t="shared" ref="N32:N47" si="8">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
+        <f t="shared" ref="N32:N47" si="3">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>200</v>
       </c>
       <c r="O32" s="7">
-        <f t="shared" ref="O32:O50" si="9">MEDIAN(C32,N32,D32)</f>
+        <f t="shared" ref="O32:O50" si="4">MEDIAN(C32,N32,D32)</f>
         <v>200</v>
       </c>
       <c r="P32" s="8">
-        <f t="shared" ref="P32:P51" si="10">O32/SUM(O$32:O$50)</f>
+        <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
         <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -1589,21 +1611,21 @@
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="O33" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P33" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6">
         <v>50</v>
@@ -1622,21 +1644,21 @@
         <v>25</v>
       </c>
       <c r="N34" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="O34" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="P34" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="6">
         <v>60</v>
@@ -1653,21 +1675,21 @@
       <c r="L35" s="5"/>
       <c r="M35" s="6"/>
       <c r="N35" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="O35" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="P35" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>2.7797081306462822E-2</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" s="6">
         <v>50</v>
@@ -1688,21 +1710,21 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="O36" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="P36" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.1695621959694229E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" s="6">
         <v>100</v>
@@ -1719,21 +1741,21 @@
       <c r="L37" s="6"/>
       <c r="M37" s="5"/>
       <c r="N37" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="O37" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P37" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6">
         <v>80</v>
@@ -1750,21 +1772,21 @@
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="O38" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="P38" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>3.7062775075283765E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -1789,21 +1811,21 @@
       </c>
       <c r="M39" s="5"/>
       <c r="N39" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="O39" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>143</v>
       </c>
       <c r="P39" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>6.6249710447069718E-2</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6">
         <v>40</v>
@@ -1822,21 +1844,21 @@
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="O40" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
       <c r="P40" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.2622191336576326E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -1857,21 +1879,21 @@
         <v>15</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="O41" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="P41" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>6.0227009497336115E-2</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B42" s="6">
         <v>0</v>
@@ -1892,21 +1914,21 @@
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="O42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P42" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B43" s="6">
         <v>0</v>
@@ -1927,21 +1949,21 @@
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="O43" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P43" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="6">
         <v>100</v>
@@ -1958,21 +1980,21 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
       <c r="N44" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="O44" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>4.63284688441047E-2</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="6">
         <v>0</v>
@@ -1997,21 +2019,21 @@
         <v>1</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>50.5</v>
       </c>
       <c r="O45" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>50.5</v>
       </c>
       <c r="P45" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>2.3395876766272874E-2</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="6">
         <v>50</v>
@@ -2030,21 +2052,21 @@
         <v>25</v>
       </c>
       <c r="N46" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="O46" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="P46" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B47" s="6">
         <v>50</v>
@@ -2063,21 +2085,21 @@
         <v>25</v>
       </c>
       <c r="N47" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="O47" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="P47" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>9.2656937688209401E-2</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="5">
         <v>0</v>
@@ -2096,21 +2118,21 @@
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="7">
-        <f t="shared" ref="N48:N50" si="11">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
+        <f t="shared" ref="N48:N50" si="6">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
         <v>48</v>
       </c>
       <c r="O48" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="P48" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>2.2237665045170257E-2</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B49" s="6">
         <v>60</v>
@@ -2131,15 +2153,15 @@
         <v>15</v>
       </c>
       <c r="N49" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>165</v>
       </c>
       <c r="O49" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>165</v>
       </c>
       <c r="P49" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>7.6441973592772758E-2</v>
       </c>
     </row>
@@ -2158,15 +2180,15 @@
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
       <c r="N50" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O50" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P50" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2185,13 +2207,13 @@
         <v>2158.5</v>
       </c>
       <c r="P51" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2278,21 +2300,21 @@
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
       <c r="N54" s="7">
-        <f t="shared" ref="N54:N71" si="12">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <f t="shared" ref="N54:N71" si="7">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
       <c r="O54" s="7">
-        <f t="shared" ref="O54:O71" si="13">MEDIAN(C54,N54,D54)</f>
+        <f t="shared" ref="O54:O71" si="8">MEDIAN(C54,N54,D54)</f>
         <v>135</v>
       </c>
       <c r="P54" s="8">
-        <f t="shared" ref="P54:P72" si="14">O54/SUM(O$54:O$71)</f>
+        <f t="shared" ref="P54:P72" si="9">O54/SUM(O$54:O$71)</f>
         <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B55" s="6">
         <v>40</v>
@@ -2313,21 +2335,21 @@
         <v>5</v>
       </c>
       <c r="N55" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="O55" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
       <c r="P55" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0.12244897959183673</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B56" s="6">
         <v>50</v>
@@ -2346,21 +2368,21 @@
         <v>10</v>
       </c>
       <c r="N56" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>110</v>
       </c>
       <c r="O56" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>110</v>
       </c>
       <c r="P56" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0.14965986394557823</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B57" s="6">
         <v>40</v>
@@ -2379,21 +2401,21 @@
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
       <c r="N57" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="O57" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>80</v>
       </c>
       <c r="P57" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B58" s="6">
         <v>75</v>
@@ -2414,21 +2436,21 @@
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
       <c r="N58" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>135</v>
       </c>
       <c r="O58" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="P58" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0.18367346938775511</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B59" s="6">
         <v>20</v>
@@ -2447,21 +2469,21 @@
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
       <c r="N59" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="O59" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>80</v>
       </c>
       <c r="P59" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0.10884353741496598</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B60" s="5">
         <v>25</v>
@@ -2482,15 +2504,15 @@
         <v>10</v>
       </c>
       <c r="N60" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>105</v>
       </c>
       <c r="O60" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>105</v>
       </c>
       <c r="P60" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -2509,15 +2531,15 @@
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
       <c r="N61" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O61" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P61" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2536,15 +2558,15 @@
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
       <c r="N62" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O62" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P62" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2563,15 +2585,15 @@
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
       <c r="N63" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O63" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P63" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2590,15 +2612,15 @@
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
       <c r="N64" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O64" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P64" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2617,15 +2639,15 @@
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
       <c r="N65" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O65" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P65" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2644,15 +2666,15 @@
       <c r="L66" s="5"/>
       <c r="M66" s="5"/>
       <c r="N66" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O66" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P66" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2671,15 +2693,15 @@
       <c r="L67" s="5"/>
       <c r="M67" s="5"/>
       <c r="N67" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O67" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P67" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2698,15 +2720,15 @@
       <c r="L68" s="5"/>
       <c r="M68" s="5"/>
       <c r="N68" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O68" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P68" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2725,15 +2747,15 @@
       <c r="L69" s="5"/>
       <c r="M69" s="5"/>
       <c r="N69" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O69" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P69" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2752,15 +2774,15 @@
       <c r="L70" s="5"/>
       <c r="M70" s="5"/>
       <c r="N70" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O70" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P70" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2779,15 +2801,15 @@
       <c r="L71" s="5"/>
       <c r="M71" s="5"/>
       <c r="N71" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O71" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P71" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2806,7 +2828,7 @@
         <v>735</v>
       </c>
       <c r="P72" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Makes spontaneous appendicitis rarer (#10336)
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,15 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Byond coding\aurorastation\tools\Event Probabilities\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A05395-473D-4530-8180-791D1AFD0288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -211,7 +227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,12 +301,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -332,7 +351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,9 +384,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,6 +436,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -575,11 +628,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="T68" sqref="T68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1903,15 +1956,15 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="5">
-        <f t="shared" ref="N32:N50" si="3">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
+        <f t="shared" ref="N32:N48" si="3">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>200</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" ref="O32:O50" si="4">MEDIAN(C32,N32,D32)</f>
+        <f t="shared" ref="O32:O48" si="4">MEDIAN(C32,N32,D32)</f>
         <v>200</v>
       </c>
       <c r="P32" s="6">
-        <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
+        <f>O32/SUM(O$32:O$50)</f>
         <v>9.1386794608179112E-2</v>
       </c>
       <c r="Q32" s="2"/>
@@ -1927,10 +1980,10 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1940,22 +1993,22 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4">
         <v>25</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
       <c r="N33" s="5">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="O33" s="5">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="P33" s="6">
-        <f t="shared" si="5"/>
-        <v>4.5693397304089556E-2</v>
+        <f>O33/SUM(O$32:O$50)</f>
+        <v>9.1386794608179112E-2</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
@@ -1970,10 +2023,10 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B34" s="4">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1985,20 +2038,18 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4">
-        <v>25</v>
-      </c>
+      <c r="M34" s="4"/>
       <c r="N34" s="5">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="O34" s="5">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="P34" s="6">
-        <f t="shared" si="5"/>
-        <v>9.1386794608179112E-2</v>
+        <f>O34/SUM(O$32:O$50)</f>
+        <v>2.7416038382453736E-2</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
@@ -2013,33 +2064,37 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35" s="4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4">
+        <v>5</v>
+      </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="J35" s="4">
+        <v>20</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="5">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="O35" s="5">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="P35" s="6">
-        <f t="shared" si="5"/>
-        <v>2.7416038382453736E-2</v>
+        <f>O35/SUM(O$32:O$50)</f>
+        <v>4.1124057573680602E-2</v>
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
@@ -2054,37 +2109,33 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B36" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="4">
-        <v>5</v>
-      </c>
+      <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="4">
-        <v>20</v>
-      </c>
+      <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="5">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="O36" s="5">
         <f t="shared" si="4"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="P36" s="6">
-        <f t="shared" si="5"/>
-        <v>4.1124057573680602E-2</v>
+        <f>O36/SUM(O$32:O$50)</f>
+        <v>4.5693397304089556E-2</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
@@ -2099,10 +2150,10 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2117,15 +2168,15 @@
       <c r="M37" s="4"/>
       <c r="N37" s="5">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="O37" s="5">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="P37" s="6">
-        <f t="shared" si="5"/>
-        <v>4.5693397304089556E-2</v>
+        <f>O37/SUM(O$32:O$50)</f>
+        <v>3.6554717843271647E-2</v>
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
@@ -2140,33 +2191,41 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B38" s="4">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="F38" s="4">
+        <v>45</v>
+      </c>
+      <c r="G38" s="4">
+        <v>25</v>
+      </c>
+      <c r="H38" s="4">
+        <v>6</v>
+      </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
+      <c r="L38" s="4">
+        <v>6</v>
+      </c>
       <c r="M38" s="4"/>
       <c r="N38" s="5">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="O38" s="5">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="P38" s="6">
-        <f t="shared" si="5"/>
-        <v>3.6554717843271647E-2</v>
+        <f>O38/SUM(O$32:O$50)</f>
+        <v>6.5341558144848072E-2</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
@@ -2181,41 +2240,35 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B39" s="4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="4">
-        <v>45</v>
-      </c>
-      <c r="G39" s="4">
-        <v>25</v>
-      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
       <c r="H39" s="4">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="4">
-        <v>6</v>
-      </c>
+      <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="5">
         <f t="shared" si="3"/>
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="O39" s="5">
         <f t="shared" si="4"/>
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="P39" s="6">
-        <f t="shared" si="5"/>
-        <v>6.5341558144848072E-2</v>
+        <f>O39/SUM(O$32:O$50)</f>
+        <v>4.2037925519762397E-2</v>
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
@@ -2230,35 +2283,37 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B40" s="4">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4">
-        <v>13</v>
-      </c>
+      <c r="G40" s="4">
+        <v>20</v>
+      </c>
+      <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4">
+        <v>15</v>
+      </c>
       <c r="N40" s="5">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="O40" s="5">
         <f t="shared" si="4"/>
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="P40" s="6">
-        <f t="shared" si="5"/>
-        <v>4.2037925519762397E-2</v>
+        <f>O40/SUM(O$32:O$50)</f>
+        <v>5.9401416495316425E-2</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
@@ -2273,7 +2328,7 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
@@ -2288,22 +2343,22 @@
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="K41" s="4">
+        <v>15</v>
+      </c>
       <c r="L41" s="4"/>
-      <c r="M41" s="4">
-        <v>15</v>
-      </c>
+      <c r="M41" s="4"/>
       <c r="N41" s="5">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="O41" s="5">
         <f t="shared" si="4"/>
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="P41" s="6">
-        <f t="shared" si="5"/>
-        <v>5.9401416495316425E-2</v>
+        <f>O41/SUM(O$32:O$50)</f>
+        <v>4.5693397304089556E-2</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -2318,7 +2373,7 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4">
         <v>0</v>
@@ -2333,10 +2388,10 @@
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
-      <c r="K42" s="4">
+      <c r="K42" s="4"/>
+      <c r="L42" s="4">
         <v>15</v>
       </c>
-      <c r="L42" s="4"/>
       <c r="M42" s="4"/>
       <c r="N42" s="5">
         <f t="shared" si="3"/>
@@ -2347,7 +2402,7 @@
         <v>100</v>
       </c>
       <c r="P42" s="6">
-        <f t="shared" si="5"/>
+        <f>O42/SUM(O$32:O$50)</f>
         <v>4.5693397304089556E-2</v>
       </c>
       <c r="Q42" s="2"/>
@@ -2363,25 +2418,21 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B43" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4">
-        <v>20</v>
-      </c>
+      <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="4">
-        <v>15</v>
-      </c>
+      <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="5">
         <f t="shared" si="3"/>
@@ -2392,7 +2443,7 @@
         <v>100</v>
       </c>
       <c r="P43" s="6">
-        <f t="shared" si="5"/>
+        <f>O43/SUM(O$32:O$50)</f>
         <v>4.5693397304089556E-2</v>
       </c>
       <c r="Q43" s="2"/>
@@ -2408,14 +2459,20 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B44" s="4">
-        <v>100</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>10</v>
+      </c>
+      <c r="D44" s="4">
+        <v>125</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -2423,18 +2480,20 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
+      <c r="M44" s="4">
+        <v>1</v>
+      </c>
       <c r="N44" s="5">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>50.5</v>
       </c>
       <c r="O44" s="5">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>50.5</v>
       </c>
       <c r="P44" s="6">
-        <f t="shared" si="5"/>
-        <v>4.5693397304089556E-2</v>
+        <f>O44/SUM(O$32:O$50)</f>
+        <v>2.3075165638565227E-2</v>
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
@@ -2449,20 +2508,14 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="4">
         <v>50</v>
       </c>
-      <c r="B45" s="4">
-        <v>0</v>
-      </c>
-      <c r="C45" s="4">
-        <v>10</v>
-      </c>
-      <c r="D45" s="4">
-        <v>125</v>
-      </c>
-      <c r="E45" s="4">
-        <v>1</v>
-      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -2471,19 +2524,19 @@
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="N45" s="5">
         <f t="shared" si="3"/>
-        <v>50.5</v>
+        <v>200</v>
       </c>
       <c r="O45" s="5">
         <f t="shared" si="4"/>
-        <v>50.5</v>
+        <v>200</v>
       </c>
       <c r="P45" s="6">
-        <f t="shared" si="5"/>
-        <v>2.3075165638565227E-2</v>
+        <f>O45/SUM(O$32:O$50)</f>
+        <v>9.1386794608179112E-2</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
@@ -2498,7 +2551,7 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B46" s="4">
         <v>50</v>
@@ -2525,7 +2578,7 @@
         <v>200</v>
       </c>
       <c r="P46" s="6">
-        <f t="shared" si="5"/>
+        <f>O46/SUM(O$32:O$50)</f>
         <v>9.1386794608179112E-2</v>
       </c>
       <c r="Q46" s="2"/>
@@ -2541,10 +2594,10 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B47" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2554,22 +2607,22 @@
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="K47" s="4">
+        <v>12</v>
+      </c>
       <c r="L47" s="4"/>
-      <c r="M47" s="4">
-        <v>25</v>
-      </c>
+      <c r="M47" s="4"/>
       <c r="N47" s="5">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="O47" s="5">
         <f t="shared" si="4"/>
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="P47" s="6">
-        <f t="shared" si="5"/>
-        <v>9.1386794608179112E-2</v>
+        <f>O47/SUM(O$32:O$50)</f>
+        <v>2.193283070596299E-2</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
@@ -2583,11 +2636,11 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" s="4">
-        <v>0</v>
+      <c r="A48" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="7">
+        <v>30</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -2596,23 +2649,27 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4">
-        <v>12</v>
+      <c r="J48" s="4">
+        <v>15</v>
+      </c>
+      <c r="K48" s="7">
+        <v>15</v>
       </c>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4">
+        <v>15</v>
+      </c>
       <c r="N48" s="5">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>195</v>
       </c>
       <c r="O48" s="5">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>195</v>
       </c>
       <c r="P48" s="6">
-        <f t="shared" si="5"/>
-        <v>2.193283070596299E-2</v>
+        <f>O48/SUM(O$32:O$50)</f>
+        <v>8.9102124742974645E-2</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
@@ -2626,11 +2683,11 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="7">
-        <v>30</v>
+      <c r="A49" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -2639,27 +2696,23 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="4">
-        <v>15</v>
-      </c>
-      <c r="K49" s="7">
-        <v>15</v>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4">
+        <v>25</v>
       </c>
       <c r="L49" s="4"/>
-      <c r="M49" s="4">
-        <v>15</v>
-      </c>
+      <c r="M49" s="4"/>
       <c r="N49" s="5">
-        <f t="shared" si="3"/>
-        <v>195</v>
+        <f>IF(C49&gt;0,MAX(B49,C49),B49)+E49*$A$3+F49*$B$3+G49*$C$3+H49*$D$3+I49*$E$3+J49*$F$3+K49*$G$3+L49*$H$3+M49*$I$3</f>
+        <v>100</v>
       </c>
       <c r="O49" s="5">
-        <f t="shared" si="4"/>
-        <v>195</v>
+        <f>MEDIAN(C49,N49,D49)</f>
+        <v>100</v>
       </c>
       <c r="P49" s="6">
-        <f t="shared" si="5"/>
-        <v>8.9102124742974645E-2</v>
+        <f>O49/SUM(O$32:O$50)</f>
+        <v>4.5693397304089556E-2</v>
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
@@ -2687,15 +2740,15 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C50&gt;0,MAX(B50,C50),B50)+E50*$A$3+F50*$B$3+G50*$C$3+H50*$D$3+I50*$E$3+J50*$F$3+K50*$G$3+L50*$H$3+M50*$I$3</f>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f t="shared" si="4"/>
+        <f>MEDIAN(C50,N50,D50)</f>
         <v>0</v>
       </c>
       <c r="P50" s="6">
-        <f t="shared" si="5"/>
+        <f>O50/SUM(O$32:O$50)</f>
         <v>0</v>
       </c>
       <c r="Q50" s="2"/>
@@ -2729,7 +2782,7 @@
         <v>2188.5</v>
       </c>
       <c r="P51" s="6">
-        <f t="shared" si="5"/>
+        <f>O51/SUM(O$32:O$50)</f>
         <v>1</v>
       </c>
       <c r="Q51" s="2"/>
@@ -2852,15 +2905,15 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="5">
-        <f t="shared" ref="N54:N71" si="6">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <f t="shared" ref="N54:N70" si="5">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
       <c r="O54" s="5">
-        <f t="shared" ref="O54:O71" si="7">MEDIAN(C54,N54,D54)</f>
+        <f t="shared" ref="O54:O70" si="6">MEDIAN(C54,N54,D54)</f>
         <v>135</v>
       </c>
       <c r="P54" s="6">
-        <f t="shared" ref="P54:P72" si="8">O54/SUM(O$54:O$71)</f>
+        <f>O54/SUM(O$54:O$70)</f>
         <v>0.15976331360946747</v>
       </c>
       <c r="Q54" s="2"/>
@@ -2897,15 +2950,15 @@
         <v>5</v>
       </c>
       <c r="N55" s="5">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="O55" s="5">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
-      <c r="O55" s="5">
-        <f t="shared" si="7"/>
-        <v>90</v>
-      </c>
       <c r="P55" s="6">
-        <f t="shared" si="8"/>
+        <f>O55/SUM(O$54:O$70)</f>
         <v>0.10650887573964497</v>
       </c>
       <c r="Q55" s="2"/>
@@ -2940,15 +2993,15 @@
         <v>10</v>
       </c>
       <c r="N56" s="5">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+      <c r="O56" s="5">
         <f t="shared" si="6"/>
         <v>110</v>
       </c>
-      <c r="O56" s="5">
-        <f t="shared" si="7"/>
-        <v>110</v>
-      </c>
       <c r="P56" s="6">
-        <f t="shared" si="8"/>
+        <f>O56/SUM(O$54:O$70)</f>
         <v>0.13017751479289941</v>
       </c>
       <c r="Q56" s="2"/>
@@ -2983,15 +3036,15 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="5">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="O57" s="5">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
-      <c r="O57" s="5">
-        <f t="shared" si="7"/>
-        <v>80</v>
-      </c>
       <c r="P57" s="6">
-        <f t="shared" si="8"/>
+        <f>O57/SUM(O$54:O$70)</f>
         <v>9.4674556213017749E-2</v>
       </c>
       <c r="Q57" s="2"/>
@@ -3028,15 +3081,15 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="5">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="O58" s="5">
         <f t="shared" si="6"/>
         <v>135</v>
       </c>
-      <c r="O58" s="5">
-        <f t="shared" si="7"/>
-        <v>135</v>
-      </c>
       <c r="P58" s="6">
-        <f t="shared" si="8"/>
+        <f>O58/SUM(O$54:O$70)</f>
         <v>0.15976331360946747</v>
       </c>
       <c r="Q58" s="2"/>
@@ -3073,15 +3126,15 @@
         <v>10</v>
       </c>
       <c r="N59" s="5">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+      <c r="O59" s="5">
         <f t="shared" si="6"/>
         <v>105</v>
       </c>
-      <c r="O59" s="5">
-        <f t="shared" si="7"/>
-        <v>105</v>
-      </c>
       <c r="P59" s="6">
-        <f t="shared" si="8"/>
+        <f>O59/SUM(O$54:O$70)</f>
         <v>0.1242603550295858</v>
       </c>
       <c r="Q59" s="2"/>
@@ -3118,15 +3171,15 @@
         <v>15</v>
       </c>
       <c r="N60" s="5">
+        <f t="shared" si="5"/>
+        <v>145</v>
+      </c>
+      <c r="O60" s="5">
         <f t="shared" si="6"/>
         <v>145</v>
       </c>
-      <c r="O60" s="5">
-        <f t="shared" si="7"/>
-        <v>145</v>
-      </c>
       <c r="P60" s="6">
-        <f t="shared" si="8"/>
+        <f>O60/SUM(O$54:O$70)</f>
         <v>0.17159763313609466</v>
       </c>
       <c r="Q60" s="2"/>
@@ -3161,15 +3214,15 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="5">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="O61" s="5">
         <f t="shared" si="6"/>
         <v>45</v>
       </c>
-      <c r="O61" s="5">
-        <f t="shared" si="7"/>
-        <v>45</v>
-      </c>
       <c r="P61" s="6">
-        <f t="shared" si="8"/>
+        <f>O61/SUM(O$54:O$70)</f>
         <v>5.3254437869822487E-2</v>
       </c>
       <c r="Q61" s="2"/>
@@ -3198,15 +3251,15 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O62" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O62" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P62" s="6">
-        <f t="shared" si="8"/>
+        <f>O62/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q62" s="2"/>
@@ -3235,15 +3288,15 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O63" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O63" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P63" s="6">
-        <f t="shared" si="8"/>
+        <f>O63/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q63" s="2"/>
@@ -3272,15 +3325,15 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O64" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O64" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P64" s="6">
-        <f t="shared" si="8"/>
+        <f>O64/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q64" s="2"/>
@@ -3309,15 +3362,15 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O65" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O65" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P65" s="6">
-        <f t="shared" si="8"/>
+        <f>O65/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q65" s="2"/>
@@ -3346,15 +3399,15 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O66" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O66" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P66" s="6">
-        <f t="shared" si="8"/>
+        <f>O66/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q66" s="2"/>
@@ -3383,15 +3436,15 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O67" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O67" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P67" s="6">
-        <f t="shared" si="8"/>
+        <f>O67/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q67" s="2"/>
@@ -3420,15 +3473,15 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O68" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O68" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P68" s="6">
-        <f t="shared" si="8"/>
+        <f>O68/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q68" s="2"/>
@@ -3457,15 +3510,15 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O69" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O69" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P69" s="6">
-        <f t="shared" si="8"/>
+        <f>O69/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q69" s="2"/>
@@ -3494,15 +3547,15 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O70" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O70" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
       <c r="P70" s="6">
-        <f t="shared" si="8"/>
+        <f>O70/SUM(O$54:O$70)</f>
         <v>0</v>
       </c>
       <c r="Q70" s="2"/>
@@ -3517,30 +3570,27 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
       <c r="O71" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>SUM(O53:O70)</f>
+        <v>845</v>
       </c>
       <c r="P71" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>O71/SUM(O$54:O$70)</f>
+        <v>1</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
@@ -3568,14 +3618,8 @@
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
-      <c r="O72" s="5">
-        <f>SUM(O53:O71)</f>
-        <v>845</v>
-      </c>
-      <c r="P72" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
       <c r="R72" s="2"/>
       <c r="S72" s="2"/>
@@ -29515,62 +29559,6 @@
       <c r="Y998" s="2"/>
       <c r="Z998" s="2"/>
     </row>
-    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
-      <c r="K999" s="2"/>
-      <c r="L999" s="2"/>
-      <c r="M999" s="2"/>
-      <c r="N999" s="2"/>
-      <c r="O999" s="2"/>
-      <c r="P999" s="2"/>
-      <c r="Q999" s="2"/>
-      <c r="R999" s="2"/>
-      <c r="S999" s="2"/>
-      <c r="T999" s="2"/>
-      <c r="U999" s="2"/>
-      <c r="V999" s="2"/>
-      <c r="W999" s="2"/>
-      <c r="X999" s="2"/>
-      <c r="Y999" s="2"/>
-      <c r="Z999" s="2"/>
-    </row>
-    <row r="1000" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="2"/>
-      <c r="G1000" s="2"/>
-      <c r="H1000" s="2"/>
-      <c r="I1000" s="2"/>
-      <c r="J1000" s="2"/>
-      <c r="K1000" s="2"/>
-      <c r="L1000" s="2"/>
-      <c r="M1000" s="2"/>
-      <c r="N1000" s="2"/>
-      <c r="O1000" s="2"/>
-      <c r="P1000" s="2"/>
-      <c r="Q1000" s="2"/>
-      <c r="R1000" s="2"/>
-      <c r="S1000" s="2"/>
-      <c r="T1000" s="2"/>
-      <c r="U1000" s="2"/>
-      <c r="V1000" s="2"/>
-      <c r="W1000" s="2"/>
-      <c r="X1000" s="2"/>
-      <c r="Y1000" s="2"/>
-      <c r="Z1000" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Drone Uprising Event (#10766)
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Byond coding\aurorastation\tools\Event Probabilities\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A05395-473D-4530-8180-791D1AFD0288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -223,11 +217,20 @@
   <si>
     <t>Downed Ship</t>
   </si>
+  <si>
+    <t>Drone Malfunction</t>
+  </si>
+  <si>
+    <t>Drone Uprising</t>
+  </si>
+  <si>
+    <t>Drone Revolution</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +312,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -351,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,26 +387,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,23 +422,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -628,11 +597,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="T68" sqref="T68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -925,7 +894,7 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>6.1538461538461542E-2</v>
+        <v>5.7692307692307696E-2</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -968,7 +937,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>4.1025641025641026E-2</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1011,7 +980,7 @@
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>1.7948717948717947E-2</v>
+        <v>1.6826923076923076E-2</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1054,7 +1023,7 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>3.0769230769230771E-2</v>
+        <v>2.8846153846153848E-2</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1095,7 +1064,7 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.14423076923076922</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1138,7 +1107,7 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>4.1025641025641026E-2</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1179,7 +1148,7 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" si="2"/>
-        <v>5.1282051282051282E-3</v>
+        <v>4.807692307692308E-3</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1226,7 +1195,7 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" si="2"/>
-        <v>7.6923076923076927E-3</v>
+        <v>7.2115384615384619E-3</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1267,7 +1236,7 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.14423076923076922</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1314,7 +1283,7 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="2"/>
-        <v>2.564102564102564E-2</v>
+        <v>2.403846153846154E-2</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1359,7 +1328,7 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" si="2"/>
-        <v>7.179487179487179E-2</v>
+        <v>6.7307692307692304E-2</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -1404,7 +1373,7 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" si="2"/>
-        <v>5.8974358974358973E-2</v>
+        <v>5.5288461538461536E-2</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1445,7 +1414,7 @@
       </c>
       <c r="P19" s="6">
         <f t="shared" si="2"/>
-        <v>2.8205128205128206E-2</v>
+        <v>2.6442307692307692E-2</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1486,7 +1455,7 @@
       </c>
       <c r="P20" s="6">
         <f t="shared" si="2"/>
-        <v>5.128205128205128E-2</v>
+        <v>4.807692307692308E-2</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1527,7 +1496,7 @@
       </c>
       <c r="P21" s="6">
         <f t="shared" si="2"/>
-        <v>4.1025641025641026E-2</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1568,7 +1537,7 @@
       </c>
       <c r="P22" s="6">
         <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <v>0.14423076923076922</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -1611,7 +1580,7 @@
       </c>
       <c r="P23" s="6">
         <f t="shared" si="2"/>
-        <v>4.6153846153846156E-2</v>
+        <v>4.3269230769230768E-2</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1652,7 +1621,7 @@
       </c>
       <c r="P24" s="6">
         <f t="shared" si="2"/>
-        <v>1.0256410256410256E-2</v>
+        <v>9.6153846153846159E-3</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -1666,14 +1635,20 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="4">
+        <v>10</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4">
+        <v>30</v>
+      </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1681,15 +1656,15 @@
       <c r="M25" s="4"/>
       <c r="N25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="O25" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="P25" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -1830,7 +1805,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="5">
         <f>SUM(O7:O28)</f>
-        <v>1950</v>
+        <v>2080</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="2"/>
@@ -1964,8 +1939,8 @@
         <v>200</v>
       </c>
       <c r="P32" s="6">
-        <f>O32/SUM(O$32:O$50)</f>
-        <v>9.1386794608179112E-2</v>
+        <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
+        <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -2007,8 +1982,8 @@
         <v>200</v>
       </c>
       <c r="P33" s="6">
-        <f>O33/SUM(O$32:O$50)</f>
-        <v>9.1386794608179112E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
@@ -2048,8 +2023,8 @@
         <v>60</v>
       </c>
       <c r="P34" s="6">
-        <f>O34/SUM(O$32:O$50)</f>
-        <v>2.7416038382453736E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.5712449110777802E-2</v>
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
@@ -2093,8 +2068,8 @@
         <v>90</v>
       </c>
       <c r="P35" s="6">
-        <f>O35/SUM(O$32:O$50)</f>
-        <v>4.1124057573680602E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.8568673666166703E-2</v>
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
@@ -2134,8 +2109,8 @@
         <v>100</v>
       </c>
       <c r="P36" s="6">
-        <f>O36/SUM(O$32:O$50)</f>
-        <v>4.5693397304089556E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
@@ -2175,8 +2150,8 @@
         <v>80</v>
       </c>
       <c r="P37" s="6">
-        <f>O37/SUM(O$32:O$50)</f>
-        <v>3.6554717843271647E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.4283265481037072E-2</v>
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
@@ -2224,8 +2199,8 @@
         <v>143</v>
       </c>
       <c r="P38" s="6">
-        <f>O38/SUM(O$32:O$50)</f>
-        <v>6.5341558144848072E-2</v>
+        <f t="shared" si="5"/>
+        <v>6.1281337047353758E-2</v>
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
@@ -2267,8 +2242,8 @@
         <v>92</v>
       </c>
       <c r="P39" s="6">
-        <f>O39/SUM(O$32:O$50)</f>
-        <v>4.2037925519762397E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.9425755303192631E-2</v>
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
@@ -2312,8 +2287,8 @@
         <v>130</v>
       </c>
       <c r="P40" s="6">
-        <f>O40/SUM(O$32:O$50)</f>
-        <v>5.9401416495316425E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.5710306406685235E-2</v>
       </c>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
@@ -2357,8 +2332,8 @@
         <v>100</v>
       </c>
       <c r="P41" s="6">
-        <f>O41/SUM(O$32:O$50)</f>
-        <v>4.5693397304089556E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -2402,8 +2377,8 @@
         <v>100</v>
       </c>
       <c r="P42" s="6">
-        <f>O42/SUM(O$32:O$50)</f>
-        <v>4.5693397304089556E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -2443,8 +2418,8 @@
         <v>100</v>
       </c>
       <c r="P43" s="6">
-        <f>O43/SUM(O$32:O$50)</f>
-        <v>4.5693397304089556E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
@@ -2492,8 +2467,8 @@
         <v>50.5</v>
       </c>
       <c r="P44" s="6">
-        <f>O44/SUM(O$32:O$50)</f>
-        <v>2.3075165638565227E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.1641311334904649E-2</v>
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
@@ -2535,8 +2510,8 @@
         <v>200</v>
       </c>
       <c r="P45" s="6">
-        <f>O45/SUM(O$32:O$50)</f>
-        <v>9.1386794608179112E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
@@ -2578,8 +2553,8 @@
         <v>200</v>
       </c>
       <c r="P46" s="6">
-        <f>O46/SUM(O$32:O$50)</f>
-        <v>9.1386794608179112E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
@@ -2621,8 +2596,8 @@
         <v>48</v>
       </c>
       <c r="P47" s="6">
-        <f>O47/SUM(O$32:O$50)</f>
-        <v>2.193283070596299E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.0569959288622243E-2</v>
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
@@ -2668,8 +2643,8 @@
         <v>195</v>
       </c>
       <c r="P48" s="6">
-        <f>O48/SUM(O$32:O$50)</f>
-        <v>8.9102124742974645E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.3565459610027856E-2</v>
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
@@ -2711,8 +2686,8 @@
         <v>100</v>
       </c>
       <c r="P49" s="6">
-        <f>O49/SUM(O$32:O$50)</f>
-        <v>4.5693397304089556E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
@@ -2726,14 +2701,20 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="4">
+        <v>25</v>
+      </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
+      <c r="H50" s="4">
+        <v>30</v>
+      </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -2741,15 +2722,15 @@
       <c r="M50" s="4"/>
       <c r="N50" s="5">
         <f>IF(C50&gt;0,MAX(B50,C50),B50)+E50*$A$3+F50*$B$3+G50*$C$3+H50*$D$3+I50*$E$3+J50*$F$3+K50*$G$3+L50*$H$3+M50*$I$3</f>
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="O50" s="5">
         <f>MEDIAN(C50,N50,D50)</f>
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="P50" s="6">
-        <f>O50/SUM(O$32:O$50)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>6.2138418684379686E-2</v>
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
@@ -2779,10 +2760,10 @@
       <c r="N51" s="2"/>
       <c r="O51" s="5">
         <f>SUM(O32:O50)</f>
-        <v>2188.5</v>
+        <v>2333.5</v>
       </c>
       <c r="P51" s="6">
-        <f>O51/SUM(O$32:O$50)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q51" s="2"/>
@@ -2905,16 +2886,16 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="5">
-        <f t="shared" ref="N54:N70" si="5">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <f t="shared" ref="N54:N70" si="6">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
       <c r="O54" s="5">
-        <f t="shared" ref="O54:O70" si="6">MEDIAN(C54,N54,D54)</f>
+        <f t="shared" ref="O54:O70" si="7">MEDIAN(C54,N54,D54)</f>
         <v>135</v>
       </c>
       <c r="P54" s="6">
-        <f>O54/SUM(O$54:O$70)</f>
-        <v>0.15976331360946747</v>
+        <f t="shared" ref="P54:P71" si="8">O54/SUM(O$54:O$70)</f>
+        <v>0.14438502673796791</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
@@ -2950,16 +2931,16 @@
         <v>5</v>
       </c>
       <c r="N55" s="5">
-        <f t="shared" si="5"/>
-        <v>90</v>
-      </c>
-      <c r="O55" s="5">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
+      <c r="O55" s="5">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
       <c r="P55" s="6">
-        <f>O55/SUM(O$54:O$70)</f>
-        <v>0.10650887573964497</v>
+        <f t="shared" si="8"/>
+        <v>9.6256684491978606E-2</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
@@ -2993,16 +2974,16 @@
         <v>10</v>
       </c>
       <c r="N56" s="5">
-        <f t="shared" si="5"/>
-        <v>110</v>
-      </c>
-      <c r="O56" s="5">
         <f t="shared" si="6"/>
         <v>110</v>
       </c>
+      <c r="O56" s="5">
+        <f t="shared" si="7"/>
+        <v>110</v>
+      </c>
       <c r="P56" s="6">
-        <f>O56/SUM(O$54:O$70)</f>
-        <v>0.13017751479289941</v>
+        <f t="shared" si="8"/>
+        <v>0.11764705882352941</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
@@ -3036,16 +3017,16 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="5">
-        <f t="shared" si="5"/>
-        <v>80</v>
-      </c>
-      <c r="O57" s="5">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
+      <c r="O57" s="5">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
       <c r="P57" s="6">
-        <f>O57/SUM(O$54:O$70)</f>
-        <v>9.4674556213017749E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.5561497326203204E-2</v>
       </c>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
@@ -3081,16 +3062,16 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="5">
-        <f t="shared" si="5"/>
-        <v>135</v>
-      </c>
-      <c r="O58" s="5">
         <f t="shared" si="6"/>
         <v>135</v>
       </c>
+      <c r="O58" s="5">
+        <f t="shared" si="7"/>
+        <v>135</v>
+      </c>
       <c r="P58" s="6">
-        <f>O58/SUM(O$54:O$70)</f>
-        <v>0.15976331360946747</v>
+        <f t="shared" si="8"/>
+        <v>0.14438502673796791</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -3126,16 +3107,16 @@
         <v>10</v>
       </c>
       <c r="N59" s="5">
-        <f t="shared" si="5"/>
-        <v>105</v>
-      </c>
-      <c r="O59" s="5">
         <f t="shared" si="6"/>
         <v>105</v>
       </c>
+      <c r="O59" s="5">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
       <c r="P59" s="6">
-        <f>O59/SUM(O$54:O$70)</f>
-        <v>0.1242603550295858</v>
+        <f t="shared" si="8"/>
+        <v>0.11229946524064172</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
@@ -3171,16 +3152,16 @@
         <v>15</v>
       </c>
       <c r="N60" s="5">
-        <f t="shared" si="5"/>
-        <v>145</v>
-      </c>
-      <c r="O60" s="5">
         <f t="shared" si="6"/>
         <v>145</v>
       </c>
+      <c r="O60" s="5">
+        <f t="shared" si="7"/>
+        <v>145</v>
+      </c>
       <c r="P60" s="6">
-        <f>O60/SUM(O$54:O$70)</f>
-        <v>0.17159763313609466</v>
+        <f t="shared" si="8"/>
+        <v>0.15508021390374332</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
@@ -3214,16 +3195,16 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="5">
-        <f t="shared" si="5"/>
-        <v>45</v>
-      </c>
-      <c r="O61" s="5">
         <f t="shared" si="6"/>
         <v>45</v>
       </c>
+      <c r="O61" s="5">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
       <c r="P61" s="6">
-        <f>O61/SUM(O$54:O$70)</f>
-        <v>5.3254437869822487E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.8128342245989303E-2</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
@@ -3237,30 +3218,40 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="4">
+        <v>0</v>
+      </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
+      <c r="H62" s="4">
+        <v>10</v>
+      </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
+      <c r="K62" s="4">
+        <v>5</v>
+      </c>
       <c r="L62" s="4"/>
-      <c r="M62" s="4"/>
+      <c r="M62" s="4">
+        <v>5</v>
+      </c>
       <c r="N62" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>90</v>
       </c>
       <c r="O62" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>90</v>
       </c>
       <c r="P62" s="6">
-        <f>O62/SUM(O$54:O$70)</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>9.6256684491978606E-2</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
@@ -3288,15 +3279,15 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O63" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O63" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P63" s="6">
-        <f>O63/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q63" s="2"/>
@@ -3325,15 +3316,15 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O64" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O64" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P64" s="6">
-        <f>O64/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q64" s="2"/>
@@ -3362,15 +3353,15 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O65" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O65" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P65" s="6">
-        <f>O65/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q65" s="2"/>
@@ -3399,15 +3390,15 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O66" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O66" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P66" s="6">
-        <f>O66/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q66" s="2"/>
@@ -3436,15 +3427,15 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O67" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O67" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P67" s="6">
-        <f>O67/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q67" s="2"/>
@@ -3473,15 +3464,15 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O68" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O68" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P68" s="6">
-        <f>O68/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q68" s="2"/>
@@ -3510,15 +3501,15 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O69" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O69" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P69" s="6">
-        <f>O69/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q69" s="2"/>
@@ -3547,15 +3538,15 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O70" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="O70" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="P70" s="6">
-        <f>O70/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q70" s="2"/>
@@ -3586,10 +3577,10 @@
       <c r="N71" s="2"/>
       <c r="O71" s="5">
         <f>SUM(O53:O70)</f>
-        <v>845</v>
+        <v>935</v>
       </c>
       <c r="P71" s="6">
-        <f>O71/SUM(O$54:O$70)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q71" s="2"/>

</xml_diff>

<commit_message>
Non-Hostile Migrations and Angry Goats
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Drone Revolution</t>
+  </si>
+  <si>
+    <t>Cozmozoan Migration</t>
   </si>
 </sst>
 </file>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,7 +897,7 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>5.7692307692307696E-2</v>
+        <v>5.6074766355140186E-2</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -937,7 +940,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7383177570093455E-2</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -980,7 +983,7 @@
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>1.6826923076923076E-2</v>
+        <v>1.6355140186915886E-2</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1023,7 +1026,7 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>2.8846153846153848E-2</v>
+        <v>2.8037383177570093E-2</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0.14423076923076922</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1107,7 +1110,7 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7383177570093455E-2</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1148,7 +1151,7 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" si="2"/>
-        <v>4.807692307692308E-3</v>
+        <v>4.6728971962616819E-3</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1195,7 +1198,7 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" si="2"/>
-        <v>7.2115384615384619E-3</v>
+        <v>7.0093457943925233E-3</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1236,7 +1239,7 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" si="2"/>
-        <v>0.14423076923076922</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="2"/>
-        <v>2.403846153846154E-2</v>
+        <v>2.336448598130841E-2</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1328,7 +1331,7 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" si="2"/>
-        <v>6.7307692307692304E-2</v>
+        <v>6.5420560747663545E-2</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -1373,7 +1376,7 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" si="2"/>
-        <v>5.5288461538461536E-2</v>
+        <v>5.3738317757009345E-2</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1414,7 +1417,7 @@
       </c>
       <c r="P19" s="6">
         <f t="shared" si="2"/>
-        <v>2.6442307692307692E-2</v>
+        <v>2.5700934579439252E-2</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1455,7 +1458,7 @@
       </c>
       <c r="P20" s="6">
         <f t="shared" si="2"/>
-        <v>4.807692307692308E-2</v>
+        <v>4.6728971962616821E-2</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1496,7 +1499,7 @@
       </c>
       <c r="P21" s="6">
         <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7383177570093455E-2</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1537,7 +1540,7 @@
       </c>
       <c r="P22" s="6">
         <f t="shared" si="2"/>
-        <v>0.14423076923076922</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -1580,7 +1583,7 @@
       </c>
       <c r="P23" s="6">
         <f t="shared" si="2"/>
-        <v>4.3269230769230768E-2</v>
+        <v>4.2056074766355138E-2</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1621,7 +1624,7 @@
       </c>
       <c r="P24" s="6">
         <f t="shared" si="2"/>
-        <v>9.6153846153846159E-3</v>
+        <v>9.3457943925233638E-3</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -1664,7 +1667,7 @@
       </c>
       <c r="P25" s="6">
         <f t="shared" si="2"/>
-        <v>6.25E-2</v>
+        <v>6.0747663551401869E-2</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -1678,8 +1681,12 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="4">
+        <v>60</v>
+      </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1693,15 +1700,15 @@
       <c r="M26" s="4"/>
       <c r="N26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O26" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.8037383177570093E-2</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -1805,7 +1812,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="5">
         <f>SUM(O7:O28)</f>
-        <v>2080</v>
+        <v>2140</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Non-Hostile Migrations and Angry Goats (#12016)
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>Drone Revolution</t>
+  </si>
+  <si>
+    <t>Cozmozoan Migration</t>
   </si>
 </sst>
 </file>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,7 +897,7 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>5.7692307692307696E-2</v>
+        <v>5.6074766355140186E-2</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -937,7 +940,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7383177570093455E-2</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -980,7 +983,7 @@
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>1.6826923076923076E-2</v>
+        <v>1.6355140186915886E-2</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1023,7 +1026,7 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>2.8846153846153848E-2</v>
+        <v>2.8037383177570093E-2</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0.14423076923076922</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1107,7 +1110,7 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7383177570093455E-2</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1148,7 +1151,7 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" si="2"/>
-        <v>4.807692307692308E-3</v>
+        <v>4.6728971962616819E-3</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1195,7 +1198,7 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" si="2"/>
-        <v>7.2115384615384619E-3</v>
+        <v>7.0093457943925233E-3</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1236,7 +1239,7 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" si="2"/>
-        <v>0.14423076923076922</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="2"/>
-        <v>2.403846153846154E-2</v>
+        <v>2.336448598130841E-2</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1328,7 +1331,7 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" si="2"/>
-        <v>6.7307692307692304E-2</v>
+        <v>6.5420560747663545E-2</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -1373,7 +1376,7 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" si="2"/>
-        <v>5.5288461538461536E-2</v>
+        <v>5.3738317757009345E-2</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1414,7 +1417,7 @@
       </c>
       <c r="P19" s="6">
         <f t="shared" si="2"/>
-        <v>2.6442307692307692E-2</v>
+        <v>2.5700934579439252E-2</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1455,7 +1458,7 @@
       </c>
       <c r="P20" s="6">
         <f t="shared" si="2"/>
-        <v>4.807692307692308E-2</v>
+        <v>4.6728971962616821E-2</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1496,7 +1499,7 @@
       </c>
       <c r="P21" s="6">
         <f t="shared" si="2"/>
-        <v>3.8461538461538464E-2</v>
+        <v>3.7383177570093455E-2</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1537,7 +1540,7 @@
       </c>
       <c r="P22" s="6">
         <f t="shared" si="2"/>
-        <v>0.14423076923076922</v>
+        <v>0.14018691588785046</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -1580,7 +1583,7 @@
       </c>
       <c r="P23" s="6">
         <f t="shared" si="2"/>
-        <v>4.3269230769230768E-2</v>
+        <v>4.2056074766355138E-2</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1621,7 +1624,7 @@
       </c>
       <c r="P24" s="6">
         <f t="shared" si="2"/>
-        <v>9.6153846153846159E-3</v>
+        <v>9.3457943925233638E-3</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -1664,7 +1667,7 @@
       </c>
       <c r="P25" s="6">
         <f t="shared" si="2"/>
-        <v>6.25E-2</v>
+        <v>6.0747663551401869E-2</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -1678,8 +1681,12 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="4">
+        <v>60</v>
+      </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1693,15 +1700,15 @@
       <c r="M26" s="4"/>
       <c r="N26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O26" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.8037383177570093E-2</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -1805,7 +1812,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="5">
         <f>SUM(O7:O28)</f>
-        <v>2080</v>
+        <v>2140</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Removes Random Golems (#12287)
habemus revert
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spark\Desktop\Fixed\Aurora.3\tools\Event Probabilities\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79AD941-A3E5-42FC-A82F-925B71B11376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -17,6 +23,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -212,9 +219,6 @@
     <t>Severe Infestation</t>
   </si>
   <si>
-    <t>Golem Rune</t>
-  </si>
-  <si>
     <t>Downed Ship</t>
   </si>
   <si>
@@ -233,7 +237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,9 +394,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,6 +446,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -600,11 +638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -897,7 +935,7 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" ref="P7:P29" si="2">O7/SUM(O$7:O$28)</f>
-        <v>5.6074766355140186E-2</v>
+        <v>5.6603773584905662E-2</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -940,7 +978,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>3.7383177570093455E-2</v>
+        <v>3.7735849056603772E-2</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -983,7 +1021,7 @@
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>1.6355140186915886E-2</v>
+        <v>1.6509433962264151E-2</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1026,7 +1064,7 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>2.8037383177570093E-2</v>
+        <v>2.8301886792452831E-2</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1067,7 +1105,7 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0.14018691588785046</v>
+        <v>0.14150943396226415</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1110,7 +1148,7 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>3.7383177570093455E-2</v>
+        <v>3.7735849056603772E-2</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1151,7 +1189,7 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" si="2"/>
-        <v>4.6728971962616819E-3</v>
+        <v>4.7169811320754715E-3</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1198,7 +1236,7 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" si="2"/>
-        <v>7.0093457943925233E-3</v>
+        <v>7.0754716981132077E-3</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1239,7 +1277,7 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" si="2"/>
-        <v>0.14018691588785046</v>
+        <v>0.14150943396226415</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1286,7 +1324,7 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" si="2"/>
-        <v>2.336448598130841E-2</v>
+        <v>2.358490566037736E-2</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1331,7 +1369,7 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" si="2"/>
-        <v>6.5420560747663545E-2</v>
+        <v>6.6037735849056603E-2</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -1376,7 +1414,7 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" si="2"/>
-        <v>5.3738317757009345E-2</v>
+        <v>5.4245283018867926E-2</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1417,7 +1455,7 @@
       </c>
       <c r="P19" s="6">
         <f t="shared" si="2"/>
-        <v>2.5700934579439252E-2</v>
+        <v>2.5943396226415096E-2</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1458,7 +1496,7 @@
       </c>
       <c r="P20" s="6">
         <f t="shared" si="2"/>
-        <v>4.6728971962616821E-2</v>
+        <v>4.716981132075472E-2</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1499,7 +1537,7 @@
       </c>
       <c r="P21" s="6">
         <f t="shared" si="2"/>
-        <v>3.7383177570093455E-2</v>
+        <v>3.7735849056603772E-2</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1540,7 +1578,7 @@
       </c>
       <c r="P22" s="6">
         <f t="shared" si="2"/>
-        <v>0.14018691588785046</v>
+        <v>0.14150943396226415</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -1583,7 +1621,7 @@
       </c>
       <c r="P23" s="6">
         <f t="shared" si="2"/>
-        <v>4.2056074766355138E-2</v>
+        <v>4.2452830188679243E-2</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1598,33 +1636,35 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4">
+        <v>30</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="5">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(B24+E24*$A$3+F24*$B$3+G24*$C$3+H24*$D$3+I24*$E$3+J24*$F$3+K24*$G$3+L24*$H$3+M24*$I$3)</f>
+        <v>130</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>MEDIAN(C24,N24,D24)</f>
+        <v>130</v>
       </c>
       <c r="P24" s="6">
-        <f t="shared" si="2"/>
-        <v>9.3457943925233638E-3</v>
+        <f>O24/SUM(O$7:O$28)</f>
+        <v>6.1320754716981132E-2</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -1639,35 +1679,33 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B25" s="4">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4">
-        <v>30</v>
-      </c>
+      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="5">
-        <f t="shared" si="0"/>
-        <v>130</v>
+        <f>SUM(B25+E25*$A$3+F25*$B$3+G25*$C$3+H25*$D$3+I25*$E$3+J25*$F$3+K25*$G$3+L25*$H$3+M25*$I$3)</f>
+        <v>60</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="1"/>
-        <v>130</v>
+        <f>MEDIAN(C25,N25,D25)</f>
+        <v>60</v>
       </c>
       <c r="P25" s="6">
-        <f t="shared" si="2"/>
-        <v>6.0747663551401869E-2</v>
+        <f>O25/SUM(O$7:O$28)</f>
+        <v>2.8301886792452831E-2</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -1681,12 +1719,8 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="4">
-        <v>60</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1699,16 +1733,16 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="5">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <f t="shared" ref="N26" si="3">SUM(B26+E26*$A$3+F26*$B$3+G26*$C$3+H26*$D$3+I26*$E$3+J26*$F$3+K26*$G$3+L26*$H$3+M26*$I$3)</f>
+        <v>0</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" ref="O26" si="4">MEDIAN(C26,N26,D26)</f>
+        <v>0</v>
       </c>
       <c r="P26" s="6">
-        <f t="shared" si="2"/>
-        <v>2.8037383177570093E-2</v>
+        <f t="shared" ref="P26" si="5">O26/SUM(O$7:O$28)</f>
+        <v>0</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -1812,7 +1846,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="5">
         <f>SUM(O7:O28)</f>
-        <v>2140</v>
+        <v>2120</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="2"/>
@@ -1938,15 +1972,15 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="5">
-        <f t="shared" ref="N32:N48" si="3">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
+        <f t="shared" ref="N32:N48" si="6">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>200</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" ref="O32:O48" si="4">MEDIAN(C32,N32,D32)</f>
+        <f t="shared" ref="O32:O48" si="7">MEDIAN(C32,N32,D32)</f>
         <v>200</v>
       </c>
       <c r="P32" s="6">
-        <f t="shared" ref="P32:P51" si="5">O32/SUM(O$32:O$50)</f>
+        <f t="shared" ref="P32:P51" si="8">O32/SUM(O$32:O$50)</f>
         <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q32" s="2"/>
@@ -1981,15 +2015,15 @@
         <v>25</v>
       </c>
       <c r="N33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="P33" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q33" s="2"/>
@@ -2022,15 +2056,15 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="P34" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.5712449110777802E-2</v>
       </c>
       <c r="Q34" s="2"/>
@@ -2067,15 +2101,15 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="O35" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="P35" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.8568673666166703E-2</v>
       </c>
       <c r="Q35" s="2"/>
@@ -2108,15 +2142,15 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="P36" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q36" s="2"/>
@@ -2149,15 +2183,15 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="P37" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.4283265481037072E-2</v>
       </c>
       <c r="Q37" s="2"/>
@@ -2198,15 +2232,15 @@
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>143</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>143</v>
       </c>
       <c r="P38" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.1281337047353758E-2</v>
       </c>
       <c r="Q38" s="2"/>
@@ -2241,15 +2275,15 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>92</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>92</v>
       </c>
       <c r="P39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3.9425755303192631E-2</v>
       </c>
       <c r="Q39" s="2"/>
@@ -2286,15 +2320,15 @@
         <v>15</v>
       </c>
       <c r="N40" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="P40" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5.5710306406685235E-2</v>
       </c>
       <c r="Q40" s="2"/>
@@ -2331,15 +2365,15 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="P41" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q41" s="2"/>
@@ -2376,15 +2410,15 @@
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="P42" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q42" s="2"/>
@@ -2417,15 +2451,15 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="P43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q43" s="2"/>
@@ -2466,15 +2500,15 @@
         <v>1</v>
       </c>
       <c r="N44" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>50.5</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>50.5</v>
       </c>
       <c r="P44" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.1641311334904649E-2</v>
       </c>
       <c r="Q44" s="2"/>
@@ -2509,15 +2543,15 @@
         <v>25</v>
       </c>
       <c r="N45" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="P45" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q45" s="2"/>
@@ -2552,15 +2586,15 @@
         <v>25</v>
       </c>
       <c r="N46" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="P46" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.5708163702592668E-2</v>
       </c>
       <c r="Q46" s="2"/>
@@ -2595,15 +2629,15 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
       <c r="N47" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="P47" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2.0569959288622243E-2</v>
       </c>
       <c r="Q47" s="2"/>
@@ -2642,15 +2676,15 @@
         <v>15</v>
       </c>
       <c r="N48" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>195</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>195</v>
       </c>
       <c r="P48" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.3565459610027856E-2</v>
       </c>
       <c r="Q48" s="2"/>
@@ -2693,7 +2727,7 @@
         <v>100</v>
       </c>
       <c r="P49" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.2854081851296334E-2</v>
       </c>
       <c r="Q49" s="2"/>
@@ -2709,7 +2743,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="4">
         <v>25</v>
@@ -2736,7 +2770,7 @@
         <v>145</v>
       </c>
       <c r="P50" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.2138418684379686E-2</v>
       </c>
       <c r="Q50" s="2"/>
@@ -2770,7 +2804,7 @@
         <v>2333.5</v>
       </c>
       <c r="P51" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Q51" s="2"/>
@@ -2893,15 +2927,15 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="5">
-        <f t="shared" ref="N54:N70" si="6">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <f t="shared" ref="N54:N70" si="9">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
       <c r="O54" s="5">
-        <f t="shared" ref="O54:O70" si="7">MEDIAN(C54,N54,D54)</f>
+        <f t="shared" ref="O54:O70" si="10">MEDIAN(C54,N54,D54)</f>
         <v>135</v>
       </c>
       <c r="P54" s="6">
-        <f t="shared" ref="P54:P71" si="8">O54/SUM(O$54:O$70)</f>
+        <f t="shared" ref="P54:P71" si="11">O54/SUM(O$54:O$70)</f>
         <v>0.14438502673796791</v>
       </c>
       <c r="Q54" s="2"/>
@@ -2938,15 +2972,15 @@
         <v>5</v>
       </c>
       <c r="N55" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="O55" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="P55" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>9.6256684491978606E-2</v>
       </c>
       <c r="Q55" s="2"/>
@@ -2981,15 +3015,15 @@
         <v>10</v>
       </c>
       <c r="N56" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="O56" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>110</v>
       </c>
       <c r="P56" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="Q56" s="2"/>
@@ -3024,15 +3058,15 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="O57" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="P57" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>8.5561497326203204E-2</v>
       </c>
       <c r="Q57" s="2"/>
@@ -3069,15 +3103,15 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>135</v>
       </c>
       <c r="O58" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>135</v>
       </c>
       <c r="P58" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.14438502673796791</v>
       </c>
       <c r="Q58" s="2"/>
@@ -3114,15 +3148,15 @@
         <v>10</v>
       </c>
       <c r="N59" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>105</v>
       </c>
       <c r="O59" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
       <c r="P59" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.11229946524064172</v>
       </c>
       <c r="Q59" s="2"/>
@@ -3159,15 +3193,15 @@
         <v>15</v>
       </c>
       <c r="N60" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>145</v>
       </c>
       <c r="O60" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>145</v>
       </c>
       <c r="P60" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.15508021390374332</v>
       </c>
       <c r="Q60" s="2"/>
@@ -3183,7 +3217,7 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B61" s="4">
         <v>5</v>
@@ -3202,15 +3236,15 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="O61" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="P61" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.8128342245989303E-2</v>
       </c>
       <c r="Q61" s="2"/>
@@ -3226,7 +3260,7 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="4">
         <v>0</v>
@@ -3249,15 +3283,15 @@
         <v>5</v>
       </c>
       <c r="N62" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="O62" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="P62" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>9.6256684491978606E-2</v>
       </c>
       <c r="Q62" s="2"/>
@@ -3286,15 +3320,15 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O63" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P63" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q63" s="2"/>
@@ -3323,15 +3357,15 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O64" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P64" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q64" s="2"/>
@@ -3360,15 +3394,15 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
       <c r="N65" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O65" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P65" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q65" s="2"/>
@@ -3397,15 +3431,15 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O66" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P66" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q66" s="2"/>
@@ -3434,15 +3468,15 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O67" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P67" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q67" s="2"/>
@@ -3471,15 +3505,15 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O68" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P68" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q68" s="2"/>
@@ -3508,15 +3542,15 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O69" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P69" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q69" s="2"/>
@@ -3545,15 +3579,15 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O70" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P70" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q70" s="2"/>
@@ -3587,7 +3621,7 @@
         <v>935</v>
       </c>
       <c r="P71" s="6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Q71" s="2"/>

</xml_diff>

<commit_message>
Update event prob table to something resembling current settings
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9657EC88-D63A-4A7A-A2CC-092D534D34DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E19BBF-68F0-473C-AF70-513937143D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Moderate</t>
   </si>
   <si>
-    <t>Communication Blackout</t>
-  </si>
-  <si>
     <t>Electrical Storm</t>
   </si>
   <si>
@@ -165,12 +162,6 @@
   </si>
   <si>
     <t>Ion Storm</t>
-  </si>
-  <si>
-    <t>Prison Break</t>
-  </si>
-  <si>
-    <t>Containment Error - Virology</t>
   </si>
   <si>
     <t>Containment Error - Xenobiology</t>
@@ -186,9 +177,6 @@
   </si>
   <si>
     <t>Moderate Spider Infestation</t>
-  </si>
-  <si>
-    <t>Viral Infection</t>
   </si>
   <si>
     <t>Moderate Infestation</t>
@@ -219,6 +207,21 @@
   </si>
   <si>
     <t>Min Pop</t>
+  </si>
+  <si>
+    <t>Comet Expulsion</t>
+  </si>
+  <si>
+    <t>Containment Error - Bridge</t>
+  </si>
+  <si>
+    <t>Containment Error - Security</t>
+  </si>
+  <si>
+    <t>Comms Blackout</t>
+  </si>
+  <si>
+    <t>Comms Blackout - Damage</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -284,11 +287,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -305,6 +349,11 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,13 +569,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE11BF8-2C51-4794-BAB0-B08C213463FD}">
-  <dimension ref="A1:AA994"/>
+  <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -627,7 +678,7 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>SUM(B3:I3)*1.5</f>
-        <v>34.5</v>
+        <v>31.5</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -648,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="4">
         <v>6</v>
@@ -777,7 +828,7 @@
         <v>9</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>17</v>
@@ -819,16 +870,16 @@
       <c r="M7" s="4"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5">
-        <f>SUM(B7+E7*$A$3+F7*$B$3+G7*$C$3+H7*$D$3+I7*$E$3+J7*$F$3+K7*$G$3+L7*$H$3+M7*$I$3)</f>
+        <f t="shared" ref="O7:O27" si="0">SUM(B7+E7*$A$3+F7*$B$3+G7*$C$3+H7*$D$3+I7*$E$3+J7*$F$3+K7*$G$3+L7*$H$3+M7*$I$3)</f>
         <v>120</v>
       </c>
       <c r="P7" s="5">
-        <f>MEDIAN(C7,O7,D7)</f>
+        <f t="shared" ref="P7:P27" si="1">MEDIAN(C7,O7,D7)</f>
         <v>120</v>
       </c>
       <c r="Q7" s="6">
-        <f t="shared" ref="Q7:Q11" si="0">P7/SUM(P$7:P$27)</f>
-        <v>5.8823529411764705E-2</v>
+        <f t="shared" ref="Q7:Q11" si="2">P7/SUM(P$7:P$27)</f>
+        <v>5.5172413793103448E-2</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -865,16 +916,16 @@
         <v>1</v>
       </c>
       <c r="O8" s="5">
-        <f>SUM(B8+E8*$A$3+F8*$B$3+G8*$C$3+H8*$D$3+I8*$E$3+J8*$F$3+K8*$G$3+L8*$H$3+M8*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="P8" s="5">
-        <f>MEDIAN(C8,O8,D8)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="Q8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.9215686274509803E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.6781609195402298E-2</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -911,16 +962,16 @@
         <v>1</v>
       </c>
       <c r="O9" s="5">
-        <f>SUM(B9+E9*$A$3+F9*$B$3+G9*$C$3+H9*$D$3+I9*$E$3+J9*$F$3+K9*$G$3+L9*$H$3+M9*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="P9" s="5">
-        <f>MEDIAN(C9,O9,D9)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="Q9" s="6">
-        <f t="shared" si="0"/>
-        <v>1.7156862745098041E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.6091954022988506E-2</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -957,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="O10" s="5">
-        <f>SUM(B10+E10*$A$3+F10*$B$3+G10*$C$3+H10*$D$3+I10*$E$3+J10*$F$3+K10*$G$3+L10*$H$3+M10*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="P10" s="5">
-        <f>MEDIAN(C10,O10,D10)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="Q10" s="6">
-        <f t="shared" si="0"/>
-        <v>2.9411764705882353E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.7586206896551724E-2</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -1001,16 +1052,16 @@
         <v>1</v>
       </c>
       <c r="O11" s="5">
-        <f>SUM(B11+E11*$A$3+F11*$B$3+G11*$C$3+H11*$D$3+I11*$E$3+J11*$F$3+K11*$G$3+L11*$H$3+M11*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="P11" s="5">
-        <f>MEDIAN(C11,O11,D11)</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="Q11" s="6">
-        <f t="shared" si="0"/>
-        <v>0.14705882352941177</v>
+        <f t="shared" si="2"/>
+        <v>0.13793103448275862</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -1045,16 +1096,16 @@
         <v>1</v>
       </c>
       <c r="O12" s="8">
-        <f>SUM(B12+E12*$A$3+F12*$B$3+G12*$C$3+H12*$D$3+I12*$E$3+J12*$F$3+K12*$G$3+L12*$H$3+M12*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="P12" s="8">
-        <f>MEDIAN(C12,O12,D12)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="Q12" s="9">
-        <f t="shared" ref="Q12:Q28" si="1">P12/SUM(P$7:P$27)</f>
-        <v>4.9019607843137254E-3</v>
+        <f t="shared" ref="Q12:Q28" si="3">P12/SUM(P$7:P$27)</f>
+        <v>4.5977011494252873E-3</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -1095,16 +1146,16 @@
         <v>1</v>
       </c>
       <c r="O13" s="5">
-        <f>SUM(B13+E13*$A$3+F13*$B$3+G13*$C$3+H13*$D$3+I13*$E$3+J13*$F$3+K13*$G$3+L13*$H$3+M13*$I$3)</f>
-        <v>34.5</v>
+        <f t="shared" si="0"/>
+        <v>31.5</v>
       </c>
       <c r="P13" s="5">
-        <f>MEDIAN(C13,O13,D13)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="Q13" s="6">
-        <f t="shared" si="1"/>
-        <v>7.3529411764705881E-3</v>
+        <f t="shared" si="3"/>
+        <v>6.8965517241379309E-3</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1139,16 +1190,16 @@
         <v>1</v>
       </c>
       <c r="O14" s="5">
-        <f>SUM(B14+E14*$A$3+F14*$B$3+G14*$C$3+H14*$D$3+I14*$E$3+J14*$F$3+K14*$G$3+L14*$H$3+M14*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="P14" s="5">
-        <f>MEDIAN(C14,O14,D14)</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="Q14" s="6">
-        <f t="shared" si="1"/>
-        <v>0.14705882352941177</v>
+        <f t="shared" si="3"/>
+        <v>0.13793103448275862</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -1189,16 +1240,16 @@
         <v>1</v>
       </c>
       <c r="O15" s="5">
-        <f>SUM(B15+E15*$A$3+F15*$B$3+G15*$C$3+H15*$D$3+I15*$E$3+J15*$F$3+K15*$G$3+L15*$H$3+M15*$I$3)</f>
-        <v>138</v>
+        <f t="shared" si="0"/>
+        <v>126</v>
       </c>
       <c r="P15" s="5">
-        <f>MEDIAN(C15,O15,D15)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="Q15" s="6">
-        <f t="shared" si="1"/>
-        <v>2.4509803921568627E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.2988505747126436E-2</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -1237,16 +1288,16 @@
         <v>1</v>
       </c>
       <c r="O16" s="5">
-        <f>SUM(B16+E16*$A$3+F16*$B$3+G16*$C$3+H16*$D$3+I16*$E$3+J16*$F$3+K16*$G$3+L16*$H$3+M16*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="P16" s="5">
-        <f>MEDIAN(C16,O16,D16)</f>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="Q16" s="6">
-        <f t="shared" si="1"/>
-        <v>6.8627450980392163E-2</v>
+        <f t="shared" si="3"/>
+        <v>6.4367816091954022E-2</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -1285,16 +1336,16 @@
         <v>1</v>
       </c>
       <c r="O17" s="5">
-        <f>SUM(B17+E17*$A$3+F17*$B$3+G17*$C$3+H17*$D$3+I17*$E$3+J17*$F$3+K17*$G$3+L17*$H$3+M17*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="P17" s="5">
-        <f>MEDIAN(C17,O17,D17)</f>
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="Q17" s="6">
-        <f t="shared" si="1"/>
-        <v>5.6372549019607844E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.2873563218390804E-2</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -1329,16 +1380,16 @@
         <v>1</v>
       </c>
       <c r="O18" s="5">
-        <f>SUM(B18+E18*$A$3+F18*$B$3+G18*$C$3+H18*$D$3+I18*$E$3+J18*$F$3+K18*$G$3+L18*$H$3+M18*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="P18" s="5">
-        <f>MEDIAN(C18,O18,D18)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="Q18" s="6">
-        <f t="shared" si="1"/>
-        <v>2.6960784313725492E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.528735632183908E-2</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -1373,16 +1424,16 @@
         <v>1</v>
       </c>
       <c r="O19" s="5">
-        <f>SUM(B19+E19*$A$3+F19*$B$3+G19*$C$3+H19*$D$3+I19*$E$3+J19*$F$3+K19*$G$3+L19*$H$3+M19*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="P19" s="5">
-        <f>MEDIAN(C19,O19,D19)</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="Q19" s="6">
-        <f t="shared" si="1"/>
-        <v>4.9019607843137254E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.5977011494252873E-2</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -1417,16 +1468,16 @@
         <v>1</v>
       </c>
       <c r="O20" s="5">
-        <f>SUM(B20+E20*$A$3+F20*$B$3+G20*$C$3+H20*$D$3+I20*$E$3+J20*$F$3+K20*$G$3+L20*$H$3+M20*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="P20" s="5">
-        <f>MEDIAN(C20,O20,D20)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="Q20" s="6">
-        <f t="shared" si="1"/>
-        <v>3.9215686274509803E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.6781609195402298E-2</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -1461,16 +1512,16 @@
         <v>1</v>
       </c>
       <c r="O21" s="5">
-        <f>SUM(B21+E21*$A$3+F21*$B$3+G21*$C$3+H21*$D$3+I21*$E$3+J21*$F$3+K21*$G$3+L21*$H$3+M21*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="P21" s="5">
-        <f>MEDIAN(C21,O21,D21)</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="Q21" s="6">
-        <f t="shared" si="1"/>
-        <v>0.14705882352941177</v>
+        <f t="shared" si="3"/>
+        <v>0.13793103448275862</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1498,25 +1549,29 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4">
-        <v>30</v>
-      </c>
-      <c r="K22" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="K22" s="4">
+        <v>15</v>
+      </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="M22" s="4">
+        <v>15</v>
+      </c>
       <c r="N22" s="5">
         <v>1</v>
       </c>
       <c r="O22" s="5">
-        <f>SUM(B22+E22*$A$3+F22*$B$3+G22*$C$3+H22*$D$3+I22*$E$3+J22*$F$3+K22*$G$3+L22*$H$3+M22*$I$3)</f>
-        <v>90</v>
+        <f t="shared" si="0"/>
+        <v>225</v>
       </c>
       <c r="P22" s="5">
-        <f>MEDIAN(C22,O22,D22)</f>
-        <v>90</v>
+        <f t="shared" si="1"/>
+        <v>225</v>
       </c>
       <c r="Q22" s="6">
-        <f t="shared" si="1"/>
-        <v>4.4117647058823532E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.10344827586206896</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -1553,16 +1608,16 @@
         <v>1</v>
       </c>
       <c r="O23" s="5">
-        <f>SUM(B23+E23*$A$3+F23*$B$3+G23*$C$3+H23*$D$3+I23*$E$3+J23*$F$3+K23*$G$3+L23*$H$3+M23*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="P23" s="5">
-        <f>MEDIAN(C23,O23,D23)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="Q23" s="6">
-        <f t="shared" si="1"/>
-        <v>6.3725490196078427E-2</v>
+        <f t="shared" si="3"/>
+        <v>5.9770114942528735E-2</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1597,16 +1652,16 @@
         <v>1</v>
       </c>
       <c r="O24" s="5">
-        <f>SUM(B24+E24*$A$3+F24*$B$3+G24*$C$3+H24*$D$3+I24*$E$3+J24*$F$3+K24*$G$3+L24*$H$3+M24*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="P24" s="5">
-        <f>MEDIAN(C24,O24,D24)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="Q24" s="6">
-        <f t="shared" si="1"/>
-        <v>2.9411764705882353E-2</v>
+        <f t="shared" si="3"/>
+        <v>2.7586206896551724E-2</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -1635,15 +1690,15 @@
       <c r="M25" s="4"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5">
-        <f>SUM(B25+E25*$A$3+F25*$B$3+G25*$C$3+H25*$D$3+I25*$E$3+J25*$F$3+K25*$G$3+L25*$H$3+M25*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P25" s="5">
-        <f>MEDIAN(C25,O25,D25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R25" s="2"/>
@@ -1673,15 +1728,15 @@
       <c r="M26" s="4"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5">
-        <f>SUM(B26+E26*$A$3+F26*$B$3+G26*$C$3+H26*$D$3+I26*$E$3+J26*$F$3+K26*$G$3+L26*$H$3+M26*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P26" s="5">
-        <f>MEDIAN(C26,O26,D26)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q26" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R26" s="2"/>
@@ -1711,15 +1766,15 @@
       <c r="M27" s="4"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5">
-        <f>SUM(B27+E27*$A$3+F27*$B$3+G27*$C$3+H27*$D$3+I27*$E$3+J27*$F$3+K27*$G$3+L27*$H$3+M27*$I$3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P27" s="5">
-        <f>MEDIAN(C27,O27,D27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R27" s="2"/>
@@ -1751,10 +1806,10 @@
       <c r="O28" s="2"/>
       <c r="P28" s="5">
         <f>SUM(P7:P27)</f>
-        <v>2040</v>
+        <v>2175</v>
       </c>
       <c r="Q28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R28" s="2"/>
@@ -1840,7 +1895,7 @@
         <v>9</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>17</v>
@@ -1882,16 +1937,16 @@
       <c r="M31" s="4"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5">
-        <f>IF(C31&gt;0,MAX(B31,C31),B31)+E31*$A$3+F31*$B$3+G31*$C$3+H31*$D$3+I31*$E$3+J31*$F$3+K31*$G$3+L31*$H$3+M31*$I$3</f>
+        <f t="shared" ref="O31:O47" si="4">IF(C31&gt;0,MAX(B31,C31),B31)+E31*$A$3+F31*$B$3+G31*$C$3+H31*$D$3+I31*$E$3+J31*$F$3+K31*$G$3+L31*$H$3+M31*$I$3</f>
         <v>200</v>
       </c>
       <c r="P31" s="5">
-        <f>MEDIAN(C31,O31,D31)</f>
+        <f t="shared" ref="P31:P47" si="5">MEDIAN(C31,O31,D31)</f>
         <v>200</v>
       </c>
       <c r="Q31" s="6">
         <f>P31/SUM(P$31:P$47)</f>
-        <v>9.7967180994366881E-2</v>
+        <v>0.10191082802547771</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -1906,10 +1961,10 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B32" s="4">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1919,23 +1974,25 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="4">
+        <v>25</v>
+      </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="5">
         <v>1</v>
       </c>
       <c r="O32" s="5">
-        <f>IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
-        <v>60</v>
+        <f t="shared" ref="O32" si="6">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
+        <v>100</v>
       </c>
       <c r="P32" s="5">
-        <f>MEDIAN(C32,O32,D32)</f>
-        <v>60</v>
+        <f t="shared" ref="P32" si="7">MEDIAN(C32,O32,D32)</f>
+        <v>100</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" ref="Q32:Q48" si="2">P32/SUM(P$31:P$47)</f>
-        <v>2.9390154298310066E-2</v>
+        <f>P32/SUM(P$31:P$47)</f>
+        <v>5.0955414012738856E-2</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -1950,23 +2007,19 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B33" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="4">
-        <v>5</v>
-      </c>
+      <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="4">
-        <v>20</v>
-      </c>
+      <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -1974,16 +2027,16 @@
         <v>1</v>
       </c>
       <c r="O33" s="5">
-        <f>IF(C33&gt;0,MAX(B33,C33),B33)+E33*$A$3+F33*$B$3+G33*$C$3+H33*$D$3+I33*$E$3+J33*$F$3+K33*$G$3+L33*$H$3+M33*$I$3</f>
-        <v>90</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
       </c>
       <c r="P33" s="5">
-        <f>MEDIAN(C33,O33,D33)</f>
-        <v>90</v>
+        <f t="shared" si="5"/>
+        <v>100</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" si="2"/>
-        <v>4.4085231447465102E-2</v>
+        <f>P33/SUM(P$31:P$47)</f>
+        <v>5.0955414012738856E-2</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -1998,7 +2051,7 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B34" s="4">
         <v>100</v>
@@ -2008,7 +2061,9 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="H34" s="4">
+        <v>25</v>
+      </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -2018,16 +2073,16 @@
         <v>1</v>
       </c>
       <c r="O34" s="5">
-        <f>IF(C34&gt;0,MAX(B34,C34),B34)+E34*$A$3+F34*$B$3+G34*$C$3+H34*$D$3+I34*$E$3+J34*$F$3+K34*$G$3+L34*$H$3+M34*$I$3</f>
-        <v>100</v>
+        <f t="shared" ref="O34" si="8">IF(C34&gt;0,MAX(B34,C34),B34)+E34*$A$3+F34*$B$3+G34*$C$3+H34*$D$3+I34*$E$3+J34*$F$3+K34*$G$3+L34*$H$3+M34*$I$3</f>
+        <v>200</v>
       </c>
       <c r="P34" s="5">
-        <f>MEDIAN(C34,O34,D34)</f>
-        <v>100</v>
+        <f t="shared" ref="P34" si="9">MEDIAN(C34,O34,D34)</f>
+        <v>200</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8983590497183441E-2</v>
+        <f>P34/SUM(P$31:P$47)</f>
+        <v>0.10191082802547771</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -2042,19 +2097,23 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B35" s="4">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="4">
+        <v>5</v>
+      </c>
       <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="J35" s="4">
+        <v>20</v>
+      </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -2062,16 +2121,16 @@
         <v>1</v>
       </c>
       <c r="O35" s="5">
-        <f>IF(C35&gt;0,MAX(B35,C35),B35)+E35*$A$3+F35*$B$3+G35*$C$3+H35*$D$3+I35*$E$3+J35*$F$3+K35*$G$3+L35*$H$3+M35*$I$3</f>
-        <v>80</v>
+        <f t="shared" si="4"/>
+        <v>90</v>
       </c>
       <c r="P35" s="5">
-        <f>MEDIAN(C35,O35,D35)</f>
-        <v>80</v>
+        <f t="shared" si="5"/>
+        <v>90</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" si="2"/>
-        <v>3.9186872397746757E-2</v>
+        <f>P35/SUM(P$31:P$47)</f>
+        <v>4.5859872611464965E-2</v>
       </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -2086,7 +2145,7 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B36" s="4">
         <v>0</v>
@@ -2094,36 +2153,28 @@
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="4">
-        <v>45</v>
-      </c>
-      <c r="G36" s="4">
-        <v>25</v>
-      </c>
-      <c r="H36" s="4">
-        <v>6</v>
-      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="4">
-        <v>6</v>
-      </c>
+      <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="5">
         <v>1</v>
       </c>
       <c r="O36" s="5">
-        <f>IF(C36&gt;0,MAX(B36,C36),B36)+E36*$A$3+F36*$B$3+G36*$C$3+H36*$D$3+I36*$E$3+J36*$F$3+K36*$G$3+L36*$H$3+M36*$I$3</f>
-        <v>143</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="P36" s="5">
-        <f>MEDIAN(C36,O36,D36)</f>
-        <v>143</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="Q36" s="6">
-        <f t="shared" si="2"/>
-        <v>7.0046534410972319E-2</v>
+        <f>P36/SUM(P$31:P$47)</f>
+        <v>0</v>
       </c>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
@@ -2138,7 +2189,7 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B37" s="4">
         <v>0</v>
@@ -2147,31 +2198,27 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4">
-        <v>20</v>
-      </c>
+      <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="4">
-        <v>15</v>
-      </c>
+      <c r="M37" s="4"/>
       <c r="N37" s="5">
         <v>1</v>
       </c>
       <c r="O37" s="5">
-        <f>IF(C37&gt;0,MAX(B37,C37),B37)+E37*$A$3+F37*$B$3+G37*$C$3+H37*$D$3+I37*$E$3+J37*$F$3+K37*$G$3+L37*$H$3+M37*$I$3</f>
-        <v>130</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="P37" s="5">
-        <f>MEDIAN(C37,O37,D37)</f>
-        <v>130</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="Q37" s="6">
-        <f t="shared" si="2"/>
-        <v>6.3678667646338477E-2</v>
+        <f>P37/SUM(P$31:P$47)</f>
+        <v>0</v>
       </c>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
@@ -2186,7 +2233,7 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B38" s="4">
         <v>0</v>
@@ -2194,32 +2241,36 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="F38" s="4">
+        <v>45</v>
+      </c>
       <c r="G38" s="4">
-        <v>20</v>
-      </c>
-      <c r="H38" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="H38" s="4">
+        <v>6</v>
+      </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="4">
-        <v>15</v>
-      </c>
-      <c r="L38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4">
+        <v>6</v>
+      </c>
       <c r="M38" s="4"/>
       <c r="N38" s="5">
         <v>1</v>
       </c>
       <c r="O38" s="5">
-        <f>IF(C38&gt;0,MAX(B38,C38),B38)+E38*$A$3+F38*$B$3+G38*$C$3+H38*$D$3+I38*$E$3+J38*$F$3+K38*$G$3+L38*$H$3+M38*$I$3</f>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>131</v>
       </c>
       <c r="P38" s="5">
-        <f>MEDIAN(C38,O38,D38)</f>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>131</v>
       </c>
       <c r="Q38" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8983590497183441E-2</v>
+        <f>P38/SUM(P$31:P$47)</f>
+        <v>6.67515923566879E-2</v>
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
@@ -2234,7 +2285,7 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B39" s="4">
         <v>0</v>
@@ -2250,24 +2301,24 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="4">
+      <c r="L39" s="4"/>
+      <c r="M39" s="4">
         <v>15</v>
       </c>
-      <c r="M39" s="4"/>
       <c r="N39" s="5">
         <v>1</v>
       </c>
       <c r="O39" s="5">
-        <f>IF(C39&gt;0,MAX(B39,C39),B39)+E39*$A$3+F39*$B$3+G39*$C$3+H39*$D$3+I39*$E$3+J39*$F$3+K39*$G$3+L39*$H$3+M39*$I$3</f>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>130</v>
       </c>
       <c r="P39" s="5">
-        <f>MEDIAN(C39,O39,D39)</f>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>130</v>
       </c>
       <c r="Q39" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8983590497183441E-2</v>
+        <f>P39/SUM(P$31:P$47)</f>
+        <v>6.6242038216560509E-2</v>
       </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
@@ -2282,17 +2333,21 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B40" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="G40" s="4">
+        <v>20</v>
+      </c>
+      <c r="H40" s="4">
+        <v>15</v>
+      </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -2302,16 +2357,16 @@
         <v>1</v>
       </c>
       <c r="O40" s="5">
-        <f>IF(C40&gt;0,MAX(B40,C40),B40)+E40*$A$3+F40*$B$3+G40*$C$3+H40*$D$3+I40*$E$3+J40*$F$3+K40*$G$3+L40*$H$3+M40*$I$3</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P40" s="5">
-        <f>MEDIAN(C40,O40,D40)</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="Q40" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8983590497183441E-2</v>
+        <f>P40/SUM(P$31:P$47)</f>
+        <v>5.0955414012738856E-2</v>
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
@@ -2326,44 +2381,40 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
       </c>
-      <c r="C41" s="4">
-        <v>10</v>
-      </c>
-      <c r="D41" s="4">
-        <v>125</v>
-      </c>
-      <c r="E41" s="4">
-        <v>1</v>
-      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="G41" s="4">
+        <v>20</v>
+      </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4">
-        <v>1</v>
-      </c>
+      <c r="L41" s="4">
+        <v>25</v>
+      </c>
+      <c r="M41" s="4"/>
       <c r="N41" s="5">
         <v>1</v>
       </c>
       <c r="O41" s="5">
-        <f>IF(C41&gt;0,MAX(B41,C41),B41)+E41*$A$3+F41*$B$3+G41*$C$3+H41*$D$3+I41*$E$3+J41*$F$3+K41*$G$3+L41*$H$3+M41*$I$3</f>
-        <v>50.5</v>
+        <f t="shared" si="4"/>
+        <v>90</v>
       </c>
       <c r="P41" s="5">
-        <f>MEDIAN(C41,O41,D41)</f>
-        <v>50.5</v>
+        <f t="shared" si="5"/>
+        <v>90</v>
       </c>
       <c r="Q41" s="6">
-        <f t="shared" si="2"/>
-        <v>2.4736713201077638E-2</v>
+        <f>P41/SUM(P$31:P$47)</f>
+        <v>4.5859872611464965E-2</v>
       </c>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
@@ -2378,10 +2429,10 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B42" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2391,25 +2442,25 @@
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="K42" s="4">
+        <v>20</v>
+      </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="4">
-        <v>25</v>
-      </c>
+      <c r="M42" s="4"/>
       <c r="N42" s="5">
         <v>1</v>
       </c>
       <c r="O42" s="5">
-        <f>IF(C42&gt;0,MAX(B42,C42),B42)+E42*$A$3+F42*$B$3+G42*$C$3+H42*$D$3+I42*$E$3+J42*$F$3+K42*$G$3+L42*$H$3+M42*$I$3</f>
-        <v>200</v>
+        <f t="shared" si="4"/>
+        <v>180</v>
       </c>
       <c r="P42" s="5">
-        <f>MEDIAN(C42,O42,D42)</f>
-        <v>200</v>
+        <f t="shared" si="5"/>
+        <v>180</v>
       </c>
       <c r="Q42" s="6">
-        <f t="shared" si="2"/>
-        <v>9.7967180994366881E-2</v>
+        <f>P42/SUM(P$31:P$47)</f>
+        <v>9.171974522292993E-2</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
@@ -2424,14 +2475,20 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B43" s="4">
-        <v>50</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <v>10</v>
+      </c>
+      <c r="D43" s="4">
+        <v>125</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1</v>
+      </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -2440,22 +2497,22 @@
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="N43" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O43" s="5">
-        <f>IF(C43&gt;0,MAX(B43,C43),B43)+E43*$A$3+F43*$B$3+G43*$C$3+H43*$D$3+I43*$E$3+J43*$F$3+K43*$G$3+L43*$H$3+M43*$I$3</f>
-        <v>200</v>
+        <f t="shared" si="4"/>
+        <v>71.5</v>
       </c>
       <c r="P43" s="5">
-        <f>MEDIAN(C43,O43,D43)</f>
-        <v>200</v>
+        <f t="shared" si="5"/>
+        <v>71.5</v>
       </c>
       <c r="Q43" s="6">
-        <f t="shared" si="2"/>
-        <v>9.7967180994366881E-2</v>
+        <f>P43/SUM(P$31:P$47)</f>
+        <v>3.6433121019108283E-2</v>
       </c>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
@@ -2470,10 +2527,10 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B44" s="4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2483,25 +2540,25 @@
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
-      <c r="K44" s="4">
-        <v>12</v>
-      </c>
+      <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
+      <c r="M44" s="4">
+        <v>15</v>
+      </c>
       <c r="N44" s="5">
         <v>1</v>
       </c>
       <c r="O44" s="5">
-        <f>IF(C44&gt;0,MAX(B44,C44),B44)+E44*$A$3+F44*$B$3+G44*$C$3+H44*$D$3+I44*$E$3+J44*$F$3+K44*$G$3+L44*$H$3+M44*$I$3</f>
-        <v>48</v>
+        <f t="shared" si="4"/>
+        <v>140</v>
       </c>
       <c r="P44" s="5">
-        <f>MEDIAN(C44,O44,D44)</f>
-        <v>48</v>
+        <f t="shared" si="5"/>
+        <v>140</v>
       </c>
       <c r="Q44" s="6">
-        <f t="shared" si="2"/>
-        <v>2.3512123438648051E-2</v>
+        <f>P44/SUM(P$31:P$47)</f>
+        <v>7.1337579617834393E-2</v>
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
@@ -2516,10 +2573,10 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B45" s="4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2528,30 +2585,26 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="4">
-        <v>15</v>
-      </c>
-      <c r="K45" s="4">
-        <v>15</v>
-      </c>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N45" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O45" s="5">
-        <f>IF(C45&gt;0,MAX(B45,C45),B45)+E45*$A$3+F45*$B$3+G45*$C$3+H45*$D$3+I45*$E$3+J45*$F$3+K45*$G$3+L45*$H$3+M45*$I$3</f>
-        <v>195</v>
+        <f t="shared" si="4"/>
+        <v>110</v>
       </c>
       <c r="P45" s="5">
-        <f>MEDIAN(C45,O45,D45)</f>
-        <v>195</v>
+        <f t="shared" si="5"/>
+        <v>110</v>
       </c>
       <c r="Q45" s="6">
-        <f t="shared" si="2"/>
-        <v>9.5518001469507716E-2</v>
+        <f>P45/SUM(P$31:P$47)</f>
+        <v>5.605095541401274E-2</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
@@ -2566,10 +2619,10 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B46" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2578,26 +2631,30 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="J46" s="4">
+        <v>15</v>
+      </c>
       <c r="K46" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="M46" s="4">
+        <v>15</v>
+      </c>
       <c r="N46" s="5">
         <v>1</v>
       </c>
       <c r="O46" s="5">
-        <f>IF(C46&gt;0,MAX(B46,C46),B46)+E46*$A$3+F46*$B$3+G46*$C$3+H46*$D$3+I46*$E$3+J46*$F$3+K46*$G$3+L46*$H$3+M46*$I$3</f>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>175</v>
       </c>
       <c r="P46" s="5">
-        <f>MEDIAN(C46,O46,D46)</f>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>175</v>
       </c>
       <c r="Q46" s="6">
-        <f t="shared" si="2"/>
-        <v>4.8983590497183441E-2</v>
+        <f>P46/SUM(P$31:P$47)</f>
+        <v>8.9171974522292988E-2</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
@@ -2611,39 +2668,39 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="4">
+      <c r="A47" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="11">
         <v>25</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11">
         <v>30</v>
       </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="5">
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="12">
         <v>1</v>
       </c>
       <c r="O47" s="5">
-        <f>IF(C47&gt;0,MAX(B47,C47),B47)+E47*$A$3+F47*$B$3+G47*$C$3+H47*$D$3+I47*$E$3+J47*$F$3+K47*$G$3+L47*$H$3+M47*$I$3</f>
+        <f t="shared" si="4"/>
         <v>145</v>
       </c>
       <c r="P47" s="5">
-        <f>MEDIAN(C47,O47,D47)</f>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="Q47" s="6">
-        <f t="shared" si="2"/>
-        <v>7.1026206220915988E-2</v>
+        <f>P47/SUM(P$31:P$47)</f>
+        <v>7.3885350318471335E-2</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
@@ -2657,28 +2714,39 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
+      <c r="A48" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="13">
+        <v>20</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13">
+        <v>15</v>
+      </c>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="14">
+        <v>1</v>
+      </c>
+      <c r="O48" s="10">
+        <f t="shared" ref="O48:O50" si="10">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
+        <v>80</v>
+      </c>
       <c r="P48" s="5">
-        <f>SUM(P31:P47)</f>
-        <v>2041.5</v>
+        <f t="shared" ref="P48:P50" si="11">MEDIAN(C48,O48,D48)</f>
+        <v>80</v>
       </c>
       <c r="Q48" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>P48/SUM(P$31:P$47)</f>
+        <v>4.0764331210191081E-2</v>
       </c>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
@@ -2692,25 +2760,34 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="14">
+        <v>1</v>
+      </c>
+      <c r="O49" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="6">
+        <f>P49/SUM(P$31:P$47)</f>
+        <v>0</v>
+      </c>
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
@@ -2723,56 +2800,33 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="14">
         <v>1</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N50" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O50" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q50" s="3" t="s">
-        <v>19</v>
+      <c r="O50" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="6">
+        <f>P50/SUM(P$31:P$47)</f>
+        <v>0</v>
       </c>
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
@@ -2786,35 +2840,28 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="4">
-        <v>135</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5">
-        <f>IF(C51&gt;0,MAX(B51,C51),B51)+E51*$A$3+F51*$B$3+G51*$C$3+H51*$D$3+I51*$E$3+J51*$F$3+K51*$G$3+L51*$H$3+M51*$I$3</f>
-        <v>135</v>
-      </c>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
       <c r="P51" s="5">
-        <f>MEDIAN(C51,O51,D51)</f>
-        <v>135</v>
+        <f>SUM(P31:P47)</f>
+        <v>1962.5</v>
       </c>
       <c r="Q51" s="6">
-        <f>P51/SUM(P$51:P$64)</f>
-        <v>0.19285714285714287</v>
+        <f>P51/SUM(P$31:P$47)</f>
+        <v>1</v>
       </c>
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
@@ -2828,42 +2875,25 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="4">
-        <v>40</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4">
-        <v>5</v>
-      </c>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4">
-        <v>5</v>
-      </c>
-      <c r="N52" s="5">
-        <v>10</v>
-      </c>
-      <c r="O52" s="5">
-        <f>IF(C52&gt;0,MAX(B52,C52),B52)+E52*$A$3+F52*$B$3+G52*$C$3+H52*$D$3+I52*$E$3+J52*$F$3+K52*$G$3+L52*$H$3+M52*$I$3</f>
-        <v>90</v>
-      </c>
-      <c r="P52" s="5">
-        <f>MEDIAN(C52,O52,D52)</f>
-        <v>90</v>
-      </c>
-      <c r="Q52" s="6">
-        <f>P52/SUM(P$51:P$64)</f>
-        <v>0.12857142857142856</v>
-      </c>
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
@@ -2876,41 +2906,56 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N53" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="4">
-        <v>75</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4">
-        <v>10</v>
-      </c>
-      <c r="I53" s="4">
-        <v>20</v>
-      </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="5">
-        <v>1</v>
-      </c>
-      <c r="O53" s="5">
-        <f>IF(C53&gt;0,MAX(B53,C53),B53)+E53*$A$3+F53*$B$3+G53*$C$3+H53*$D$3+I53*$E$3+J53*$F$3+K53*$G$3+L53*$H$3+M53*$I$3</f>
-        <v>135</v>
-      </c>
-      <c r="P53" s="5">
-        <f>MEDIAN(C53,O53,D53)</f>
-        <v>135</v>
-      </c>
-      <c r="Q53" s="6">
-        <f t="shared" ref="Q53:Q65" si="3">P53/SUM(P$51:P$64)</f>
-        <v>0.19285714285714287</v>
+      <c r="O53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
@@ -2925,10 +2970,10 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B54" s="4">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2938,27 +2983,21 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
-      <c r="K54" s="4">
-        <v>5</v>
-      </c>
+      <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4">
-        <v>10</v>
-      </c>
-      <c r="N54" s="5">
-        <v>8</v>
-      </c>
+      <c r="M54" s="4"/>
+      <c r="N54" s="5"/>
       <c r="O54" s="5">
-        <f>IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
-        <v>105</v>
+        <f t="shared" ref="O54:O67" si="12">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <v>135</v>
       </c>
       <c r="P54" s="5">
-        <f>MEDIAN(C54,O54,D54)</f>
-        <v>105</v>
+        <f t="shared" ref="P54:P67" si="13">MEDIAN(C54,O54,D54)</f>
+        <v>135</v>
       </c>
       <c r="Q54" s="6">
-        <f t="shared" si="3"/>
-        <v>0.15</v>
+        <f>P54/SUM(P$54:P$67)</f>
+        <v>0.156794425087108</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
@@ -2973,40 +3012,40 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B55" s="4">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
+      <c r="H55" s="4">
+        <v>5</v>
+      </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
-      <c r="K55" s="4">
-        <v>10</v>
-      </c>
+      <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N55" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O55" s="5">
-        <f>IF(C55&gt;0,MAX(B55,C55),B55)+E55*$A$3+F55*$B$3+G55*$C$3+H55*$D$3+I55*$E$3+J55*$F$3+K55*$G$3+L55*$H$3+M55*$I$3</f>
-        <v>145</v>
+        <f t="shared" si="12"/>
+        <v>90</v>
       </c>
       <c r="P55" s="5">
-        <f>MEDIAN(C55,O55,D55)</f>
-        <v>145</v>
+        <f t="shared" si="13"/>
+        <v>90</v>
       </c>
       <c r="Q55" s="6">
-        <f t="shared" si="3"/>
-        <v>0.20714285714285716</v>
+        <f>P55/SUM(P$54:P$67)</f>
+        <v>0.10452961672473868</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -3021,10 +3060,10 @@
     </row>
     <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B56" s="4">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -3034,29 +3073,27 @@
       <c r="H56" s="4">
         <v>10</v>
       </c>
-      <c r="I56" s="4"/>
+      <c r="I56" s="4">
+        <v>20</v>
+      </c>
       <c r="J56" s="4"/>
-      <c r="K56" s="4">
-        <v>5</v>
-      </c>
+      <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="4">
-        <v>5</v>
-      </c>
+      <c r="M56" s="4"/>
       <c r="N56" s="5">
         <v>1</v>
       </c>
       <c r="O56" s="5">
-        <f>IF(C56&gt;0,MAX(B56,C56),B56)+E56*$A$3+F56*$B$3+G56*$C$3+H56*$D$3+I56*$E$3+J56*$F$3+K56*$G$3+L56*$H$3+M56*$I$3</f>
-        <v>90</v>
+        <f t="shared" si="12"/>
+        <v>135</v>
       </c>
       <c r="P56" s="5">
-        <f>MEDIAN(C56,O56,D56)</f>
-        <v>90</v>
+        <f t="shared" si="13"/>
+        <v>135</v>
       </c>
       <c r="Q56" s="6">
-        <f t="shared" si="3"/>
-        <v>0.12857142857142856</v>
+        <f t="shared" ref="Q56:Q68" si="14">P56/SUM(P$54:P$67)</f>
+        <v>0.156794425087108</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
@@ -3070,8 +3107,12 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="4">
+        <v>25</v>
+      </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -3080,21 +3121,27 @@
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
+      <c r="K57" s="4">
+        <v>10</v>
+      </c>
       <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="5"/>
+      <c r="M57" s="4">
+        <v>10</v>
+      </c>
+      <c r="N57" s="5">
+        <v>8</v>
+      </c>
       <c r="O57" s="5">
-        <f>IF(C57&gt;0,MAX(B57,C57),B57)+E57*$A$3+F57*$B$3+G57*$C$3+H57*$D$3+I57*$E$3+J57*$F$3+K57*$G$3+L57*$H$3+M57*$I$3</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>125</v>
       </c>
       <c r="P57" s="5">
-        <f>MEDIAN(C57,O57,D57)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>125</v>
       </c>
       <c r="Q57" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.14518002322880372</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
@@ -3108,8 +3155,12 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="4">
+        <v>15</v>
+      </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -3118,21 +3169,27 @@
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
+      <c r="K58" s="4">
+        <v>5</v>
+      </c>
       <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="5"/>
+      <c r="M58" s="4">
+        <v>15</v>
+      </c>
+      <c r="N58" s="5">
+        <v>1</v>
+      </c>
       <c r="O58" s="5">
-        <f>IF(C58&gt;0,MAX(B58,C58),B58)+E58*$A$3+F58*$B$3+G58*$C$3+H58*$D$3+I58*$E$3+J58*$F$3+K58*$G$3+L58*$H$3+M58*$I$3</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>125</v>
       </c>
       <c r="P58" s="5">
-        <f>MEDIAN(C58,O58,D58)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>125</v>
       </c>
       <c r="Q58" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.14518002322880372</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -3146,31 +3203,43 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="4">
+        <v>0</v>
+      </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
+      <c r="H59" s="4">
+        <v>10</v>
+      </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
+      <c r="K59" s="4">
+        <v>5</v>
+      </c>
       <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="5"/>
+      <c r="M59" s="4">
+        <v>5</v>
+      </c>
+      <c r="N59" s="5">
+        <v>1</v>
+      </c>
       <c r="O59" s="5">
-        <f>IF(C59&gt;0,MAX(B59,C59),B59)+E59*$A$3+F59*$B$3+G59*$C$3+H59*$D$3+I59*$E$3+J59*$F$3+K59*$G$3+L59*$H$3+M59*$I$3</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>90</v>
       </c>
       <c r="P59" s="5">
-        <f>MEDIAN(C59,O59,D59)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>90</v>
       </c>
       <c r="Q59" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.10452961672473868</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -3184,31 +3253,39 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
+      <c r="H60" s="4">
+        <v>20</v>
+      </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
-      <c r="N60" s="5"/>
+      <c r="N60" s="5">
+        <v>8</v>
+      </c>
       <c r="O60" s="5">
-        <f>IF(C60&gt;0,MAX(B60,C60),B60)+E60*$A$3+F60*$B$3+G60*$C$3+H60*$D$3+I60*$E$3+J60*$F$3+K60*$G$3+L60*$H$3+M60*$I$3</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>81</v>
       </c>
       <c r="P60" s="5">
-        <f>MEDIAN(C60,O60,D60)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>81</v>
       </c>
       <c r="Q60" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>9.4076655052264813E-2</v>
       </c>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
@@ -3222,31 +3299,39 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="4">
+        <v>20</v>
+      </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
+      <c r="H61" s="4">
+        <v>15</v>
+      </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
-      <c r="N61" s="5"/>
+      <c r="N61" s="5">
+        <v>1</v>
+      </c>
       <c r="O61" s="5">
-        <f>IF(C61&gt;0,MAX(B61,C61),B61)+E61*$A$3+F61*$B$3+G61*$C$3+H61*$D$3+I61*$E$3+J61*$F$3+K61*$G$3+L61*$H$3+M61*$I$3</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>80</v>
       </c>
       <c r="P61" s="5">
-        <f>MEDIAN(C61,O61,D61)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>80</v>
       </c>
       <c r="Q61" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>9.2915214866434379E-2</v>
       </c>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
@@ -3275,15 +3360,15 @@
       <c r="M62" s="4"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5">
-        <f>IF(C62&gt;0,MAX(B62,C62),B62)+E62*$A$3+F62*$B$3+G62*$C$3+H62*$D$3+I62*$E$3+J62*$F$3+K62*$G$3+L62*$H$3+M62*$I$3</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P62" s="5">
-        <f>MEDIAN(C62,O62,D62)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q62" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R62" s="2"/>
@@ -3313,15 +3398,15 @@
       <c r="M63" s="4"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5">
-        <f>IF(C63&gt;0,MAX(B63,C63),B63)+E63*$A$3+F63*$B$3+G63*$C$3+H63*$D$3+I63*$E$3+J63*$F$3+K63*$G$3+L63*$H$3+M63*$I$3</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P63" s="5">
-        <f>MEDIAN(C63,O63,D63)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q63" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R63" s="2"/>
@@ -3351,15 +3436,15 @@
       <c r="M64" s="4"/>
       <c r="N64" s="5"/>
       <c r="O64" s="5">
-        <f>IF(C64&gt;0,MAX(B64,C64),B64)+E64*$A$3+F64*$B$3+G64*$C$3+H64*$D$3+I64*$E$3+J64*$F$3+K64*$G$3+L64*$H$3+M64*$I$3</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P64" s="5">
-        <f>MEDIAN(C64,O64,D64)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="Q64" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="R64" s="2"/>
@@ -3374,28 +3459,31 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-      <c r="O65" s="2"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="P65" s="5">
-        <f>SUM(P50:P64)</f>
-        <v>700</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="Q65" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
@@ -3409,23 +3497,32 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="P66" s="5">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q66" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
@@ -3438,23 +3535,32 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="P67" s="5">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
@@ -3482,8 +3588,14 @@
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
+      <c r="P68" s="5">
+        <f>SUM(P53:P67)</f>
+        <v>861</v>
+      </c>
+      <c r="Q68" s="6">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
@@ -9208,9 +9320,93 @@
       <c r="Z265" s="2"/>
       <c r="AA265" s="2"/>
     </row>
-    <row r="266" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2"/>
+      <c r="B266" s="2"/>
+      <c r="C266" s="2"/>
+      <c r="D266" s="2"/>
+      <c r="E266" s="2"/>
+      <c r="F266" s="2"/>
+      <c r="G266" s="2"/>
+      <c r="H266" s="2"/>
+      <c r="I266" s="2"/>
+      <c r="J266" s="2"/>
+      <c r="K266" s="2"/>
+      <c r="L266" s="2"/>
+      <c r="M266" s="2"/>
+      <c r="N266" s="2"/>
+      <c r="O266" s="2"/>
+      <c r="P266" s="2"/>
+      <c r="Q266" s="2"/>
+      <c r="R266" s="2"/>
+      <c r="S266" s="2"/>
+      <c r="T266" s="2"/>
+      <c r="U266" s="2"/>
+      <c r="V266" s="2"/>
+      <c r="W266" s="2"/>
+      <c r="X266" s="2"/>
+      <c r="Y266" s="2"/>
+      <c r="Z266" s="2"/>
+      <c r="AA266" s="2"/>
+    </row>
+    <row r="267" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2"/>
+      <c r="B267" s="2"/>
+      <c r="C267" s="2"/>
+      <c r="D267" s="2"/>
+      <c r="E267" s="2"/>
+      <c r="F267" s="2"/>
+      <c r="G267" s="2"/>
+      <c r="H267" s="2"/>
+      <c r="I267" s="2"/>
+      <c r="J267" s="2"/>
+      <c r="K267" s="2"/>
+      <c r="L267" s="2"/>
+      <c r="M267" s="2"/>
+      <c r="N267" s="2"/>
+      <c r="O267" s="2"/>
+      <c r="P267" s="2"/>
+      <c r="Q267" s="2"/>
+      <c r="R267" s="2"/>
+      <c r="S267" s="2"/>
+      <c r="T267" s="2"/>
+      <c r="U267" s="2"/>
+      <c r="V267" s="2"/>
+      <c r="W267" s="2"/>
+      <c r="X267" s="2"/>
+      <c r="Y267" s="2"/>
+      <c r="Z267" s="2"/>
+      <c r="AA267" s="2"/>
+    </row>
+    <row r="268" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2"/>
+      <c r="B268" s="2"/>
+      <c r="C268" s="2"/>
+      <c r="D268" s="2"/>
+      <c r="E268" s="2"/>
+      <c r="F268" s="2"/>
+      <c r="G268" s="2"/>
+      <c r="H268" s="2"/>
+      <c r="I268" s="2"/>
+      <c r="J268" s="2"/>
+      <c r="K268" s="2"/>
+      <c r="L268" s="2"/>
+      <c r="M268" s="2"/>
+      <c r="N268" s="2"/>
+      <c r="O268" s="2"/>
+      <c r="P268" s="2"/>
+      <c r="Q268" s="2"/>
+      <c r="R268" s="2"/>
+      <c r="S268" s="2"/>
+      <c r="T268" s="2"/>
+      <c r="U268" s="2"/>
+      <c r="V268" s="2"/>
+      <c r="W268" s="2"/>
+      <c r="X268" s="2"/>
+      <c r="Y268" s="2"/>
+      <c r="Z268" s="2"/>
+      <c r="AA268" s="2"/>
+    </row>
     <row r="269" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="270" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="271" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9937,6 +10133,9 @@
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
More event variations and fixes
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9998939-5C99-43CF-BE54-AFA03018F4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD698411-A99F-4BEF-8B59-8D9B4AB818E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18120" yWindow="-4995" windowWidth="18240" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>Assumed Personnel</t>
   </si>
@@ -345,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,8 +364,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -586,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE11BF8-2C51-4794-BAB0-B08C213463FD}">
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -693,10 +692,10 @@
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f>SUM(B3:I3)*1.5</f>
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
@@ -851,7 +850,7 @@
       <c r="P6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="R6" s="2"/>
@@ -890,15 +889,15 @@
         <f t="shared" ref="O7:O27" si="0">SUM(B7+E7*$A$3+F7*$B$3+G7*$C$3+H7*$D$3+I7*$E$3+J7*$F$3+K7*$G$3+L7*$H$3+M7*$I$3)</f>
         <v>120</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <f t="shared" ref="P7:P27" si="1">MEDIAN(C7,O7,D7)</f>
         <v>120</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="17">
         <f>IF($A$3 &gt; N7, P7/SUM(P$7:P$27), 0)</f>
-        <v>5.8111380145278453E-2</v>
-      </c>
-      <c r="R7" s="15"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="R7" s="14"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -936,15 +935,15 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="15">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="Q8" s="18">
-        <f t="shared" ref="Q8:Q27" si="2">IF($A$3 &gt; N8, P8/SUM(P$7:P$27), 0)</f>
-        <v>3.1476997578692496E-2</v>
-      </c>
-      <c r="R8" s="14"/>
+      <c r="Q8" s="17">
+        <f>IF($A$3 &gt; N8, P8/SUM(P$7:P$27), 0)</f>
+        <v>2.9545454545454545E-2</v>
+      </c>
+      <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -986,9 +985,9 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="Q9" s="18">
-        <f t="shared" si="2"/>
-        <v>1.6949152542372881E-2</v>
+      <c r="Q9" s="17">
+        <f>IF($A$3 &gt; N9, P9/SUM(P$7:P$27), 0)</f>
+        <v>1.5909090909090907E-2</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -1032,9 +1031,9 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="Q10" s="18">
-        <f t="shared" si="2"/>
-        <v>2.4213075060532687E-2</v>
+      <c r="Q10" s="17">
+        <f>IF($A$3 &gt; N10, P10/SUM(P$7:P$27), 0)</f>
+        <v>2.2727272727272728E-2</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -1076,9 +1075,9 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="Q11" s="18">
-        <f t="shared" si="2"/>
-        <v>0.14527845036319612</v>
+      <c r="Q11" s="17">
+        <f>IF($A$3 &gt; N11, P11/SUM(P$7:P$27), 0)</f>
+        <v>0.13636363636363635</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -1120,9 +1119,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="Q12" s="18">
-        <f t="shared" si="2"/>
-        <v>4.8426150121065378E-3</v>
+      <c r="Q12" s="17">
+        <f>IF($A$3 &gt; N12, P12/SUM(P$7:P$27), 0)</f>
+        <v>4.5454545454545452E-3</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -1164,15 +1163,15 @@
       </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="P13" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="Q13" s="18">
-        <f t="shared" si="2"/>
-        <v>7.2639225181598066E-3</v>
+      <c r="Q13" s="17">
+        <f>IF($A$3 &gt; N13, P13/SUM(P$7:P$27), 0)</f>
+        <v>6.8181818181818179E-3</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1214,9 +1213,9 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="Q14" s="18">
-        <f t="shared" si="2"/>
-        <v>0.14527845036319612</v>
+      <c r="Q14" s="17">
+        <f>IF($A$3 &gt; N14, P14/SUM(P$7:P$27), 0)</f>
+        <v>0.13636363636363635</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -1258,15 +1257,15 @@
       </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="Q15" s="18">
-        <f t="shared" si="2"/>
-        <v>2.4213075060532687E-2</v>
+      <c r="Q15" s="17">
+        <f>IF($A$3 &gt; N15, P15/SUM(P$7:P$27), 0)</f>
+        <v>2.2727272727272728E-2</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -1312,9 +1311,9 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="Q16" s="18">
-        <f t="shared" si="2"/>
-        <v>5.8111380145278453E-2</v>
+      <c r="Q16" s="17">
+        <f>IF($A$3 &gt; N16, P16/SUM(P$7:P$27), 0)</f>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -1360,9 +1359,9 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="Q17" s="18">
-        <f t="shared" si="2"/>
-        <v>5.3268765133171914E-2</v>
+      <c r="Q17" s="17">
+        <f>IF($A$3 &gt; N17, P17/SUM(P$7:P$27), 0)</f>
+        <v>0.05</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -1404,9 +1403,9 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="Q18" s="18">
-        <f t="shared" si="2"/>
-        <v>2.6634382566585957E-2</v>
+      <c r="Q18" s="17">
+        <f>IF($A$3 &gt; N18, P18/SUM(P$7:P$27), 0)</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -1448,9 +1447,9 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="Q19" s="18">
-        <f t="shared" si="2"/>
-        <v>4.8426150121065374E-2</v>
+      <c r="Q19" s="17">
+        <f>IF($A$3 &gt; N19, P19/SUM(P$7:P$27), 0)</f>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -1492,9 +1491,9 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="Q20" s="18">
-        <f t="shared" si="2"/>
-        <v>3.8740920096852302E-2</v>
+      <c r="Q20" s="17">
+        <f>IF($A$3 &gt; N20, P20/SUM(P$7:P$27), 0)</f>
+        <v>3.6363636363636362E-2</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -1536,9 +1535,9 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="Q21" s="18">
-        <f t="shared" si="2"/>
-        <v>0.14527845036319612</v>
+      <c r="Q21" s="17">
+        <f>IF($A$3 &gt; N21, P21/SUM(P$7:P$27), 0)</f>
+        <v>0.13636363636363635</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1586,9 +1585,9 @@
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="Q22" s="18">
-        <f t="shared" si="2"/>
-        <v>9.4430992736077482E-2</v>
+      <c r="Q22" s="17">
+        <f>IF($A$3 &gt; N22, P22/SUM(P$7:P$27), 0)</f>
+        <v>8.8636363636363638E-2</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -1632,9 +1631,9 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="Q23" s="18">
-        <f t="shared" si="2"/>
-        <v>4.8426150121065374E-2</v>
+      <c r="Q23" s="17">
+        <f>IF($A$3 &gt; N23, P23/SUM(P$7:P$27), 0)</f>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1676,9 +1675,9 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="Q24" s="18">
-        <f t="shared" si="2"/>
-        <v>2.9055690072639227E-2</v>
+      <c r="Q24" s="17">
+        <f>IF($A$3 &gt; N24, P24/SUM(P$7:P$27), 0)</f>
+        <v>2.7272727272727271E-2</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -1692,31 +1691,41 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="4">
+        <v>50</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4">
+        <v>20</v>
+      </c>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="J25" s="4">
+        <v>25</v>
+      </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="5"/>
+      <c r="N25" s="5">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>135</v>
+      </c>
+      <c r="Q25" s="17">
+        <f>IF($A$3 &gt; N25, P25/SUM(P$7:P$27), 0)</f>
+        <v>6.1363636363636363E-2</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -1752,8 +1761,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="18">
-        <f t="shared" si="2"/>
+      <c r="Q26" s="17">
+        <f>IF($A$3 &gt; N26, P26/SUM(P$7:P$27), 0)</f>
         <v>0</v>
       </c>
       <c r="R26" s="2"/>
@@ -1790,8 +1799,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="18">
-        <f t="shared" si="2"/>
+      <c r="Q27" s="17">
+        <f>IF($A$3 &gt; N27, P27/SUM(P$7:P$27), 0)</f>
         <v>0</v>
       </c>
       <c r="R27" s="2"/>
@@ -1823,10 +1832,10 @@
       <c r="O28" s="2"/>
       <c r="P28" s="5">
         <f>SUM(P7:P27)</f>
-        <v>2065</v>
+        <v>2200</v>
       </c>
       <c r="Q28" s="6">
-        <f t="shared" ref="Q12:Q28" si="3">P28/SUM(P$7:P$27)</f>
+        <f>P28/SUM(P$7:P$27)</f>
         <v>1</v>
       </c>
       <c r="R28" s="2"/>
@@ -1956,16 +1965,16 @@
         <v>0</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" ref="O31:O47" si="4">IF(C31&gt;0,MAX(B31,C31),B31)+E31*$A$3+F31*$B$3+G31*$C$3+H31*$D$3+I31*$E$3+J31*$F$3+K31*$G$3+L31*$H$3+M31*$I$3</f>
+        <f t="shared" ref="O31:O47" si="2">IF(C31&gt;0,MAX(B31,C31),B31)+E31*$A$3+F31*$B$3+G31*$C$3+H31*$D$3+I31*$E$3+J31*$F$3+K31*$G$3+L31*$H$3+M31*$I$3</f>
         <v>200</v>
       </c>
       <c r="P31" s="5">
-        <f t="shared" ref="P31:P47" si="5">MEDIAN(C31,O31,D31)</f>
+        <f t="shared" ref="P31:P47" si="3">MEDIAN(C31,O31,D31)</f>
         <v>200</v>
       </c>
       <c r="Q31" s="6">
         <f>IF($A$3 &gt; N31, P31/SUM(P$31:P$50), 0)</f>
-        <v>0.11176306230790724</v>
+        <v>0.11344299489506524</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -2002,16 +2011,16 @@
         <v>1</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" ref="O32" si="6">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
+        <f t="shared" ref="O32" si="4">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>100</v>
       </c>
       <c r="P32" s="5">
-        <f t="shared" ref="P32" si="7">MEDIAN(C32,O32,D32)</f>
+        <f t="shared" ref="P32" si="5">MEDIAN(C32,O32,D32)</f>
         <v>100</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" ref="Q32:Q50" si="8">IF($A$3 &gt; N32, P32/SUM(P$31:P$50), 0)</f>
-        <v>5.5881531153953619E-2</v>
+        <f>IF($A$3 &gt; N32, P32/SUM(P$31:P$50), 0)</f>
+        <v>5.6721497447532618E-2</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -2046,16 +2055,16 @@
         <v>1</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="P33" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" si="8"/>
-        <v>5.5881531153953619E-2</v>
+        <f>IF($A$3 &gt; N33, P33/SUM(P$31:P$50), 0)</f>
+        <v>5.6721497447532618E-2</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -2092,16 +2101,16 @@
         <v>6</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" ref="O34" si="9">IF(C34&gt;0,MAX(B34,C34),B34)+E34*$A$3+F34*$B$3+G34*$C$3+H34*$D$3+I34*$E$3+J34*$F$3+K34*$G$3+L34*$H$3+M34*$I$3</f>
+        <f t="shared" ref="O34" si="6">IF(C34&gt;0,MAX(B34,C34),B34)+E34*$A$3+F34*$B$3+G34*$C$3+H34*$D$3+I34*$E$3+J34*$F$3+K34*$G$3+L34*$H$3+M34*$I$3</f>
         <v>175</v>
       </c>
       <c r="P34" s="5">
-        <f t="shared" ref="P34" si="10">MEDIAN(C34,O34,D34)</f>
+        <f t="shared" ref="P34" si="7">MEDIAN(C34,O34,D34)</f>
         <v>175</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" si="8"/>
-        <v>9.7792679519418835E-2</v>
+        <f>IF($A$3 &gt; N34, P34/SUM(P$31:P$50), 0)</f>
+        <v>9.9262620533182078E-2</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -2119,15 +2128,17 @@
         <v>39</v>
       </c>
       <c r="B35" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="4">
+        <v>10</v>
+      </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4">
@@ -2140,16 +2151,16 @@
         <v>1</v>
       </c>
       <c r="O35" s="5">
-        <f t="shared" si="4"/>
-        <v>85</v>
+        <f t="shared" si="2"/>
+        <v>105</v>
       </c>
       <c r="P35" s="5">
-        <f t="shared" si="5"/>
-        <v>85</v>
+        <f t="shared" si="3"/>
+        <v>105</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" si="8"/>
-        <v>4.7499301480860574E-2</v>
+        <f>IF($A$3 &gt; N35, P35/SUM(P$31:P$50), 0)</f>
+        <v>5.9557572319909248E-2</v>
       </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -2184,15 +2195,15 @@
         <v>1</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P36" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q36" s="6">
-        <f t="shared" si="8"/>
+        <f>IF($A$3 &gt; N36, P36/SUM(P$31:P$50), 0)</f>
         <v>0</v>
       </c>
       <c r="R36" s="2"/>
@@ -2228,15 +2239,15 @@
         <v>1</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P37" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q37" s="6">
-        <f t="shared" si="8"/>
+        <f>IF($A$3 &gt; N37, P37/SUM(P$31:P$50), 0)</f>
         <v>0</v>
       </c>
       <c r="R37" s="2"/>
@@ -2280,16 +2291,16 @@
         <v>1</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="4"/>
-        <v>119</v>
+        <f t="shared" si="2"/>
+        <v>74</v>
       </c>
       <c r="P38" s="5">
-        <f t="shared" si="5"/>
-        <v>119</v>
+        <f t="shared" si="3"/>
+        <v>74</v>
       </c>
       <c r="Q38" s="6">
-        <f t="shared" si="8"/>
-        <v>6.6499022073204808E-2</v>
+        <f>IF($A$3 &gt; N38, P38/SUM(P$31:P$50), 0)</f>
+        <v>4.1973908111174137E-2</v>
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
@@ -2328,16 +2339,16 @@
         <v>1</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="P39" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="Q39" s="6">
-        <f t="shared" si="8"/>
-        <v>5.5881531153953619E-2</v>
+        <f>IF($A$3 &gt; N39, P39/SUM(P$31:P$50), 0)</f>
+        <v>5.6721497447532618E-2</v>
       </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
@@ -2376,16 +2387,16 @@
         <v>1</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="P40" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="Q40" s="6">
-        <f t="shared" si="8"/>
-        <v>4.7499301480860574E-2</v>
+        <f>IF($A$3 &gt; N40, P40/SUM(P$31:P$50), 0)</f>
+        <v>4.821327283040272E-2</v>
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
@@ -2424,16 +2435,16 @@
         <v>1</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="P41" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="Q41" s="6">
-        <f t="shared" si="8"/>
-        <v>3.6322995250069851E-2</v>
+        <f>IF($A$3 &gt; N41, P41/SUM(P$31:P$50), 0)</f>
+        <v>3.6868973340896199E-2</v>
       </c>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
@@ -2470,16 +2481,16 @@
         <v>1</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="P42" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="Q42" s="6">
-        <f t="shared" si="8"/>
-        <v>0.10058675607711651</v>
+        <f>IF($A$3 &gt; N42, P42/SUM(P$31:P$50), 0)</f>
+        <v>0.1020986954055587</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
@@ -2522,16 +2533,16 @@
         <v>1</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="4"/>
-        <v>55.5</v>
+        <f t="shared" si="2"/>
+        <v>54</v>
       </c>
       <c r="P43" s="5">
-        <f t="shared" si="5"/>
-        <v>55.5</v>
+        <f t="shared" si="3"/>
+        <v>54</v>
       </c>
       <c r="Q43" s="6">
-        <f t="shared" si="8"/>
-        <v>3.1014249790444259E-2</v>
+        <f>IF($A$3 &gt; N43, P43/SUM(P$31:P$50), 0)</f>
+        <v>3.0629608621667612E-2</v>
       </c>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
@@ -2568,16 +2579,16 @@
         <v>1</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="P44" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="Q44" s="6">
-        <f t="shared" si="8"/>
-        <v>6.1469684269348977E-2</v>
+        <f>IF($A$3 &gt; N44, P44/SUM(P$31:P$50), 0)</f>
+        <v>6.2393647192285878E-2</v>
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
@@ -2614,16 +2625,16 @@
         <v>8</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="P45" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="Q45" s="6">
-        <f t="shared" si="8"/>
-        <v>5.0293378038558254E-2</v>
+        <f>IF($A$3 &gt; N45, P45/SUM(P$31:P$50), 0)</f>
+        <v>5.104934770277935E-2</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
@@ -2664,16 +2675,16 @@
         <v>1</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
       <c r="P46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="Q46" s="6">
-        <f t="shared" si="8"/>
-        <v>8.1028220173232746E-2</v>
+        <f>IF($A$3 &gt; N46, P46/SUM(P$31:P$50), 0)</f>
+        <v>8.2246171298922296E-2</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
@@ -2710,16 +2721,16 @@
         <v>1</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="P47" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>115</v>
       </c>
       <c r="Q47" s="6">
-        <f t="shared" si="8"/>
-        <v>6.4263760827046656E-2</v>
+        <f>IF($A$3 &gt; N47, P47/SUM(P$31:P$50), 0)</f>
+        <v>6.5229722064662501E-2</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
@@ -2756,16 +2767,16 @@
         <v>1</v>
       </c>
       <c r="O48" s="9">
-        <f t="shared" ref="O48:O50" si="11">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
+        <f t="shared" ref="O48:O50" si="8">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
         <v>65</v>
       </c>
       <c r="P48" s="5">
-        <f t="shared" ref="P48:P50" si="12">MEDIAN(C48,O48,D48)</f>
+        <f t="shared" ref="P48:P50" si="9">MEDIAN(C48,O48,D48)</f>
         <v>65</v>
       </c>
       <c r="Q48" s="6">
-        <f t="shared" si="8"/>
-        <v>3.6322995250069851E-2</v>
+        <f>IF($A$3 &gt; N48, P48/SUM(P$31:P$50), 0)</f>
+        <v>3.6868973340896199E-2</v>
       </c>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
@@ -2796,15 +2807,15 @@
         <v>1</v>
       </c>
       <c r="O49" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P49" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q49" s="6">
-        <f t="shared" si="8"/>
+        <f>IF($A$3 &gt; N49, P49/SUM(P$31:P$50), 0)</f>
         <v>0</v>
       </c>
       <c r="R49" s="2"/>
@@ -2836,15 +2847,15 @@
         <v>1</v>
       </c>
       <c r="O50" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P50" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q50" s="6">
-        <f t="shared" si="8"/>
+        <f>IF($A$3 &gt; N50, P50/SUM(P$31:P$50), 0)</f>
         <v>0</v>
       </c>
       <c r="R50" s="2"/>
@@ -2876,7 +2887,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="5">
         <f>SUM(P31:P50)</f>
-        <v>1789.5</v>
+        <v>1763</v>
       </c>
       <c r="Q51" s="6">
         <f>P51/SUM(P$31:P$50)</f>
@@ -3009,16 +3020,16 @@
         <v>0</v>
       </c>
       <c r="O54" s="5">
-        <f t="shared" ref="O54:O67" si="13">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <f t="shared" ref="O54:O67" si="10">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
       <c r="P54" s="5">
-        <f t="shared" ref="P54:P67" si="14">MEDIAN(C54,O54,D54)</f>
+        <f t="shared" ref="P54:P67" si="11">MEDIAN(C54,O54,D54)</f>
         <v>135</v>
       </c>
       <c r="Q54" s="6">
         <f>IF($A$3 &gt; N54, P54/SUM(P$54:P$67), 0)</f>
-        <v>0.18467852257181944</v>
+        <v>0.16343825665859565</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
@@ -3057,16 +3068,16 @@
         <v>10</v>
       </c>
       <c r="O55" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>75</v>
       </c>
       <c r="P55" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>75</v>
       </c>
       <c r="Q55" s="6">
-        <f t="shared" ref="Q55:Q67" si="15">IF($A$3 &gt; N55, P55/SUM(P$54:P$67), 0)</f>
-        <v>0.10259917920656635</v>
+        <f>IF($A$3 &gt; N55, P55/SUM(P$54:P$67), 0)</f>
+        <v>9.0799031476997583E-2</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -3105,16 +3116,16 @@
         <v>4</v>
       </c>
       <c r="O56" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>125</v>
       </c>
       <c r="P56" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>125</v>
       </c>
       <c r="Q56" s="6">
-        <f t="shared" si="15"/>
-        <v>0.17099863201094392</v>
+        <f>IF($A$3 &gt; N56, P56/SUM(P$54:P$67), 0)</f>
+        <v>0.1513317191283293</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
@@ -3153,16 +3164,16 @@
         <v>8</v>
       </c>
       <c r="O57" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
       <c r="P57" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>105</v>
       </c>
       <c r="Q57" s="6">
-        <f t="shared" si="15"/>
-        <v>0.1436388508891929</v>
+        <f>IF($A$3 &gt; N57, P57/SUM(P$54:P$67), 0)</f>
+        <v>0.1271186440677966</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
@@ -3201,16 +3212,16 @@
         <v>1</v>
       </c>
       <c r="O58" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>95</v>
       </c>
       <c r="P58" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>95</v>
       </c>
       <c r="Q58" s="6">
-        <f t="shared" si="15"/>
-        <v>0.12995896032831739</v>
+        <f>IF($A$3 &gt; N58, P58/SUM(P$54:P$67), 0)</f>
+        <v>0.11501210653753027</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -3251,16 +3262,16 @@
         <v>4</v>
       </c>
       <c r="O59" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="P59" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>70</v>
       </c>
       <c r="Q59" s="6">
-        <f t="shared" si="15"/>
-        <v>9.575923392612859E-2</v>
+        <f>IF($A$3 &gt; N59, P59/SUM(P$54:P$67), 0)</f>
+        <v>8.4745762711864403E-2</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -3297,16 +3308,16 @@
         <v>8</v>
       </c>
       <c r="O60" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>61</v>
       </c>
       <c r="P60" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>61</v>
       </c>
       <c r="Q60" s="6">
-        <f t="shared" si="15"/>
-        <v>8.3447332421340628E-2</v>
+        <f>IF($A$3 &gt; N60, P60/SUM(P$54:P$67), 0)</f>
+        <v>7.3849878934624691E-2</v>
       </c>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
@@ -3343,16 +3354,16 @@
         <v>1</v>
       </c>
       <c r="O61" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="P61" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
       <c r="Q61" s="6">
-        <f t="shared" si="15"/>
-        <v>8.8919288645690833E-2</v>
+        <f>IF($A$3 &gt; N61, P61/SUM(P$54:P$67), 0)</f>
+        <v>7.8692493946731237E-2</v>
       </c>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
@@ -3366,31 +3377,43 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="4">
+        <v>30</v>
+      </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="4">
+        <v>20</v>
+      </c>
       <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
+      <c r="H62" s="4">
+        <v>15</v>
+      </c>
       <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
+      <c r="J62" s="4">
+        <v>20</v>
+      </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
-      <c r="N62" s="5"/>
+      <c r="N62" s="5">
+        <v>1</v>
+      </c>
       <c r="O62" s="5">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>95</v>
       </c>
       <c r="P62" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>95</v>
       </c>
       <c r="Q62" s="6">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f>IF($A$3 &gt; N62, P62/SUM(P$54:P$67), 0)</f>
+        <v>0.11501210653753027</v>
       </c>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
@@ -3419,15 +3442,15 @@
       <c r="M63" s="4"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P63" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q63" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($A$3 &gt; N63, P63/SUM(P$54:P$67), 0)</f>
         <v>0</v>
       </c>
       <c r="R63" s="2"/>
@@ -3457,15 +3480,15 @@
       <c r="M64" s="4"/>
       <c r="N64" s="5"/>
       <c r="O64" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P64" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q64" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($A$3 &gt; N64, P64/SUM(P$54:P$67), 0)</f>
         <v>0</v>
       </c>
       <c r="R64" s="2"/>
@@ -3495,15 +3518,15 @@
       <c r="M65" s="4"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P65" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q65" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($A$3 &gt; N65, P65/SUM(P$54:P$67), 0)</f>
         <v>0</v>
       </c>
       <c r="R65" s="2"/>
@@ -3533,15 +3556,15 @@
       <c r="M66" s="4"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P66" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q66" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($A$3 &gt; N66, P66/SUM(P$54:P$67), 0)</f>
         <v>0</v>
       </c>
       <c r="R66" s="2"/>
@@ -3571,15 +3594,15 @@
       <c r="M67" s="4"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P67" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q67" s="6">
-        <f t="shared" si="15"/>
+        <f>IF($A$3 &gt; N67, P67/SUM(P$54:P$67), 0)</f>
         <v>0</v>
       </c>
       <c r="R67" s="2"/>
@@ -3611,10 +3634,10 @@
       <c r="O68" s="2"/>
       <c r="P68" s="5">
         <f>SUM(P53:P67)</f>
-        <v>731</v>
+        <v>826</v>
       </c>
       <c r="Q68" s="6">
-        <f t="shared" ref="Q56:Q68" si="16">P68/SUM(P$54:P$67)</f>
+        <f t="shared" ref="Q68" si="12">P68/SUM(P$54:P$67)</f>
         <v>1</v>
       </c>
       <c r="R68" s="2"/>

</xml_diff>

<commit_message>
New/Changed Events Tuning (#20888)
First round of tuning after the addition of new electrical storms,
changes in behavior, etc. Details in the changelogs, but apart from
general balancing of event weights and effects, this PR also expands the
description info on Telecomms machinery to communicate that you need to
use Nanopaste to repair them (which I don't think was documented in-game
anywhere), and also adds a stack of Nanopaste to the TComms vestibule to
facilitate repairs if no one is around to produce the stuff.

Also you can beat Telecomms machinery with a stick to start garbling
them now! Take that, Medical channel!

There will probably be another round of balancing after this to make
sure the events all feel and play maximally right/fun.

---------

Signed-off-by: Batrachophreno <Batrochophreno@gmail.com>
Co-authored-by: SleepyGemmy <99297919+SleepyGemmy@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD698411-A99F-4BEF-8B59-8D9B4AB818E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7184E218-7B06-4BB4-B93C-B09395072FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18120" yWindow="-4995" windowWidth="18240" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE11BF8-2C51-4794-BAB0-B08C213463FD}">
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,7 +894,7 @@
         <v>120</v>
       </c>
       <c r="Q7" s="17">
-        <f>IF($A$3 &gt; N7, P7/SUM(P$7:P$27), 0)</f>
+        <f t="shared" ref="Q7:Q27" si="2">IF($A$3 &gt; N7, P7/SUM(P$7:P$27), 0)</f>
         <v>5.4545454545454543E-2</v>
       </c>
       <c r="R7" s="14"/>
@@ -924,7 +924,9 @@
         <v>15</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4">
+        <v>20</v>
+      </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -933,15 +935,15 @@
       </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="P8" s="15">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="Q8" s="17">
-        <f>IF($A$3 &gt; N8, P8/SUM(P$7:P$27), 0)</f>
-        <v>2.9545454545454545E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.8636363636363635E-2</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -986,7 +988,7 @@
         <v>35</v>
       </c>
       <c r="Q9" s="17">
-        <f>IF($A$3 &gt; N9, P9/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>1.5909090909090907E-2</v>
       </c>
       <c r="R9" s="2"/>
@@ -1032,7 +1034,7 @@
         <v>50</v>
       </c>
       <c r="Q10" s="17">
-        <f>IF($A$3 &gt; N10, P10/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>2.2727272727272728E-2</v>
       </c>
       <c r="R10" s="2"/>
@@ -1076,7 +1078,7 @@
         <v>300</v>
       </c>
       <c r="Q11" s="17">
-        <f>IF($A$3 &gt; N11, P11/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R11" s="2"/>
@@ -1120,7 +1122,7 @@
         <v>10</v>
       </c>
       <c r="Q12" s="17">
-        <f>IF($A$3 &gt; N12, P12/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>4.5454545454545452E-3</v>
       </c>
       <c r="R12" s="2"/>
@@ -1170,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="Q13" s="17">
-        <f>IF($A$3 &gt; N13, P13/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>6.8181818181818179E-3</v>
       </c>
       <c r="R13" s="2"/>
@@ -1214,7 +1216,7 @@
         <v>300</v>
       </c>
       <c r="Q14" s="17">
-        <f>IF($A$3 &gt; N14, P14/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R14" s="2"/>
@@ -1264,7 +1266,7 @@
         <v>50</v>
       </c>
       <c r="Q15" s="17">
-        <f>IF($A$3 &gt; N15, P15/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>2.2727272727272728E-2</v>
       </c>
       <c r="R15" s="2"/>
@@ -1312,7 +1314,7 @@
         <v>120</v>
       </c>
       <c r="Q16" s="17">
-        <f>IF($A$3 &gt; N16, P16/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>5.4545454545454543E-2</v>
       </c>
       <c r="R16" s="2"/>
@@ -1360,7 +1362,7 @@
         <v>110</v>
       </c>
       <c r="Q17" s="17">
-        <f>IF($A$3 &gt; N17, P17/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="R17" s="2"/>
@@ -1404,7 +1406,7 @@
         <v>55</v>
       </c>
       <c r="Q18" s="17">
-        <f>IF($A$3 &gt; N18, P18/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="R18" s="2"/>
@@ -1448,7 +1450,7 @@
         <v>100</v>
       </c>
       <c r="Q19" s="17">
-        <f>IF($A$3 &gt; N19, P19/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="R19" s="2"/>
@@ -1492,7 +1494,7 @@
         <v>80</v>
       </c>
       <c r="Q20" s="17">
-        <f>IF($A$3 &gt; N20, P20/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>3.6363636363636362E-2</v>
       </c>
       <c r="R20" s="2"/>
@@ -1536,7 +1538,7 @@
         <v>300</v>
       </c>
       <c r="Q21" s="17">
-        <f>IF($A$3 &gt; N21, P21/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R21" s="2"/>
@@ -1586,7 +1588,7 @@
         <v>195</v>
       </c>
       <c r="Q22" s="17">
-        <f>IF($A$3 &gt; N22, P22/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>8.8636363636363638E-2</v>
       </c>
       <c r="R22" s="2"/>
@@ -1632,7 +1634,7 @@
         <v>100</v>
       </c>
       <c r="Q23" s="17">
-        <f>IF($A$3 &gt; N23, P23/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="R23" s="2"/>
@@ -1676,7 +1678,7 @@
         <v>60</v>
       </c>
       <c r="Q24" s="17">
-        <f>IF($A$3 &gt; N24, P24/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>2.7272727272727271E-2</v>
       </c>
       <c r="R24" s="2"/>
@@ -1695,7 +1697,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1717,15 +1719,15 @@
       </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="Q25" s="17">
-        <f>IF($A$3 &gt; N25, P25/SUM(P$7:P$27), 0)</f>
-        <v>6.1363636363636363E-2</v>
+        <f t="shared" si="2"/>
+        <v>5.2272727272727269E-2</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -1762,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="17">
-        <f>IF($A$3 &gt; N26, P26/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R26" s="2"/>
@@ -1800,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="17">
-        <f>IF($A$3 &gt; N27, P27/SUM(P$7:P$27), 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R27" s="2"/>
@@ -1965,16 +1967,16 @@
         <v>0</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" ref="O31:O47" si="2">IF(C31&gt;0,MAX(B31,C31),B31)+E31*$A$3+F31*$B$3+G31*$C$3+H31*$D$3+I31*$E$3+J31*$F$3+K31*$G$3+L31*$H$3+M31*$I$3</f>
+        <f t="shared" ref="O31:O47" si="3">IF(C31&gt;0,MAX(B31,C31),B31)+E31*$A$3+F31*$B$3+G31*$C$3+H31*$D$3+I31*$E$3+J31*$F$3+K31*$G$3+L31*$H$3+M31*$I$3</f>
         <v>200</v>
       </c>
       <c r="P31" s="5">
-        <f t="shared" ref="P31:P47" si="3">MEDIAN(C31,O31,D31)</f>
+        <f t="shared" ref="P31:P47" si="4">MEDIAN(C31,O31,D31)</f>
         <v>200</v>
       </c>
       <c r="Q31" s="6">
         <f>IF($A$3 &gt; N31, P31/SUM(P$31:P$50), 0)</f>
-        <v>0.11344299489506524</v>
+        <v>0.11954572624028691</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -2011,16 +2013,16 @@
         <v>1</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" ref="O32" si="4">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
+        <f t="shared" ref="O32" si="5">IF(C32&gt;0,MAX(B32,C32),B32)+E32*$A$3+F32*$B$3+G32*$C$3+H32*$D$3+I32*$E$3+J32*$F$3+K32*$G$3+L32*$H$3+M32*$I$3</f>
         <v>100</v>
       </c>
       <c r="P32" s="5">
-        <f t="shared" ref="P32" si="5">MEDIAN(C32,O32,D32)</f>
+        <f t="shared" ref="P32" si="6">MEDIAN(C32,O32,D32)</f>
         <v>100</v>
       </c>
       <c r="Q32" s="6">
         <f>IF($A$3 &gt; N32, P32/SUM(P$31:P$50), 0)</f>
-        <v>5.6721497447532618E-2</v>
+        <v>5.9772863120143453E-2</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -2038,7 +2040,7 @@
         <v>61</v>
       </c>
       <c r="B33" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2055,16 +2057,16 @@
         <v>1</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="3"/>
+        <v>50</v>
       </c>
       <c r="P33" s="5">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>50</v>
       </c>
       <c r="Q33" s="6">
         <f>IF($A$3 &gt; N33, P33/SUM(P$31:P$50), 0)</f>
-        <v>5.6721497447532618E-2</v>
+        <v>2.9886431560071727E-2</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -2082,7 +2084,7 @@
         <v>62</v>
       </c>
       <c r="B34" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2101,16 +2103,16 @@
         <v>6</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" ref="O34" si="6">IF(C34&gt;0,MAX(B34,C34),B34)+E34*$A$3+F34*$B$3+G34*$C$3+H34*$D$3+I34*$E$3+J34*$F$3+K34*$G$3+L34*$H$3+M34*$I$3</f>
-        <v>175</v>
+        <f t="shared" ref="O34" si="7">IF(C34&gt;0,MAX(B34,C34),B34)+E34*$A$3+F34*$B$3+G34*$C$3+H34*$D$3+I34*$E$3+J34*$F$3+K34*$G$3+L34*$H$3+M34*$I$3</f>
+        <v>125</v>
       </c>
       <c r="P34" s="5">
-        <f t="shared" ref="P34" si="7">MEDIAN(C34,O34,D34)</f>
-        <v>175</v>
+        <f t="shared" ref="P34" si="8">MEDIAN(C34,O34,D34)</f>
+        <v>125</v>
       </c>
       <c r="Q34" s="6">
-        <f>IF($A$3 &gt; N34, P34/SUM(P$31:P$50), 0)</f>
-        <v>9.9262620533182078E-2</v>
+        <f t="shared" ref="Q34" si="9">IF($A$3 &gt; N34, P34/SUM(P$31:P$50), 0)</f>
+        <v>7.4716078900179325E-2</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -2128,7 +2130,7 @@
         <v>39</v>
       </c>
       <c r="B35" s="4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -2151,16 +2153,16 @@
         <v>1</v>
       </c>
       <c r="O35" s="5">
-        <f t="shared" si="2"/>
-        <v>105</v>
+        <f t="shared" si="3"/>
+        <v>95</v>
       </c>
       <c r="P35" s="5">
-        <f t="shared" si="3"/>
-        <v>105</v>
+        <f t="shared" si="4"/>
+        <v>95</v>
       </c>
       <c r="Q35" s="6">
-        <f>IF($A$3 &gt; N35, P35/SUM(P$31:P$50), 0)</f>
-        <v>5.9557572319909248E-2</v>
+        <f t="shared" ref="Q35:Q50" si="10">IF($A$3 &gt; N35, P35/SUM(P$31:P$50), 0)</f>
+        <v>5.6784219964136282E-2</v>
       </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -2195,15 +2197,15 @@
         <v>1</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="P36" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="Q36" s="6">
-        <f>IF($A$3 &gt; N36, P36/SUM(P$31:P$50), 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R36" s="2"/>
@@ -2239,15 +2241,15 @@
         <v>1</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="P37" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="Q37" s="6">
-        <f>IF($A$3 &gt; N37, P37/SUM(P$31:P$50), 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R37" s="2"/>
@@ -2291,16 +2293,16 @@
         <v>1</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="2"/>
-        <v>74</v>
-      </c>
-      <c r="P38" s="5">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
+      <c r="P38" s="5">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
       <c r="Q38" s="6">
-        <f>IF($A$3 &gt; N38, P38/SUM(P$31:P$50), 0)</f>
-        <v>4.1973908111174137E-2</v>
+        <f t="shared" si="10"/>
+        <v>4.4231918708906158E-2</v>
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
@@ -2339,16 +2341,16 @@
         <v>1</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="P39" s="5">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
+      <c r="P39" s="5">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
       <c r="Q39" s="6">
-        <f>IF($A$3 &gt; N39, P39/SUM(P$31:P$50), 0)</f>
-        <v>5.6721497447532618E-2</v>
+        <f t="shared" si="10"/>
+        <v>5.9772863120143453E-2</v>
       </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
@@ -2387,16 +2389,16 @@
         <v>1</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="P40" s="5">
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
+      <c r="P40" s="5">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
       <c r="Q40" s="6">
-        <f>IF($A$3 &gt; N40, P40/SUM(P$31:P$50), 0)</f>
-        <v>4.821327283040272E-2</v>
+        <f t="shared" si="10"/>
+        <v>5.0806933652121938E-2</v>
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
@@ -2435,16 +2437,16 @@
         <v>1</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-      <c r="P41" s="5">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
+      <c r="P41" s="5">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
       <c r="Q41" s="6">
-        <f>IF($A$3 &gt; N41, P41/SUM(P$31:P$50), 0)</f>
-        <v>3.6868973340896199E-2</v>
+        <f t="shared" si="10"/>
+        <v>3.8852361028093245E-2</v>
       </c>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
@@ -2481,16 +2483,16 @@
         <v>1</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="2"/>
-        <v>180</v>
-      </c>
-      <c r="P42" s="5">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
+      <c r="P42" s="5">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
       <c r="Q42" s="6">
-        <f>IF($A$3 &gt; N42, P42/SUM(P$31:P$50), 0)</f>
-        <v>0.1020986954055587</v>
+        <f t="shared" si="10"/>
+        <v>0.10759115361625822</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
@@ -2533,16 +2535,16 @@
         <v>1</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="2"/>
-        <v>54</v>
-      </c>
-      <c r="P43" s="5">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
+      <c r="P43" s="5">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
       <c r="Q43" s="6">
-        <f>IF($A$3 &gt; N43, P43/SUM(P$31:P$50), 0)</f>
-        <v>3.0629608621667612E-2</v>
+        <f t="shared" si="10"/>
+        <v>3.2277346084877465E-2</v>
       </c>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
@@ -2579,16 +2581,16 @@
         <v>1</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="P44" s="5">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
+      <c r="P44" s="5">
+        <f t="shared" si="4"/>
+        <v>110</v>
+      </c>
       <c r="Q44" s="6">
-        <f>IF($A$3 &gt; N44, P44/SUM(P$31:P$50), 0)</f>
-        <v>6.2393647192285878E-2</v>
+        <f t="shared" si="10"/>
+        <v>6.5750149432157803E-2</v>
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
@@ -2625,16 +2627,16 @@
         <v>8</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="P45" s="5">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
+      <c r="P45" s="5">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
       <c r="Q45" s="6">
-        <f>IF($A$3 &gt; N45, P45/SUM(P$31:P$50), 0)</f>
-        <v>5.104934770277935E-2</v>
+        <f t="shared" si="10"/>
+        <v>5.379557680812911E-2</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
@@ -2675,16 +2677,16 @@
         <v>1</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-      <c r="P46" s="5">
         <f t="shared" si="3"/>
         <v>145</v>
       </c>
+      <c r="P46" s="5">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
       <c r="Q46" s="6">
-        <f>IF($A$3 &gt; N46, P46/SUM(P$31:P$50), 0)</f>
-        <v>8.2246171298922296E-2</v>
+        <f t="shared" si="10"/>
+        <v>8.6670651524208012E-2</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
@@ -2721,16 +2723,16 @@
         <v>1</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="2"/>
-        <v>115</v>
-      </c>
-      <c r="P47" s="5">
         <f t="shared" si="3"/>
         <v>115</v>
       </c>
+      <c r="P47" s="5">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
       <c r="Q47" s="6">
-        <f>IF($A$3 &gt; N47, P47/SUM(P$31:P$50), 0)</f>
-        <v>6.5229722064662501E-2</v>
+        <f t="shared" si="10"/>
+        <v>6.8738792588164968E-2</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
@@ -2759,7 +2761,9 @@
         <v>15</v>
       </c>
       <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
+      <c r="J48" s="12">
+        <v>20</v>
+      </c>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
@@ -2767,16 +2771,16 @@
         <v>1</v>
       </c>
       <c r="O48" s="9">
-        <f t="shared" ref="O48:O50" si="8">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
-        <v>65</v>
+        <f t="shared" ref="O48:O50" si="11">IF(C48&gt;0,MAX(B48,C48),B48)+E48*$A$3+F48*$B$3+G48*$C$3+H48*$D$3+I48*$E$3+J48*$F$3+K48*$G$3+L48*$H$3+M48*$I$3</f>
+        <v>85</v>
       </c>
       <c r="P48" s="5">
-        <f t="shared" ref="P48:P50" si="9">MEDIAN(C48,O48,D48)</f>
-        <v>65</v>
+        <f t="shared" ref="P48:P50" si="12">MEDIAN(C48,O48,D48)</f>
+        <v>85</v>
       </c>
       <c r="Q48" s="6">
-        <f>IF($A$3 &gt; N48, P48/SUM(P$31:P$50), 0)</f>
-        <v>3.6868973340896199E-2</v>
+        <f t="shared" si="10"/>
+        <v>5.0806933652121938E-2</v>
       </c>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
@@ -2807,15 +2811,15 @@
         <v>1</v>
       </c>
       <c r="O49" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P49" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q49" s="6">
-        <f>IF($A$3 &gt; N49, P49/SUM(P$31:P$50), 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R49" s="2"/>
@@ -2847,15 +2851,15 @@
         <v>1</v>
       </c>
       <c r="O50" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P50" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q50" s="6">
-        <f>IF($A$3 &gt; N50, P50/SUM(P$31:P$50), 0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R50" s="2"/>
@@ -2887,7 +2891,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="5">
         <f>SUM(P31:P50)</f>
-        <v>1763</v>
+        <v>1673</v>
       </c>
       <c r="Q51" s="6">
         <f>P51/SUM(P$31:P$50)</f>
@@ -3020,16 +3024,16 @@
         <v>0</v>
       </c>
       <c r="O54" s="5">
-        <f t="shared" ref="O54:O67" si="10">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
+        <f t="shared" ref="O54:O67" si="13">IF(C54&gt;0,MAX(B54,C54),B54)+E54*$A$3+F54*$B$3+G54*$C$3+H54*$D$3+I54*$E$3+J54*$F$3+K54*$G$3+L54*$H$3+M54*$I$3</f>
         <v>135</v>
       </c>
       <c r="P54" s="5">
-        <f t="shared" ref="P54:P67" si="11">MEDIAN(C54,O54,D54)</f>
+        <f t="shared" ref="P54:P67" si="14">MEDIAN(C54,O54,D54)</f>
         <v>135</v>
       </c>
       <c r="Q54" s="6">
-        <f>IF($A$3 &gt; N54, P54/SUM(P$54:P$67), 0)</f>
-        <v>0.16343825665859565</v>
+        <f t="shared" ref="Q54:Q67" si="15">IF($A$3 &gt; N54, P54/SUM(P$54:P$67), 0)</f>
+        <v>0.16423357664233576</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
@@ -3068,16 +3072,16 @@
         <v>10</v>
       </c>
       <c r="O55" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>75</v>
       </c>
       <c r="P55" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>75</v>
       </c>
       <c r="Q55" s="6">
-        <f>IF($A$3 &gt; N55, P55/SUM(P$54:P$67), 0)</f>
-        <v>9.0799031476997583E-2</v>
+        <f t="shared" si="15"/>
+        <v>9.1240875912408759E-2</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -3116,16 +3120,16 @@
         <v>4</v>
       </c>
       <c r="O56" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>125</v>
       </c>
       <c r="P56" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>125</v>
       </c>
       <c r="Q56" s="6">
-        <f>IF($A$3 &gt; N56, P56/SUM(P$54:P$67), 0)</f>
-        <v>0.1513317191283293</v>
+        <f t="shared" si="15"/>
+        <v>0.15206812652068127</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
@@ -3164,16 +3168,16 @@
         <v>8</v>
       </c>
       <c r="O57" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>105</v>
       </c>
       <c r="P57" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>105</v>
       </c>
       <c r="Q57" s="6">
-        <f>IF($A$3 &gt; N57, P57/SUM(P$54:P$67), 0)</f>
-        <v>0.1271186440677966</v>
+        <f t="shared" si="15"/>
+        <v>0.12773722627737227</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
@@ -3212,16 +3216,16 @@
         <v>1</v>
       </c>
       <c r="O58" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>95</v>
       </c>
       <c r="P58" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>95</v>
       </c>
       <c r="Q58" s="6">
-        <f>IF($A$3 &gt; N58, P58/SUM(P$54:P$67), 0)</f>
-        <v>0.11501210653753027</v>
+        <f t="shared" si="15"/>
+        <v>0.11557177615571776</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -3262,16 +3266,16 @@
         <v>4</v>
       </c>
       <c r="O59" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="P59" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>70</v>
       </c>
       <c r="Q59" s="6">
-        <f>IF($A$3 &gt; N59, P59/SUM(P$54:P$67), 0)</f>
-        <v>8.4745762711864403E-2</v>
+        <f t="shared" si="15"/>
+        <v>8.5158150851581502E-2</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -3297,7 +3301,7 @@
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
@@ -3308,16 +3312,16 @@
         <v>8</v>
       </c>
       <c r="O60" s="5">
-        <f t="shared" si="10"/>
-        <v>61</v>
+        <f t="shared" si="13"/>
+        <v>37</v>
       </c>
       <c r="P60" s="5">
-        <f t="shared" si="11"/>
-        <v>61</v>
+        <f t="shared" si="14"/>
+        <v>37</v>
       </c>
       <c r="Q60" s="6">
-        <f>IF($A$3 &gt; N60, P60/SUM(P$54:P$67), 0)</f>
-        <v>7.3849878934624691E-2</v>
+        <f t="shared" si="15"/>
+        <v>4.5012165450121655E-2</v>
       </c>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
@@ -3346,7 +3350,9 @@
         <v>15</v>
       </c>
       <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
+      <c r="J61" s="4">
+        <v>20</v>
+      </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -3354,16 +3360,16 @@
         <v>1</v>
       </c>
       <c r="O61" s="5">
-        <f t="shared" si="10"/>
-        <v>65</v>
+        <f t="shared" si="13"/>
+        <v>85</v>
       </c>
       <c r="P61" s="5">
-        <f t="shared" si="11"/>
-        <v>65</v>
+        <f t="shared" si="14"/>
+        <v>85</v>
       </c>
       <c r="Q61" s="6">
-        <f>IF($A$3 &gt; N61, P61/SUM(P$54:P$67), 0)</f>
-        <v>7.8692493946731237E-2</v>
+        <f t="shared" si="15"/>
+        <v>0.10340632603406326</v>
       </c>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
@@ -3404,16 +3410,16 @@
         <v>1</v>
       </c>
       <c r="O62" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>95</v>
       </c>
       <c r="P62" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>95</v>
       </c>
       <c r="Q62" s="6">
-        <f>IF($A$3 &gt; N62, P62/SUM(P$54:P$67), 0)</f>
-        <v>0.11501210653753027</v>
+        <f t="shared" si="15"/>
+        <v>0.11557177615571776</v>
       </c>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
@@ -3442,15 +3448,15 @@
       <c r="M63" s="4"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P63" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q63" s="6">
-        <f>IF($A$3 &gt; N63, P63/SUM(P$54:P$67), 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R63" s="2"/>
@@ -3480,15 +3486,15 @@
       <c r="M64" s="4"/>
       <c r="N64" s="5"/>
       <c r="O64" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P64" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q64" s="6">
-        <f>IF($A$3 &gt; N64, P64/SUM(P$54:P$67), 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R64" s="2"/>
@@ -3518,15 +3524,15 @@
       <c r="M65" s="4"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P65" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q65" s="6">
-        <f>IF($A$3 &gt; N65, P65/SUM(P$54:P$67), 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R65" s="2"/>
@@ -3556,15 +3562,15 @@
       <c r="M66" s="4"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P66" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q66" s="6">
-        <f>IF($A$3 &gt; N66, P66/SUM(P$54:P$67), 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R66" s="2"/>
@@ -3594,15 +3600,15 @@
       <c r="M67" s="4"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P67" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q67" s="6">
-        <f>IF($A$3 &gt; N67, P67/SUM(P$54:P$67), 0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R67" s="2"/>
@@ -3634,10 +3640,10 @@
       <c r="O68" s="2"/>
       <c r="P68" s="5">
         <f>SUM(P53:P67)</f>
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="Q68" s="6">
-        <f t="shared" ref="Q68" si="12">P68/SUM(P$54:P$67)</f>
+        <f t="shared" ref="Q68" si="16">P68/SUM(P$54:P$67)</f>
         <v>1</v>
       </c>
       <c r="R68" s="2"/>

</xml_diff>

<commit_message>
Reduce electrical storm frequencies further (#20968)
Electrical storms are still too frequent. Makes them less frequent!
</commit_message>
<xml_diff>
--- a/tools/Event Probabilities/Event Probabilities.xlsx
+++ b/tools/Event Probabilities/Event Probabilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Aurora.3\tools\Event Probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7184E218-7B06-4BB4-B93C-B09395072FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F3034B-0776-4BCB-8615-B3239A842E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18120" yWindow="-4995" windowWidth="18240" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE11BF8-2C51-4794-BAB0-B08C213463FD}">
   <dimension ref="A1:AA997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N60" sqref="N60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -895,7 +895,7 @@
       </c>
       <c r="Q7" s="17">
         <f t="shared" ref="Q7:Q27" si="2">IF($A$3 &gt; N7, P7/SUM(P$7:P$27), 0)</f>
-        <v>5.4545454545454543E-2</v>
+        <v>5.6737588652482268E-2</v>
       </c>
       <c r="R7" s="14"/>
       <c r="S7" s="2"/>
@@ -943,7 +943,7 @@
       </c>
       <c r="Q8" s="17">
         <f t="shared" si="2"/>
-        <v>3.8636363636363635E-2</v>
+        <v>4.0189125295508277E-2</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -989,7 +989,7 @@
       </c>
       <c r="Q9" s="17">
         <f t="shared" si="2"/>
-        <v>1.5909090909090907E-2</v>
+        <v>1.6548463356973995E-2</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="Q10" s="17">
         <f t="shared" si="2"/>
-        <v>2.2727272727272728E-2</v>
+        <v>2.3640661938534278E-2</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="Q11" s="17">
         <f t="shared" si="2"/>
-        <v>0.13636363636363635</v>
+        <v>0.14184397163120568</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="Q12" s="17">
         <f t="shared" si="2"/>
-        <v>4.5454545454545452E-3</v>
+        <v>4.7281323877068557E-3</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="Q13" s="17">
         <f t="shared" si="2"/>
-        <v>6.8181818181818179E-3</v>
+        <v>7.0921985815602835E-3</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="Q14" s="17">
         <f t="shared" si="2"/>
-        <v>0.13636363636363635</v>
+        <v>0.14184397163120568</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="Q15" s="17">
         <f t="shared" si="2"/>
-        <v>2.2727272727272728E-2</v>
+        <v>2.3640661938534278E-2</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="Q16" s="17">
         <f t="shared" si="2"/>
-        <v>5.4545454545454543E-2</v>
+        <v>5.6737588652482268E-2</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="Q17" s="17">
         <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>5.2009456264775412E-2</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="Q18" s="17">
         <f t="shared" si="2"/>
-        <v>2.5000000000000001E-2</v>
+        <v>2.6004728132387706E-2</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="Q19" s="17">
         <f t="shared" si="2"/>
-        <v>4.5454545454545456E-2</v>
+        <v>4.7281323877068557E-2</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="Q20" s="17">
         <f t="shared" si="2"/>
-        <v>3.6363636363636362E-2</v>
+        <v>3.7825059101654845E-2</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="Q21" s="17">
         <f t="shared" si="2"/>
-        <v>0.13636363636363635</v>
+        <v>0.14184397163120568</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="Q22" s="17">
         <f t="shared" si="2"/>
-        <v>8.8636363636363638E-2</v>
+        <v>9.2198581560283682E-2</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="Q23" s="17">
         <f t="shared" si="2"/>
-        <v>4.5454545454545456E-2</v>
+        <v>4.7281323877068557E-2</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="Q24" s="17">
         <f t="shared" si="2"/>
-        <v>2.7272727272727271E-2</v>
+        <v>2.8368794326241134E-2</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -1697,7 +1697,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1705,11 +1705,11 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -1719,15 +1719,15 @@
       </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="Q25" s="17">
         <f t="shared" si="2"/>
-        <v>5.2272727272727269E-2</v>
+        <v>1.4184397163120567E-2</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -1834,7 +1834,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="5">
         <f>SUM(P7:P27)</f>
-        <v>2200</v>
+        <v>2115</v>
       </c>
       <c r="Q28" s="6">
         <f>P28/SUM(P$7:P$27)</f>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="Q31" s="6">
         <f>IF($A$3 &gt; N31, P31/SUM(P$31:P$50), 0)</f>
-        <v>0.11954572624028691</v>
+        <v>0.12437810945273632</v>
       </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="Q32" s="6">
         <f>IF($A$3 &gt; N32, P32/SUM(P$31:P$50), 0)</f>
-        <v>5.9772863120143453E-2</v>
+        <v>6.2189054726368161E-2</v>
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="Q33" s="6">
         <f>IF($A$3 &gt; N33, P33/SUM(P$31:P$50), 0)</f>
-        <v>2.9886431560071727E-2</v>
+        <v>3.109452736318408E-2</v>
       </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="Q34" s="6">
         <f t="shared" ref="Q34" si="9">IF($A$3 &gt; N34, P34/SUM(P$31:P$50), 0)</f>
-        <v>7.4716078900179325E-2</v>
+        <v>7.7736318407960192E-2</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
@@ -2130,7 +2130,7 @@
         <v>39</v>
       </c>
       <c r="B35" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -2140,11 +2140,11 @@
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2154,15 +2154,15 @@
       </c>
       <c r="O35" s="5">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="P35" s="5">
         <f t="shared" si="4"/>
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="Q35" s="6">
         <f t="shared" ref="Q35:Q50" si="10">IF($A$3 &gt; N35, P35/SUM(P$31:P$50), 0)</f>
-        <v>5.6784219964136282E-2</v>
+        <v>1.8656716417910446E-2</v>
       </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="Q38" s="6">
         <f t="shared" si="10"/>
-        <v>4.4231918708906158E-2</v>
+        <v>4.6019900497512436E-2</v>
       </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="Q39" s="6">
         <f t="shared" si="10"/>
-        <v>5.9772863120143453E-2</v>
+        <v>6.2189054726368161E-2</v>
       </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="Q40" s="6">
         <f t="shared" si="10"/>
-        <v>5.0806933652121938E-2</v>
+        <v>5.2860696517412938E-2</v>
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="Q41" s="6">
         <f t="shared" si="10"/>
-        <v>3.8852361028093245E-2</v>
+        <v>4.0422885572139307E-2</v>
       </c>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="Q42" s="6">
         <f t="shared" si="10"/>
-        <v>0.10759115361625822</v>
+        <v>0.11194029850746269</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="Q43" s="6">
         <f t="shared" si="10"/>
-        <v>3.2277346084877465E-2</v>
+        <v>3.3582089552238806E-2</v>
       </c>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="Q44" s="6">
         <f t="shared" si="10"/>
-        <v>6.5750149432157803E-2</v>
+        <v>6.8407960199004969E-2</v>
       </c>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
@@ -2636,7 +2636,7 @@
       </c>
       <c r="Q45" s="6">
         <f t="shared" si="10"/>
-        <v>5.379557680812911E-2</v>
+        <v>5.5970149253731345E-2</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="Q46" s="6">
         <f t="shared" si="10"/>
-        <v>8.6670651524208012E-2</v>
+        <v>9.0174129353233837E-2</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="Q47" s="6">
         <f t="shared" si="10"/>
-        <v>6.8738792588164968E-2</v>
+        <v>7.1517412935323377E-2</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="Q48" s="6">
         <f t="shared" si="10"/>
-        <v>5.0806933652121938E-2</v>
+        <v>5.2860696517412938E-2</v>
       </c>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
@@ -2891,7 +2891,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="5">
         <f>SUM(P31:P50)</f>
-        <v>1673</v>
+        <v>1608</v>
       </c>
       <c r="Q51" s="6">
         <f>P51/SUM(P$31:P$50)</f>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="Q54" s="6">
         <f t="shared" ref="Q54:Q67" si="15">IF($A$3 &gt; N54, P54/SUM(P$54:P$67), 0)</f>
-        <v>0.16423357664233576</v>
+        <v>0.18194070080862534</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
@@ -3051,7 +3051,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="4">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -3073,15 +3073,15 @@
       </c>
       <c r="O55" s="5">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="P55" s="5">
         <f t="shared" si="14"/>
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="Q55" s="6">
         <f t="shared" si="15"/>
-        <v>9.1240875912408759E-2</v>
+        <v>5.3908355795148251E-2</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="Q56" s="6">
         <f t="shared" si="15"/>
-        <v>0.15206812652068127</v>
+        <v>0.16846361185983827</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="Q57" s="6">
         <f t="shared" si="15"/>
-        <v>0.12773722627737227</v>
+        <v>0.14150943396226415</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="Q58" s="6">
         <f t="shared" si="15"/>
-        <v>0.11557177615571776</v>
+        <v>0.1280323450134771</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="Q59" s="6">
         <f t="shared" si="15"/>
-        <v>8.5158150851581502E-2</v>
+        <v>9.4339622641509441E-2</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="Q60" s="6">
         <f t="shared" si="15"/>
-        <v>4.5012165450121655E-2</v>
+        <v>4.9865229110512131E-2</v>
       </c>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="Q61" s="6">
         <f t="shared" si="15"/>
-        <v>0.10340632603406326</v>
+        <v>0.11455525606469003</v>
       </c>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
@@ -3387,21 +3387,21 @@
         <v>39</v>
       </c>
       <c r="B62" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -3411,15 +3411,15 @@
       </c>
       <c r="O62" s="5">
         <f t="shared" si="13"/>
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="P62" s="5">
         <f t="shared" si="14"/>
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="Q62" s="6">
         <f t="shared" si="15"/>
-        <v>0.11557177615571776</v>
+        <v>6.7385444743935305E-2</v>
       </c>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
@@ -3640,7 +3640,7 @@
       <c r="O68" s="2"/>
       <c r="P68" s="5">
         <f>SUM(P53:P67)</f>
-        <v>822</v>
+        <v>742</v>
       </c>
       <c r="Q68" s="6">
         <f t="shared" ref="Q68" si="16">P68/SUM(P$54:P$67)</f>

</xml_diff>